<commit_message>
Overhaul questionnaire v2: all dropdowns, DEBMM-aligned thresholds, no text questions
Major changes:
- Rewrite questionnaire from 56 to 41 questions, all dropdown-based (no free-text)
- Remove 13 redundant checklists where companion scales already encoded the same info
- Embed quantitative thresholds from rubric directly in scale option labels
- Fix ATT&CK coverage thresholds to align with Elastic's DEBMM (30-50% at Defined)
- Fix internal testing thresholds (40-70% at Defined, 70-90% at Managed, >90% at Optimized)
- Add FN reduction percentages to false negative triage rubric
- Add AI quality checks at Defined level for Tier 4 automation
- Remove evidence/notes column from self-assessment spreadsheet (kept for audit)
- Remove text question handling from scorer
- Regenerate all dependent files: markdown questionnaires, rubric.md, templates, spreadsheets

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -781,7 +781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,242 +823,235 @@
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>It covers 21 criteria across 7 categories, with 56 questions total.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="3" t="inlineStr">
+          <t>It covers 21 criteria across 7 categories, with 41 dropdown questions total.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>All questions are answered via dropdowns (Yes/No or Scale 1-5). No free-text required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>How to Use</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>1. Fill in your organization details at the top of the Assessment tab</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>2. Answer each question using the dropdown menus or text fields</t>
+          <t>1. Fill in your organization details at the top of the Assessment tab</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>3. For Yes/No questions: select from the dropdown</t>
+          <t>2. Answer each question using the dropdown menus</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>4. For Scale questions (1-5): select from the dropdown</t>
+          <t>3. For Yes/No questions: select from the dropdown</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>5. For Text questions: type your response in the 'Your Answer' column</t>
+          <t>4. For Scale questions (1-5): select from the dropdown</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>6. Use the 'Evidence / Notes' column for supporting details (optional but recommended)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>7. Switch to the Results Dashboard tab to see your scores automatically calculated</t>
+          <t>5. Switch to the Results Dashboard tab to see your scores automatically calculated</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Maturity Levels</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>Maturity Levels</t>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Each criterion is scored on a 1-5 scale:</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>Each criterion is scored on a 1-5 scale:</t>
-        </is>
-      </c>
+      <c r="B18" s="4" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="B19" s="4" t="inlineStr"/>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1 - Initial:      Minimal or no structured activity</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1 - Initial:      Minimal or no structured activity</t>
+          <t xml:space="preserve">  2 - Repeatable:  Sporadic, inconsistent efforts</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  2 - Repeatable:  Sporadic, inconsistent efforts</t>
+          <t xml:space="preserve">  3 - Defined:       Regular, documented processes followed consistently</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  3 - Defined:       Regular, documented processes followed consistently</t>
+          <t xml:space="preserve">  4 - Managed:     Comprehensive, well-integrated with measurable outcomes</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  4 - Managed:     Comprehensive, well-integrated with measurable outcomes</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="4" t="inlineStr">
-        <is>
           <t xml:space="preserve">  5 - Optimized:   Fully automated, continuously improving</t>
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>DEBMM Tiers</t>
+        </is>
+      </c>
+    </row>
     <row r="26">
-      <c r="B26" s="3" t="inlineStr">
-        <is>
-          <t>DEBMM Tiers</t>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>Tier 0 - Foundation:     Basic groundwork (rule development, maintenance, roadmaps, threat modeling)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Tier 0 - Foundation:     Basic groundwork (rule development, maintenance, roadmaps, threat modeling)</t>
+          <t>Tier 1 - Basic:              Baseline rules, version control, telemetry, testing</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Tier 1 - Basic:              Baseline rules, version control, telemetry, testing</t>
+          <t>Tier 2 - Intermediate:  FP reduction, gap analysis, internal validation</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Tier 2 - Intermediate:  FP reduction, gap analysis, internal validation</t>
+          <t>Tier 3 - Advanced:       FN triage, external validation, advanced TTP coverage</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Tier 3 - Advanced:       FN triage, external validation, advanced TTP coverage</t>
+          <t>Tier 4 - Expert:            Threat hunting, automation, AI/LLM integration</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="4" t="inlineStr">
-        <is>
-          <t>Tier 4 - Expert:            Threat hunting, automation, AI/LLM integration</t>
-        </is>
-      </c>
+      <c r="B31" s="4" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="B32" s="4" t="inlineStr"/>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>Enrichment - People &amp; Organization:  Team structure, training, leadership</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Enrichment - People &amp; Organization:  Team structure, training, leadership</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="4" t="inlineStr">
-        <is>
           <t>Enrichment - Process &amp; Governance:   Lifecycle, metrics, collaboration</t>
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Tier Determination</t>
+        </is>
+      </c>
+    </row>
     <row r="36">
-      <c r="B36" s="3" t="inlineStr">
-        <is>
-          <t>Tier Determination</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="4" t="inlineStr">
+      <c r="B36" s="4" t="inlineStr">
         <is>
           <t>Your achieved tier is the highest tier where ALL criteria in that tier (and all lower tiers) score &gt;= 3.0 (Defined level). This enforces the progressive nature of the model - you need solid foundations before claiming advanced maturity.</t>
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>Three Scoring Paths</t>
+        </is>
+      </c>
+    </row>
     <row r="39">
-      <c r="B39" s="3" t="inlineStr">
-        <is>
-          <t>Three Scoring Paths</t>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>1. This Spreadsheet: Fill it out and scores calculate automatically in the Dashboard tab</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>1. This Spreadsheet: Fill it out and scores calculate automatically in the Dashboard tab</t>
+          <t>2. Python CLI: Export answers to YAML and run scorer/score.py for a detailed report</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>2. Python CLI: Export answers to YAML and run scorer/score.py for a detailed report</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="4" t="inlineStr">
-        <is>
           <t>3. LLM-Assisted: Run scorer/llm_scorer.py to have AI score your text answers and generate improvement recommendations</t>
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>References</t>
+        </is>
+      </c>
+    </row>
     <row r="44">
-      <c r="B44" s="3" t="inlineStr">
-        <is>
-          <t>References</t>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>Elastic DEBMM: https://www.elastic.co/security-labs/elastic-releases-debmm</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Elastic DEBMM: https://www.elastic.co/security-labs/elastic-releases-debmm</t>
+          <t>Detection Engineering Maturity Matrix: https://detectionengineering.io/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="4" t="inlineStr">
-        <is>
-          <t>Detection Engineering Maturity Matrix: https://detectionengineering.io/</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" s="4" t="inlineStr">
         <is>
           <t>MITRE ATT&amp;CK: https://attack.mitre.org/</t>
         </is>
@@ -1079,7 +1072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
@@ -1212,7 +1205,7 @@
       <c r="G10" s="9" t="n"/>
       <c r="H10" s="9" t="n"/>
     </row>
-    <row r="11" ht="30" customHeight="1">
+    <row r="11" ht="100" customHeight="1">
       <c r="A11" s="10" t="inlineStr">
         <is>
           <t>T0-Q1</t>
@@ -1230,17 +1223,22 @@
       </c>
       <c r="D11" s="10" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E11" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team follow a documented methodology for developing detection rules?</t>
+          <t>Rate the maturity of the assessed team's rule development process.
+  1 = No structured approach; rules created ad hoc or reactively (0% follow a formal process)
+  2 = Some rules follow a loose process but it is inconsistently applied (&lt;30% follow a documented process)
+  3 = Defined methodology is documented and followed for most new rules (50-70% follow process; schema alignment &gt;60%)
+  4 = Standardized across team with enforced workflows, templates, and quality gates (80-90% schema alignment; all new rules go through formal review)
+  5 = Continuous improvement via feedback loops; fully integrated with CI/CD and automated linting/validation (90-100% schema alignment)</t>
         </is>
       </c>
       <c r="F11" s="13" t="n"/>
       <c r="G11" s="14">
-        <f>IF(F11="Yes",3,IF(F11="No",1,""))</f>
+        <f>IF(F11="","",F11)</f>
         <v/>
       </c>
       <c r="H11" s="15" t="n"/>
@@ -1268,7 +1266,7 @@
       </c>
       <c r="E12" s="18" t="inlineStr">
         <is>
-          <t>Do new detection rules go through peer review before deployment?</t>
+          <t>Do all new detection rules go through peer review before production deployment?</t>
         </is>
       </c>
       <c r="F12" s="13" t="n"/>
@@ -1291,7 +1289,7 @@
       </c>
       <c r="C13" s="11" t="inlineStr">
         <is>
-          <t>Structured Rule Development Approach</t>
+          <t>Rule Creation and Maintenance</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
@@ -1301,12 +1299,12 @@
       </c>
       <c r="E13" s="12" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's rule development process.
-  1 = No structured approach; rules created ad hoc
-  2 = Some rules follow a loose process, inconsistently applied
-  3 = Defined methodology documented and followed for most rules
-  4 = Standardized across team with enforced workflows and quality gates
-  5 = Continuous improvement with CI/CD integration and automated validation</t>
+          <t>What percentage of the assessed team's rules are reviewed on a regular schedule?
+  1 = Less than 50% reviewed annually; no rule owners assigned
+  2 = 50-70% reviewed annually; rules may have informal owners but no formal peer review process
+  3 = 70-80% reviewed on schedule; rules have assigned owners and defined review cycles; peer review on most changes
+  4 = 80-90% reviewed on schedule; comprehensive lifecycle management (create, test, deploy, monitor, retire); 100% peer review on changes
+  5 = 90-100% reviewed on schedule; automated rule health monitoring flags stale or broken rules for review</t>
         </is>
       </c>
       <c r="F13" s="13" t="n"/>
@@ -1316,7 +1314,7 @@
       </c>
       <c r="H13" s="15" t="n"/>
     </row>
-    <row r="14" ht="30" customHeight="1">
+    <row r="14" ht="100" customHeight="1">
       <c r="A14" s="16" t="inlineStr">
         <is>
           <t>T0-Q4</t>
@@ -1329,22 +1327,27 @@
       </c>
       <c r="C14" s="17" t="inlineStr">
         <is>
-          <t>Rule Creation and Maintenance</t>
+          <t>Roadmap Documentation</t>
         </is>
       </c>
       <c r="D14" s="16" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E14" s="18" t="inlineStr">
         <is>
-          <t>Do the assessed team's detection rules have assigned owners?</t>
+          <t>Rate the maturity of the assessed team's detection engineering roadmap.
+  1 = No roadmap exists; work is entirely reactive or driven by individual initiative
+  2 = Informal roadmap or backlog exists (e.g., a Jira board or wiki page) but is not regularly maintained or shared (&lt;30% of work tied to a plan)
+  3 = Formal roadmap documented, reviewed at least quarterly, shared with stakeholders; priorities are clear (50-70% of planned work tracked)
+  4 = Integrated with organizational security strategy; progress tracked with metrics and reported to leadership (70-90% tracked; quarterly leadership reviews)
+  5 = Dynamic, continuously updated roadmap driven by threat intel, gap analysis, and risk priorities (90-100% tracked; auto-updated from analysis feeds)</t>
         </is>
       </c>
       <c r="F14" s="13" t="n"/>
       <c r="G14" s="19">
-        <f>IF(F14="Yes",3,IF(F14="No",1,""))</f>
+        <f>IF(F14="","",F14)</f>
         <v/>
       </c>
       <c r="H14" s="15" t="n"/>
@@ -1362,7 +1365,7 @@
       </c>
       <c r="C15" s="11" t="inlineStr">
         <is>
-          <t>Rule Creation and Maintenance</t>
+          <t>Threat Modeling</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
@@ -1372,12 +1375,12 @@
       </c>
       <c r="E15" s="12" t="inlineStr">
         <is>
-          <t>What percentage of the assessed team's rules are reviewed on a regular schedule?
-  1 = Less than 50% reviewed annually
-  2 = 50-70% reviewed annually
-  3 = 70-80% reviewed on schedule
-  4 = 80-90% reviewed on schedule with peer review on all changes
-  5 = 90-100% reviewed with automated health monitoring</t>
+          <t>How frequently does the assessed team perform threat modeling?
+  1 = Never performed or not at all
+  2 = Less than once per year; typically triggered by a major incident or audit finding
+  3 = 1-2 times per year with documented results that inform the detection roadmap
+  4 = Quarterly or more; outputs directly prioritize new detection development (&gt;70% of new detections tied to threat model outputs)
+  5 = Continuous proactive modeling incorporating real-time threat intel, attack surface changes, and emerging TTPs</t>
         </is>
       </c>
       <c r="F15" s="13" t="n"/>
@@ -1400,7 +1403,7 @@
       </c>
       <c r="C16" s="17" t="inlineStr">
         <is>
-          <t>Roadmap Documentation</t>
+          <t>Threat Modeling</t>
         </is>
       </c>
       <c r="D16" s="16" t="inlineStr">
@@ -1410,7 +1413,7 @@
       </c>
       <c r="E16" s="18" t="inlineStr">
         <is>
-          <t>Does the assessed team maintain a documented detection engineering roadmap?</t>
+          <t>Does the assessed team's threat modeling use a recognized framework?</t>
         </is>
       </c>
       <c r="F16" s="13" t="n"/>
@@ -1420,7 +1423,7 @@
       </c>
       <c r="H16" s="15" t="n"/>
     </row>
-    <row r="17" ht="100" customHeight="1">
+    <row r="17" ht="30" customHeight="1">
       <c r="A17" s="10" t="inlineStr">
         <is>
           <t>T0-Q7</t>
@@ -1433,78 +1436,54 @@
       </c>
       <c r="C17" s="11" t="inlineStr">
         <is>
-          <t>Roadmap Documentation</t>
+          <t>Threat Modeling</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>Scale 1-5</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="E17" s="12" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's detection roadmap.
-  1 = No roadmap exists; work is entirely reactive
-  2 = Informal roadmap or backlog exists but not regularly maintained
-  3 = Formal roadmap reviewed quarterly and shared with stakeholders
-  4 = Integrated with security strategy; progress tracked with metrics
-  5 = Dynamic, continuously updated based on intel, gaps, and risk</t>
+          <t>Do threat modeling outputs directly generate items on the assessed team's backlog?</t>
         </is>
       </c>
       <c r="F17" s="13" t="n"/>
       <c r="G17" s="14">
-        <f>IF(F17="","",F17)</f>
+        <f>IF(F17="Yes",4,IF(F17="No",1,""))</f>
         <v/>
       </c>
       <c r="H17" s="15" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="16" t="inlineStr">
-        <is>
-          <t>T0-Q8</t>
-        </is>
-      </c>
-      <c r="B18" s="16" t="inlineStr">
-        <is>
-          <t>Foundation</t>
-        </is>
-      </c>
-      <c r="C18" s="17" t="inlineStr">
-        <is>
-          <t>Threat Modeling</t>
-        </is>
-      </c>
-      <c r="D18" s="16" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E18" s="18" t="inlineStr">
-        <is>
-          <t>Does the assessed team perform threat modeling exercises?</t>
-        </is>
-      </c>
-      <c r="F18" s="13" t="n"/>
-      <c r="G18" s="19">
-        <f>IF(F18="Yes",3,IF(F18="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H18" s="15" t="n"/>
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Basic</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="n"/>
+      <c r="C18" s="9" t="n"/>
+      <c r="D18" s="9" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+      <c r="G18" s="9" t="n"/>
+      <c r="H18" s="9" t="n"/>
     </row>
     <row r="19" ht="100" customHeight="1">
       <c r="A19" s="10" t="inlineStr">
         <is>
-          <t>T0-Q9</t>
+          <t>T1-Q1</t>
         </is>
       </c>
       <c r="B19" s="10" t="inlineStr">
         <is>
-          <t>Foundation</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="C19" s="11" t="inlineStr">
         <is>
-          <t>Threat Modeling</t>
+          <t>Baseline Rule Creation</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
@@ -1514,12 +1493,12 @@
       </c>
       <c r="E19" s="12" t="inlineStr">
         <is>
-          <t>How frequently does the assessed team perform threat modeling?
-  1 = Never or not at all
-  2 = Less than once per year
-  3 = Quarterly with documented results
-  4 = Monthly; outputs directly inform detection priorities
-  5 = Continuous with real-time threat intelligence integration</t>
+          <t>How many custom detection rules does the assessed team maintain?
+  1 = Fewer than 10 custom rules; mostly relying on vendor/out-of-the-box rules
+  2 = 10-30 rules covering the most critical threats (e.g., ransomware, credential theft, C2)
+  3 = 30-60 rules with a mix of signature-based and behavioral detections across major categories
+  4 = 60-100 rules including behavioral and TTP-focused detections tuned per environment
+  5 = 100+ rules with continuous refinement, environment-specific tuning, and automated coverage analysis</t>
         </is>
       </c>
       <c r="F19" s="13" t="n"/>
@@ -1529,54 +1508,86 @@
       </c>
       <c r="H19" s="15" t="n"/>
     </row>
-    <row r="20" ht="60" customHeight="1">
+    <row r="20" ht="100" customHeight="1">
       <c r="A20" s="16" t="inlineStr">
         <is>
-          <t>T0-Q10</t>
+          <t>T1-Q2</t>
         </is>
       </c>
       <c r="B20" s="16" t="inlineStr">
         <is>
-          <t>Foundation</t>
+          <t>Basic</t>
         </is>
       </c>
       <c r="C20" s="17" t="inlineStr">
         <is>
-          <t>Threat Modeling</t>
+          <t>Baseline Rule Creation</t>
         </is>
       </c>
       <c r="D20" s="16" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E20" s="18" t="inlineStr">
         <is>
-          <t>Describe the assessed team's threat modeling process, including frameworks used, frequency, and how outputs inform detection development.</t>
-        </is>
-      </c>
-      <c r="F20" s="15" t="n"/>
-      <c r="G20" s="19" t="inlineStr"/>
+          <t>Estimate the assessed team's MITRE ATT&amp;CK technique coverage for priority areas.
+  1 = Unknown or not measured; no ATT&amp;CK mapping performed
+  2 = Less than 30% of priority techniques covered; coverage is ad hoc
+  3 = 30-50% of priority techniques covered with documented gaps identified
+  4 = 50-70% coverage including behavioral detections; gaps tracked against threat model
+  5 = Over 70% coverage with continuous gap analysis and automated coverage tracking</t>
+        </is>
+      </c>
+      <c r="F20" s="13" t="n"/>
+      <c r="G20" s="19">
+        <f>IF(F20="","",F20)</f>
+        <v/>
+      </c>
       <c r="H20" s="15" t="n"/>
     </row>
-    <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Basic</t>
-        </is>
-      </c>
-      <c r="B21" s="9" t="n"/>
-      <c r="C21" s="9" t="n"/>
-      <c r="D21" s="9" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-      <c r="G21" s="9" t="n"/>
-      <c r="H21" s="9" t="n"/>
+    <row r="21" ht="100" customHeight="1">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>T1-Q3</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>Ruleset Management and Maintenance</t>
+        </is>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>Scale 1-5</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>Rate the maturity of the assessed team's ruleset management.
+  1 = No formal management; rules live only in the SIEM console with no version control or documentation (&lt;20% in version control)
+  2 = Some rules stored in version control (e.g., Git) with basic documentation (20-50% in VCS)
+  3 = Most rules in version control with documentation standards; detection-as-code approach being adopted (50-80% in VCS with docs)
+  4 = Detection-as-code is standard practice; CI/CD pipelines handle rule testing and deployment; all rules documented and versioned (80-90% in DaC pipeline)
+  5 = Fully automated rule lifecycle: CI/CD, automated testing, continuous validation, and weekly maintenance cycles (100% DaC)</t>
+        </is>
+      </c>
+      <c r="F21" s="13" t="n"/>
+      <c r="G21" s="14">
+        <f>IF(F21="","",F21)</f>
+        <v/>
+      </c>
+      <c r="H21" s="15" t="n"/>
     </row>
     <row r="22" ht="100" customHeight="1">
       <c r="A22" s="16" t="inlineStr">
         <is>
-          <t>T1-Q1</t>
+          <t>T1-Q4</t>
         </is>
       </c>
       <c r="B22" s="16" t="inlineStr">
@@ -1586,7 +1597,7 @@
       </c>
       <c r="C22" s="17" t="inlineStr">
         <is>
-          <t>Baseline Rule Creation</t>
+          <t>Telemetry Quality</t>
         </is>
       </c>
       <c r="D22" s="16" t="inlineStr">
@@ -1596,12 +1607,12 @@
       </c>
       <c r="E22" s="18" t="inlineStr">
         <is>
-          <t>How many custom baseline detection rules does the assessed team maintain?
-  1 = Fewer than 10 custom rules; mostly vendor defaults
-  2 = 10-30 rules covering critical threats
-  3 = 30-60 rules with a mix of signature and behavioral detections
-  4 = 60-100 rules including behavioral and TTP-focused detections
-  5 = 100+ rules with continuous refinement and environment-specific tuning</t>
+          <t>Rate the quality and coverage of the assessed team's telemetry.
+  1 = No active telemetry management; using whatever data sources happen to be available (&lt;30% of rule types have adequate telemetry)
+  2 = Some awareness of gaps; basic health checks on critical sources like EDR and firewall logs (30-50% adequate coverage)
+  3 = Actively monitored; data source coverage mapped to detection needs; CTI enrichment beginning (50-70% coverage)
+  4 = Comprehensive with automated health monitoring, CTI enrichment, and proactive gap identification (70-90% coverage)
+  5 = Advanced workflows with real-time enrichment, automated remediation of telemetry gaps, full CTI integration (90-100% coverage)</t>
         </is>
       </c>
       <c r="F22" s="13" t="n"/>
@@ -1611,10 +1622,10 @@
       </c>
       <c r="H22" s="15" t="n"/>
     </row>
-    <row r="23" ht="100" customHeight="1">
+    <row r="23" ht="30" customHeight="1">
       <c r="A23" s="10" t="inlineStr">
         <is>
-          <t>T1-Q2</t>
+          <t>T1-Q5</t>
         </is>
       </c>
       <c r="B23" s="10" t="inlineStr">
@@ -1624,27 +1635,22 @@
       </c>
       <c r="C23" s="11" t="inlineStr">
         <is>
-          <t>Baseline Rule Creation</t>
+          <t>Telemetry Quality</t>
         </is>
       </c>
       <c r="D23" s="10" t="inlineStr">
         <is>
-          <t>Scale 1-5</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="E23" s="12" t="inlineStr">
         <is>
-          <t>Estimate the assessed team's MITRE ATT&amp;CK technique coverage for priority threat areas.
-  1 = Minimal or unknown coverage
-  2 = Less than 30% of priority techniques covered
-  3 = 40-60% of priority techniques covered
-  4 = 60-80% coverage with behavioral detections
-  5 = Over 80% coverage with continuous gap analysis</t>
+          <t>Does the assessed team maintain a documented data source inventory mapped to use cases?</t>
         </is>
       </c>
       <c r="F23" s="13" t="n"/>
       <c r="G23" s="14">
-        <f>IF(F23="","",F23)</f>
+        <f>IF(F23="Yes",3,IF(F23="No",1,""))</f>
         <v/>
       </c>
       <c r="H23" s="15" t="n"/>
@@ -1652,7 +1658,7 @@
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="16" t="inlineStr">
         <is>
-          <t>T1-Q3</t>
+          <t>T1-Q6</t>
         </is>
       </c>
       <c r="B24" s="16" t="inlineStr">
@@ -1662,7 +1668,7 @@
       </c>
       <c r="C24" s="17" t="inlineStr">
         <is>
-          <t>Ruleset Management and Maintenance</t>
+          <t>Telemetry Quality</t>
         </is>
       </c>
       <c r="D24" s="16" t="inlineStr">
@@ -1672,20 +1678,20 @@
       </c>
       <c r="E24" s="18" t="inlineStr">
         <is>
-          <t>Are the assessed team's detection rules stored in version control?</t>
+          <t>Does the assessed team have automated alerting for data source degradation?</t>
         </is>
       </c>
       <c r="F24" s="13" t="n"/>
       <c r="G24" s="19">
-        <f>IF(F24="Yes",3,IF(F24="No",1,""))</f>
+        <f>IF(F24="Yes",4,IF(F24="No",1,""))</f>
         <v/>
       </c>
       <c r="H24" s="15" t="n"/>
     </row>
-    <row r="25" ht="30" customHeight="1">
+    <row r="25" ht="100" customHeight="1">
       <c r="A25" s="10" t="inlineStr">
         <is>
-          <t>T1-Q4</t>
+          <t>T1-Q7</t>
         </is>
       </c>
       <c r="B25" s="10" t="inlineStr">
@@ -1695,22 +1701,27 @@
       </c>
       <c r="C25" s="11" t="inlineStr">
         <is>
-          <t>Ruleset Management and Maintenance</t>
+          <t>Threat Landscape Review</t>
         </is>
       </c>
       <c r="D25" s="10" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E25" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team practice detection-as-code with CI/CD pipelines?</t>
+          <t>How frequently does the assessed team review the threat landscape?
+  1 = No regular reviews; detection priorities are not informed by current threats
+  2 = Annually or bi-annually; some rule updates after major threat advisories (1-2 reviews/year)
+  3 = Quarterly with documented findings that update the detection roadmap (50-70% of rules reviewed against current threats)
+  4 = Monthly reviews integrated with threat intelligence feeds; detection priorities continuously aligned (70-90% aligned)
+  5 = Real-time threat landscape monitoring with automated intel feeds driving detection priority updates (90-100% aligned)</t>
         </is>
       </c>
       <c r="F25" s="13" t="n"/>
       <c r="G25" s="14">
-        <f>IF(F25="Yes",4,IF(F25="No",1,""))</f>
+        <f>IF(F25="","",F25)</f>
         <v/>
       </c>
       <c r="H25" s="15" t="n"/>
@@ -1718,7 +1729,7 @@
     <row r="26" ht="100" customHeight="1">
       <c r="A26" s="16" t="inlineStr">
         <is>
-          <t>T1-Q5</t>
+          <t>T1-Q8</t>
         </is>
       </c>
       <c r="B26" s="16" t="inlineStr">
@@ -1728,7 +1739,7 @@
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>Ruleset Management and Maintenance</t>
+          <t>Product Owner Engagement</t>
         </is>
       </c>
       <c r="D26" s="16" t="inlineStr">
@@ -1738,12 +1749,12 @@
       </c>
       <c r="E26" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's ruleset management.
-  1 = No formal management; rules live in the SIEM without version control
-  2 = Some rules in version control with basic documentation
-  3 = Most rules versioned with documentation standards; DaC being adopted
-  4 = DaC is standard; CI/CD handles deployment; all documented
-  5 = Fully automated lifecycle with CI/CD, testing, and weekly validation</t>
+          <t>Rate the engagement between the assessed team and product/platform owners.
+  1 = No engagement; detection needs are never communicated to product/platform teams
+  2 = Occasional ad hoc engagement, typically reactive to issues or missing features (fewer than 4 interactions per year)
+  3 = Quarterly structured engagements to communicate detection needs, request features, and provide feedback
+  4 = Monthly proactive partnership; detection requirements tracked on product roadmaps (&gt;50% of requests on roadmap)
+  5 = Continuous engagement with joint planning, shared success metrics, and detection needs directly influencing product development</t>
         </is>
       </c>
       <c r="F26" s="13" t="n"/>
@@ -1756,7 +1767,7 @@
     <row r="27" ht="100" customHeight="1">
       <c r="A27" s="10" t="inlineStr">
         <is>
-          <t>T1-Q6</t>
+          <t>T1-Q9</t>
         </is>
       </c>
       <c r="B27" s="10" t="inlineStr">
@@ -1766,7 +1777,7 @@
       </c>
       <c r="C27" s="11" t="inlineStr">
         <is>
-          <t>Telemetry Quality</t>
+          <t>Release Testing and Validation</t>
         </is>
       </c>
       <c r="D27" s="10" t="inlineStr">
@@ -1776,12 +1787,12 @@
       </c>
       <c r="E27" s="12" t="inlineStr">
         <is>
-          <t>Rate the quality and coverage of the assessed team's telemetry.
-  1 = No active management; data sources unassessed
-  2 = Some awareness of gaps; basic health checks on critical sources
-  3 = Actively monitored; coverage mapped to detection needs; CTI integration starting
-  4 = Comprehensive with automated monitoring and CTI enrichment
-  5 = Advanced workflows with real-time enrichment and automated gap remediation</t>
+          <t>Rate the maturity of the assessed team's release testing.
+  1 = No testing; rules are deployed to production without validation (&lt;20% tested)
+  2 = Basic manual testing on some rules before deployment; no standardized process or test environment (20-40% tested)
+  3 = Standardized testing with defined test cases and a staging/test environment; most rules validated before deploy (50-70% tested)
+  4 = Comprehensive testing including unit tests, integration tests, and emulation-based validation; rapid deployment for emerging threats (70-90% automated; 24hr critical deployment capability)
+  5 = Continuous automated testing in full CI/CD pipeline; every rule validated before every deployment (90-100% automated)</t>
         </is>
       </c>
       <c r="F27" s="13" t="n"/>
@@ -1791,50 +1802,34 @@
       </c>
       <c r="H27" s="15" t="n"/>
     </row>
-    <row r="28" ht="60" customHeight="1">
-      <c r="A28" s="16" t="inlineStr">
-        <is>
-          <t>T1-Q7</t>
-        </is>
-      </c>
-      <c r="B28" s="16" t="inlineStr">
-        <is>
-          <t>Basic</t>
-        </is>
-      </c>
-      <c r="C28" s="17" t="inlineStr">
-        <is>
-          <t>Telemetry Quality</t>
-        </is>
-      </c>
-      <c r="D28" s="16" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="E28" s="18" t="inlineStr">
-        <is>
-          <t>Describe the assessed team's telemetry management. How is data quality ensured and coverage gaps identified?</t>
-        </is>
-      </c>
-      <c r="F28" s="15" t="n"/>
-      <c r="G28" s="19" t="inlineStr"/>
-      <c r="H28" s="15" t="n"/>
+    <row r="28" ht="30" customHeight="1">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Intermediate</t>
+        </is>
+      </c>
+      <c r="B28" s="9" t="n"/>
+      <c r="C28" s="9" t="n"/>
+      <c r="D28" s="9" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+      <c r="G28" s="9" t="n"/>
+      <c r="H28" s="9" t="n"/>
     </row>
     <row r="29" ht="100" customHeight="1">
       <c r="A29" s="10" t="inlineStr">
         <is>
-          <t>T1-Q8</t>
+          <t>T2-Q1</t>
         </is>
       </c>
       <c r="B29" s="10" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Intermediate</t>
         </is>
       </c>
       <c r="C29" s="11" t="inlineStr">
         <is>
-          <t>Threat Landscape Review</t>
+          <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
       <c r="D29" s="10" t="inlineStr">
@@ -1844,12 +1839,12 @@
       </c>
       <c r="E29" s="12" t="inlineStr">
         <is>
-          <t>How frequently does the assessed team review the threat landscape?
-  1 = No regular reviews
-  2 = Annually or bi-annually
-  3 = Quarterly with documented findings updating the roadmap
-  4 = Monthly integrated with threat intelligence
-  5 = Real-time monitoring with automated intel feeds</t>
+          <t>Rate the maturity of the assessed team's FP reduction program.
+  1 = Minimal or no tuning; high false positive rates accepted as normal; no FP metrics tracked
+  2 = Reactive tuning when analysts complain about noisy rules; no systematic tracking of FP rates (10-25% FP reduction from baseline)
+  3 = Regular tuning cycles (at least quarterly); FP rates tracked per rule; tuning is documented (25-50% FP reduction)
+  4 = Comprehensive FP management with automated tuning suggestions, risk-based alert scoring, and continuous monitoring (&gt;50% FP reduction)
+  5 = Automated dynamic tuning with ML; near-zero unnecessary alert noise; continuous optimization (&gt;75% FP reduction from baseline)</t>
         </is>
       </c>
       <c r="F29" s="13" t="n"/>
@@ -1862,17 +1857,17 @@
     <row r="30" ht="100" customHeight="1">
       <c r="A30" s="16" t="inlineStr">
         <is>
-          <t>T1-Q9</t>
+          <t>T2-Q2</t>
         </is>
       </c>
       <c r="B30" s="16" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Intermediate</t>
         </is>
       </c>
       <c r="C30" s="17" t="inlineStr">
         <is>
-          <t>Product Owner Engagement</t>
+          <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
       <c r="D30" s="16" t="inlineStr">
@@ -1882,12 +1877,12 @@
       </c>
       <c r="E30" s="18" t="inlineStr">
         <is>
-          <t>Rate the engagement between the assessed team and product/platform owners.
-  1 = No engagement with product owners
-  2 = Occasional ad hoc engagement, reactive to issues
-  3 = Regular engagement to communicate needs and provide feedback
-  4 = Proactive partnership; detection needs on product roadmaps
-  5 = Continuous engagement with joint planning and shared metrics</t>
+          <t>What is the assessed team's estimated FP reduction from baseline?
+  1 = Unknown or not measured
+  2 = Less than 25% reduction
+  3 = 25-50% reduction with per-rule FP rate tracking
+  4 = 50-75% reduction with automated tuning recommendations
+  5 = Over 75% reduction with ML-assisted continuous tuning</t>
         </is>
       </c>
       <c r="F30" s="13" t="n"/>
@@ -1897,95 +1892,114 @@
       </c>
       <c r="H30" s="15" t="n"/>
     </row>
-    <row r="31" ht="30" customHeight="1">
+    <row r="31" ht="100" customHeight="1">
       <c r="A31" s="10" t="inlineStr">
         <is>
-          <t>T1-Q10</t>
+          <t>T2-Q3</t>
         </is>
       </c>
       <c r="B31" s="10" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Intermediate</t>
         </is>
       </c>
       <c r="C31" s="11" t="inlineStr">
         <is>
-          <t>Release Testing and Validation</t>
+          <t>Gap Analysis and Documentation</t>
         </is>
       </c>
       <c r="D31" s="10" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E31" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team test rules before production deployment?</t>
+          <t>Rate the maturity of the assessed team's gap analysis.
+  1 = No gap analysis performed; detection coverage gaps are unknown
+  2 = Some gaps identified informally after incidents expose missing detections (1-3 gaps documented; reactive only)
+  3 = Regular analysis against ATT&amp;CK or similar frameworks at least quarterly; gaps documented, prioritized, and tracked (5+ gaps documented and prioritized)
+  4 = Comprehensive analysis integrated with threat modeling and risk assessment; gaps drive the detection roadmap (continuous tracking; integrated into roadmap)
+  5 = Automated gap analysis using coverage mapping tools; real-time dashboards showing detection coverage (automated continuous analysis)</t>
         </is>
       </c>
       <c r="F31" s="13" t="n"/>
       <c r="G31" s="14">
-        <f>IF(F31="Yes",3,IF(F31="No",1,""))</f>
+        <f>IF(F31="","",F31)</f>
         <v/>
       </c>
       <c r="H31" s="15" t="n"/>
     </row>
-    <row r="32" ht="100" customHeight="1">
+    <row r="32" ht="30" customHeight="1">
       <c r="A32" s="16" t="inlineStr">
         <is>
-          <t>T1-Q11</t>
+          <t>T2-Q4</t>
         </is>
       </c>
       <c r="B32" s="16" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>Intermediate</t>
         </is>
       </c>
       <c r="C32" s="17" t="inlineStr">
         <is>
-          <t>Release Testing and Validation</t>
+          <t>Gap Analysis and Documentation</t>
         </is>
       </c>
       <c r="D32" s="16" t="inlineStr">
         <is>
-          <t>Scale 1-5</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="E32" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's release testing.
-  1 = No formal testing before deployment
-  2 = Basic manual testing on some rules
-  3 = Standardized testing with defined test cases and staging environment
-  4 = Comprehensive testing with unit, integration, and emulation validation
-  5 = Continuous automated testing in full CI/CD pipeline</t>
+          <t>Does the assessed team maintain a documented, prioritized gap list updated quarterly?</t>
         </is>
       </c>
       <c r="F32" s="13" t="n"/>
       <c r="G32" s="19">
-        <f>IF(F32="","",F32)</f>
+        <f>IF(F32="Yes",3,IF(F32="No",1,""))</f>
         <v/>
       </c>
       <c r="H32" s="15" t="n"/>
     </row>
     <row r="33" ht="30" customHeight="1">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Intermediate</t>
-        </is>
-      </c>
-      <c r="B33" s="9" t="n"/>
-      <c r="C33" s="9" t="n"/>
-      <c r="D33" s="9" t="n"/>
-      <c r="E33" s="9" t="n"/>
-      <c r="F33" s="9" t="n"/>
-      <c r="G33" s="9" t="n"/>
-      <c r="H33" s="9" t="n"/>
-    </row>
-    <row r="34" ht="30" customHeight="1">
+      <c r="A33" s="10" t="inlineStr">
+        <is>
+          <t>T2-Q5</t>
+        </is>
+      </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C33" s="11" t="inlineStr">
+        <is>
+          <t>Gap Analysis and Documentation</t>
+        </is>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E33" s="12" t="inlineStr">
+        <is>
+          <t>Are the assessed team's gaps communicated to stakeholders at least quarterly?</t>
+        </is>
+      </c>
+      <c r="F33" s="13" t="n"/>
+      <c r="G33" s="14">
+        <f>IF(F33="Yes",4,IF(F33="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="H33" s="15" t="n"/>
+    </row>
+    <row r="34" ht="100" customHeight="1">
       <c r="A34" s="16" t="inlineStr">
         <is>
-          <t>T2-Q1</t>
+          <t>T2-Q6</t>
         </is>
       </c>
       <c r="B34" s="16" t="inlineStr">
@@ -1995,123 +2009,117 @@
       </c>
       <c r="C34" s="17" t="inlineStr">
         <is>
-          <t>False Positive Tuning and Reduction</t>
+          <t>Internal Testing and Validation</t>
         </is>
       </c>
       <c r="D34" s="16" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E34" s="18" t="inlineStr">
         <is>
-          <t>Does the assessed team track false positive rates per rule?</t>
+          <t>Rate the maturity of the assessed team's internal testing program.
+  1 = No internal testing; rules are assumed to work once deployed
+  2 = Occasional manual testing of high-priority rules using basic atomic tests (&lt;40% emulation coverage)
+  3 = Regular testing program with attack emulation (e.g., Atomic Red Team, Caldera) covering major detection categories; results documented (40-70% emulation coverage; at least quarterly)
+  4 = Comprehensive testing with automated attack emulation, purple team exercises, and continuous validation (70-90% automated emulation coverage)
+  5 = Continuous automated testing with full emulation coverage and automated regression testing on every rule change (&gt;90% automated coverage)</t>
         </is>
       </c>
       <c r="F34" s="13" t="n"/>
       <c r="G34" s="19">
-        <f>IF(F34="Yes",3,IF(F34="No",1,""))</f>
+        <f>IF(F34="","",F34)</f>
         <v/>
       </c>
       <c r="H34" s="15" t="n"/>
     </row>
-    <row r="35" ht="100" customHeight="1">
-      <c r="A35" s="10" t="inlineStr">
-        <is>
-          <t>T2-Q2</t>
-        </is>
-      </c>
-      <c r="B35" s="10" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="C35" s="11" t="inlineStr">
-        <is>
-          <t>False Positive Tuning and Reduction</t>
-        </is>
-      </c>
-      <c r="D35" s="10" t="inlineStr">
+    <row r="35" ht="30" customHeight="1">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Advanced</t>
+        </is>
+      </c>
+      <c r="B35" s="9" t="n"/>
+      <c r="C35" s="9" t="n"/>
+      <c r="D35" s="9" t="n"/>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+      <c r="G35" s="9" t="n"/>
+      <c r="H35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="100" customHeight="1">
+      <c r="A36" s="16" t="inlineStr">
+        <is>
+          <t>T3-Q1</t>
+        </is>
+      </c>
+      <c r="B36" s="16" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C36" s="17" t="inlineStr">
+        <is>
+          <t>False Negative Triage</t>
+        </is>
+      </c>
+      <c r="D36" s="16" t="inlineStr">
         <is>
           <t>Scale 1-5</t>
         </is>
       </c>
-      <c r="E35" s="12" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's FP reduction efforts.
-  1 = Minimal or no tuning; high FP rates accepted
-  2 = Some reactive tuning when analysts complain
-  3 = Regular tuning cycles with tracked FP rates per rule
-  4 = Comprehensive FP management with automated tuning and risk scoring
-  5 = Automated dynamic tuning with ML; near-zero unnecessary noise</t>
-        </is>
-      </c>
-      <c r="F35" s="13" t="n"/>
-      <c r="G35" s="14">
-        <f>IF(F35="","",F35)</f>
-        <v/>
-      </c>
-      <c r="H35" s="15" t="n"/>
-    </row>
-    <row r="36" ht="60" customHeight="1">
-      <c r="A36" s="16" t="inlineStr">
-        <is>
-          <t>T2-Q3</t>
-        </is>
-      </c>
-      <c r="B36" s="16" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="C36" s="17" t="inlineStr">
-        <is>
-          <t>False Positive Tuning and Reduction</t>
-        </is>
-      </c>
-      <c r="D36" s="16" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
       <c r="E36" s="18" t="inlineStr">
         <is>
-          <t>Describe the assessed team's FP management process, metrics tracked, and reduction achieved.</t>
-        </is>
-      </c>
-      <c r="F36" s="15" t="n"/>
-      <c r="G36" s="19" t="inlineStr"/>
+          <t>Rate the assessed team's ability to detect and remediate false negatives.
+  1 = No FN identification process; missed detections only discovered during incident response
+  2 = Some FNs identified through post-incident reviews; basic tracking of missed detections (50% of tested samples trigger expected alerts)
+  3 = Systematic FN identification through regular testing and validation; root causes analyzed and documented (70-90% trigger rate; 30-50% FN reduction)
+  4 = Comprehensive FN management with automated detection validation, coverage testing, and rapid remediation (90-100% trigger rate; &gt;50% FN reduction)
+  5 = Continuous automated FN detection using real-time validation against live threat samples (near-zero FN rate; &gt;75% FN reduction)</t>
+        </is>
+      </c>
+      <c r="F36" s="13" t="n"/>
+      <c r="G36" s="19">
+        <f>IF(F36="","",F36)</f>
+        <v/>
+      </c>
       <c r="H36" s="15" t="n"/>
     </row>
-    <row r="37" ht="30" customHeight="1">
+    <row r="37" ht="100" customHeight="1">
       <c r="A37" s="10" t="inlineStr">
         <is>
-          <t>T2-Q4</t>
+          <t>T3-Q2</t>
         </is>
       </c>
       <c r="B37" s="10" t="inlineStr">
         <is>
-          <t>Intermediate</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C37" s="11" t="inlineStr">
         <is>
-          <t>Gap Analysis and Documentation</t>
+          <t>False Negative Triage</t>
         </is>
       </c>
       <c r="D37" s="10" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E37" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team perform regular gap analysis against ATT&amp;CK or similar?</t>
+          <t>What is the assessed team's detection trigger rate on tested samples?
+  1 = Unknown or not tested
+  2 = Less than 50% of test samples trigger expected detections
+  3 = 50-70% trigger rate with root cause analysis on misses
+  4 = 70-90% trigger rate with automated validation and remediation
+  5 = Over 90% trigger rate with continuous regression testing</t>
         </is>
       </c>
       <c r="F37" s="13" t="n"/>
       <c r="G37" s="14">
-        <f>IF(F37="Yes",3,IF(F37="No",1,""))</f>
+        <f>IF(F37="","",F37)</f>
         <v/>
       </c>
       <c r="H37" s="15" t="n"/>
@@ -2119,17 +2127,17 @@
     <row r="38" ht="100" customHeight="1">
       <c r="A38" s="16" t="inlineStr">
         <is>
-          <t>T2-Q5</t>
+          <t>T3-Q3</t>
         </is>
       </c>
       <c r="B38" s="16" t="inlineStr">
         <is>
-          <t>Intermediate</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C38" s="17" t="inlineStr">
         <is>
-          <t>Gap Analysis and Documentation</t>
+          <t>External Validation</t>
         </is>
       </c>
       <c r="D38" s="16" t="inlineStr">
@@ -2139,12 +2147,12 @@
       </c>
       <c r="E38" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's gap analysis.
-  1 = No gap analysis; coverage gaps unknown
-  2 = Some gaps identified informally after incidents
-  3 = Regular analysis against frameworks; gaps documented and prioritized
-  4 = Comprehensive analysis integrated with threat modeling and risk
-  5 = Automated analysis with real-time coverage dashboards</t>
+          <t>Rate the maturity of the assessed team's external validation.
+  1 = No external validation; no red team, pentest, or third-party assessment of detection effectiveness
+  2 = Annual penetration test that includes some detection assessment but is not detection-focused (1 exercise per year)
+  3 = Regular external validation through red team engagements or third-party assessments specifically focused on detection effectiveness (&gt;1 per year; findings drive improvements)
+  4 = Multiple external validation exercises annually including red team, purple team, and breach simulation; systematic feedback integration (multiple per year; &gt;70% of findings remediated within 30 days)
+  5 = Continuous BAS (breach and attack simulation) tools and regular adversary emulation exercises with real-time feedback loops</t>
         </is>
       </c>
       <c r="F38" s="13" t="n"/>
@@ -2154,135 +2162,148 @@
       </c>
       <c r="H38" s="15" t="n"/>
     </row>
-    <row r="39" ht="60" customHeight="1">
+    <row r="39" ht="100" customHeight="1">
       <c r="A39" s="10" t="inlineStr">
         <is>
-          <t>T2-Q6</t>
+          <t>T3-Q4</t>
         </is>
       </c>
       <c r="B39" s="10" t="inlineStr">
         <is>
-          <t>Intermediate</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C39" s="11" t="inlineStr">
         <is>
-          <t>Gap Analysis and Documentation</t>
+          <t>Advanced TTP Coverage</t>
         </is>
       </c>
       <c r="D39" s="10" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E39" s="12" t="inlineStr">
         <is>
-          <t>Describe the assessed team's gap analysis process and how gaps are tracked and communicated.</t>
-        </is>
-      </c>
-      <c r="F39" s="15" t="n"/>
-      <c r="G39" s="14" t="inlineStr"/>
+          <t>Rate the assessed team's coverage of advanced TTPs.
+  1 = No advanced TTP coverage; detections are signature/IOC-based only
+  2 = Limited coverage of 1-2 advanced technique categories (e.g., basic PowerShell abuse detection)
+  3 = Growing coverage of 3-4 categories informed by threat intel; behavioral detections supplement signatures (e.g., LOLBin usage, fileless execution, credential access evasion)
+  4 = Comprehensive coverage of 5+ categories including sophisticated evasion, novel attack chains, and emerging threats (e.g., defense evasion/log tampering, lateral movement via legitimate tools, supply chain vectors)
+  5 = Continuous proactive coverage using AI/ML for anomaly detection and automated response to emerging TTPs; real-time advanced TTP detection</t>
+        </is>
+      </c>
+      <c r="F39" s="13" t="n"/>
+      <c r="G39" s="14">
+        <f>IF(F39="","",F39)</f>
+        <v/>
+      </c>
       <c r="H39" s="15" t="n"/>
     </row>
-    <row r="40" ht="30" customHeight="1">
+    <row r="40" ht="100" customHeight="1">
       <c r="A40" s="16" t="inlineStr">
         <is>
-          <t>T2-Q7</t>
+          <t>T3-Q5</t>
         </is>
       </c>
       <c r="B40" s="16" t="inlineStr">
         <is>
-          <t>Intermediate</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C40" s="17" t="inlineStr">
         <is>
-          <t>Internal Testing and Validation</t>
+          <t>Advanced TTP Coverage</t>
         </is>
       </c>
       <c r="D40" s="16" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E40" s="18" t="inlineStr">
         <is>
-          <t>Does the assessed team conduct attack emulation/simulation for validation?</t>
+          <t>How many of these categories does the assessed team have behavioral detections for: LOLBins, fileless malware, credential evasion, defense evasion, lateral movement?
+  1 = None of these
+  2 = 1 of these categories
+  3 = 2-3 of these categories
+  4 = 4-5 of these categories
+  5 = All 5 plus additional categories (e.g., supply chain attacks, AI-assisted threats)</t>
         </is>
       </c>
       <c r="F40" s="13" t="n"/>
       <c r="G40" s="19">
-        <f>IF(F40="Yes",3,IF(F40="No",1,""))</f>
+        <f>IF(F40="","",F40)</f>
         <v/>
       </c>
       <c r="H40" s="15" t="n"/>
     </row>
-    <row r="41" ht="100" customHeight="1">
-      <c r="A41" s="10" t="inlineStr">
-        <is>
-          <t>T2-Q8</t>
-        </is>
-      </c>
-      <c r="B41" s="10" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="C41" s="11" t="inlineStr">
-        <is>
-          <t>Internal Testing and Validation</t>
-        </is>
-      </c>
-      <c r="D41" s="10" t="inlineStr">
+    <row r="41" ht="30" customHeight="1">
+      <c r="A41" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Expert</t>
+        </is>
+      </c>
+      <c r="B41" s="9" t="n"/>
+      <c r="C41" s="9" t="n"/>
+      <c r="D41" s="9" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+      <c r="G41" s="9" t="n"/>
+      <c r="H41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="100" customHeight="1">
+      <c r="A42" s="16" t="inlineStr">
+        <is>
+          <t>T4-Q1</t>
+        </is>
+      </c>
+      <c r="B42" s="16" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="C42" s="17" t="inlineStr">
+        <is>
+          <t>Threat Hunting in Telemetry</t>
+        </is>
+      </c>
+      <c r="D42" s="16" t="inlineStr">
         <is>
           <t>Scale 1-5</t>
         </is>
       </c>
-      <c r="E41" s="12" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's internal testing program.
-  1 = No internal testing of detection effectiveness
-  2 = Occasional manual testing of high-priority rules
-  3 = Regular testing with attack emulation; results documented
-  4 = Comprehensive with automated emulation and purple team exercises
-  5 = Continuous automated testing with full emulation and regression</t>
-        </is>
-      </c>
-      <c r="F41" s="13" t="n"/>
-      <c r="G41" s="14">
-        <f>IF(F41="","",F41)</f>
-        <v/>
-      </c>
-      <c r="H41" s="15" t="n"/>
-    </row>
-    <row r="42" ht="30" customHeight="1">
-      <c r="A42" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Advanced</t>
-        </is>
-      </c>
-      <c r="B42" s="9" t="n"/>
-      <c r="C42" s="9" t="n"/>
-      <c r="D42" s="9" t="n"/>
-      <c r="E42" s="9" t="n"/>
-      <c r="F42" s="9" t="n"/>
-      <c r="G42" s="9" t="n"/>
-      <c r="H42" s="9" t="n"/>
+      <c r="E42" s="18" t="inlineStr">
+        <is>
+          <t>Rate the maturity of the assessed team's threat hunting.
+  1 = No proactive hunting; all detection is passive through deployed rules
+  2 = Occasional ad hoc hunting triggered by intel or incidents; findings not systematically converted to detections (fewer than 2 hunts/month; &lt;30% findings converted to rules)
+  3 = Regular structured hunting at least weekly, driven by documented hypotheses from intel or gap analysis; findings feed detection development (weekly hunts; 50-70% of findings integrated into rules)
+  4 = Comprehensive daily hunting program with advanced analytics (e.g., statistical baselining, graph analysis); systematic integration of all findings (daily hunts; &gt;90% findings integrated)
+  5 = Automated real-time hunting augmented by AI/ML; hunting outputs automatically generate detection rule candidates</t>
+        </is>
+      </c>
+      <c r="F42" s="13" t="n"/>
+      <c r="G42" s="19">
+        <f>IF(F42="","",F42)</f>
+        <v/>
+      </c>
+      <c r="H42" s="15" t="n"/>
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="10" t="inlineStr">
         <is>
-          <t>T3-Q1</t>
+          <t>T4-Q2</t>
         </is>
       </c>
       <c r="B43" s="10" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Expert</t>
         </is>
       </c>
       <c r="C43" s="11" t="inlineStr">
         <is>
-          <t>False Negative Triage</t>
+          <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
       <c r="D43" s="10" t="inlineStr">
@@ -2292,169 +2313,153 @@
       </c>
       <c r="E43" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team have a process for identifying and triaging false negatives?</t>
+          <t>Are the assessed team's hunts driven by documented hypotheses?</t>
         </is>
       </c>
       <c r="F43" s="13" t="n"/>
       <c r="G43" s="14">
-        <f>IF(F43="Yes",3,IF(F43="No",1,""))</f>
+        <f>IF(F43="Yes",4,IF(F43="No",1,""))</f>
         <v/>
       </c>
       <c r="H43" s="15" t="n"/>
     </row>
-    <row r="44" ht="100" customHeight="1">
+    <row r="44" ht="30" customHeight="1">
       <c r="A44" s="16" t="inlineStr">
         <is>
-          <t>T3-Q2</t>
+          <t>T4-Q3</t>
         </is>
       </c>
       <c r="B44" s="16" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Expert</t>
         </is>
       </c>
       <c r="C44" s="17" t="inlineStr">
         <is>
-          <t>False Negative Triage</t>
+          <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
         <is>
-          <t>Scale 1-5</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="E44" s="18" t="inlineStr">
         <is>
-          <t>Rate the assessed team's ability to detect and remediate false negatives.
-  1 = No FN identification; missed detections only found during incidents
-  2 = Some FNs identified through post-incident reviews
-  3 = Systematic FN identification through regular testing; root causes analyzed
-  4 = Comprehensive with automated validation and rapid remediation
-  5 = Continuous automated FN detection with real-time validation</t>
+          <t>Is there a defined process to convert hunting findings into production rules?</t>
         </is>
       </c>
       <c r="F44" s="13" t="n"/>
       <c r="G44" s="19">
-        <f>IF(F44="","",F44)</f>
+        <f>IF(F44="Yes",4,IF(F44="No",1,""))</f>
         <v/>
       </c>
       <c r="H44" s="15" t="n"/>
     </row>
-    <row r="45" ht="60" customHeight="1">
+    <row r="45" ht="100" customHeight="1">
       <c r="A45" s="10" t="inlineStr">
         <is>
-          <t>T3-Q3</t>
+          <t>T4-Q4</t>
         </is>
       </c>
       <c r="B45" s="10" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Expert</t>
         </is>
       </c>
       <c r="C45" s="11" t="inlineStr">
         <is>
-          <t>False Negative Triage</t>
+          <t>Automation and Continuous Improvement</t>
         </is>
       </c>
       <c r="D45" s="10" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E45" s="12" t="inlineStr">
         <is>
-          <t>Describe the assessed team's FN identification and remediation process and detection trigger rates.</t>
-        </is>
-      </c>
-      <c r="F45" s="15" t="n"/>
-      <c r="G45" s="14" t="inlineStr"/>
+          <t>What percentage of the assessed team's DE tasks are automated?
+  1 = None; all processes are manual (0% automated)
+  2 = Basic automation of some repetitive tasks like deployment scripts (&lt;30% automated)
+  3 = Significant lifecycle automation including AI-based quality checks on new rules; improvement metrics tracked (40-60% automated)
+  4 = Advanced automation covering most of the lifecycle; AI/LLM tools used for rule optimization, duplication detection, and analysis (70-80% automated)
+  5 = Full AI/LLM integration throughout the detection lifecycle; automated rule generation, tuning, and retirement (&gt;90% automated; 40%+ FP reduction via AI)</t>
+        </is>
+      </c>
+      <c r="F45" s="13" t="n"/>
+      <c r="G45" s="14">
+        <f>IF(F45="","",F45)</f>
+        <v/>
+      </c>
       <c r="H45" s="15" t="n"/>
     </row>
-    <row r="46" ht="30" customHeight="1">
+    <row r="46" ht="100" customHeight="1">
       <c r="A46" s="16" t="inlineStr">
         <is>
-          <t>T3-Q4</t>
+          <t>T4-Q5</t>
         </is>
       </c>
       <c r="B46" s="16" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Expert</t>
         </is>
       </c>
       <c r="C46" s="17" t="inlineStr">
         <is>
-          <t>External Validation</t>
+          <t>Automation and Continuous Improvement</t>
         </is>
       </c>
       <c r="D46" s="16" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E46" s="18" t="inlineStr">
         <is>
-          <t>Does the assessed organization conduct external validation of detections?</t>
+          <t>How many detection lifecycle stages have automation or AI integration?
+  1 = None; all stages are manual
+  2 = 1 stage (e.g., deployment scripts only)
+  3 = 2-3 stages automated or AI-assisted
+  4 = 4-5 stages automated or AI-assisted
+  5 = All 6 stages with AI/LLM integration throughout</t>
         </is>
       </c>
       <c r="F46" s="13" t="n"/>
       <c r="G46" s="19">
-        <f>IF(F46="Yes",3,IF(F46="No",1,""))</f>
+        <f>IF(F46="","",F46)</f>
         <v/>
       </c>
       <c r="H46" s="15" t="n"/>
     </row>
-    <row r="47" ht="100" customHeight="1">
-      <c r="A47" s="10" t="inlineStr">
-        <is>
-          <t>T3-Q5</t>
-        </is>
-      </c>
-      <c r="B47" s="10" t="inlineStr">
-        <is>
-          <t>Advanced</t>
-        </is>
-      </c>
-      <c r="C47" s="11" t="inlineStr">
-        <is>
-          <t>External Validation</t>
-        </is>
-      </c>
-      <c r="D47" s="10" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E47" s="12" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's external validation.
-  1 = No external validation of detections
-  2 = Annual pentest with some detection assessment
-  3 = Regular red team or third-party assessments focused on detection
-  4 = Multiple annual exercises (red/purple team, breach simulation)
-  5 = Continuous BAS tools and regular adversary emulation</t>
-        </is>
-      </c>
-      <c r="F47" s="13" t="n"/>
-      <c r="G47" s="14">
-        <f>IF(F47="","",F47)</f>
-        <v/>
-      </c>
-      <c r="H47" s="15" t="n"/>
+    <row r="47" ht="30" customHeight="1">
+      <c r="A47" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Enrichment: People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="B47" s="9" t="n"/>
+      <c r="C47" s="9" t="n"/>
+      <c r="D47" s="9" t="n"/>
+      <c r="E47" s="9" t="n"/>
+      <c r="F47" s="9" t="n"/>
+      <c r="G47" s="9" t="n"/>
+      <c r="H47" s="9" t="n"/>
     </row>
     <row r="48" ht="100" customHeight="1">
       <c r="A48" s="16" t="inlineStr">
         <is>
-          <t>T3-Q6</t>
+          <t>EP-Q1</t>
         </is>
       </c>
       <c r="B48" s="16" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Enrichment: People &amp; Organization</t>
         </is>
       </c>
       <c r="C48" s="17" t="inlineStr">
         <is>
-          <t>Advanced TTP Coverage</t>
+          <t>Team Structure and Dedicated Roles</t>
         </is>
       </c>
       <c r="D48" s="16" t="inlineStr">
@@ -2464,12 +2469,12 @@
       </c>
       <c r="E48" s="18" t="inlineStr">
         <is>
-          <t>Rate the assessed team's coverage of advanced TTPs.
-  1 = No advanced TTP coverage; signatures and IOCs only
-  2 = Limited coverage of 1-3 advanced techniques
-  3 = Growing coverage informed by intel; behavioral detections in place
-  4 = Comprehensive coverage of evasion, novel attack chains, emerging threats
-  5 = Continuous proactive coverage using AI/ML for anomaly detection</t>
+          <t>Rate the maturity of the assessed detection engineering team structure.
+  1 = No dedicated roles; detection work is a side task for SOC analysts or other staff (0 dedicated FTEs)
+  2 = One or more staff have detection engineering as a partial responsibility; no formal team or career path
+  3 = At least one dedicated detection engineering role or team established with clear responsibilities and defined career progression
+  4 = Established multi-person team with subject matter experts across key domains (host, network, cloud, application); defined career ladder
+  5 = Mature team with deep specialization, mentorship programs, and influence on organizational security strategy</t>
         </is>
       </c>
       <c r="F48" s="13" t="n"/>
@@ -2479,64 +2484,96 @@
       </c>
       <c r="H48" s="15" t="n"/>
     </row>
-    <row r="49" ht="60" customHeight="1">
+    <row r="49" ht="100" customHeight="1">
       <c r="A49" s="10" t="inlineStr">
         <is>
-          <t>T3-Q7</t>
+          <t>EP-Q2</t>
         </is>
       </c>
       <c r="B49" s="10" t="inlineStr">
         <is>
-          <t>Advanced</t>
+          <t>Enrichment: People &amp; Organization</t>
         </is>
       </c>
       <c r="C49" s="11" t="inlineStr">
         <is>
-          <t>Advanced TTP Coverage</t>
+          <t>Skills Development and Training</t>
         </is>
       </c>
       <c r="D49" s="10" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E49" s="12" t="inlineStr">
         <is>
-          <t>Describe the assessed team's advanced TTP detection capabilities and specific techniques covered.</t>
-        </is>
-      </c>
-      <c r="F49" s="15" t="n"/>
-      <c r="G49" s="14" t="inlineStr"/>
+          <t>Rate the maturity of the assessed team's skills development.
+  1 = No formal training; learning is entirely self-directed with no organizational support or budget
+  2 = Ad hoc training; individuals may attend a conference or take a course occasionally but there is no structured program
+  3 = Written training plan with scheduled activities; regular knowledge sharing sessions (e.g., weekly/biweekly); defined skill requirements for roles
+  4 = Comprehensive program covering advanced topics; cross-training with IR, threat intel, and engineering teams; certifications supported and funded
+  5 = Continuous learning culture with community contribution (blog posts, conference talks), internal research programs, and mentorship</t>
+        </is>
+      </c>
+      <c r="F49" s="13" t="n"/>
+      <c r="G49" s="14">
+        <f>IF(F49="","",F49)</f>
+        <v/>
+      </c>
       <c r="H49" s="15" t="n"/>
     </row>
-    <row r="50" ht="30" customHeight="1">
-      <c r="A50" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Expert</t>
-        </is>
-      </c>
-      <c r="B50" s="9" t="n"/>
-      <c r="C50" s="9" t="n"/>
-      <c r="D50" s="9" t="n"/>
-      <c r="E50" s="9" t="n"/>
-      <c r="F50" s="9" t="n"/>
-      <c r="G50" s="9" t="n"/>
-      <c r="H50" s="9" t="n"/>
+    <row r="50" ht="100" customHeight="1">
+      <c r="A50" s="16" t="inlineStr">
+        <is>
+          <t>EP-Q3</t>
+        </is>
+      </c>
+      <c r="B50" s="16" t="inlineStr">
+        <is>
+          <t>Enrichment: People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="C50" s="17" t="inlineStr">
+        <is>
+          <t>Leadership Commitment and Executive Sponsorship</t>
+        </is>
+      </c>
+      <c r="D50" s="16" t="inlineStr">
+        <is>
+          <t>Scale 1-5</t>
+        </is>
+      </c>
+      <c r="E50" s="18" t="inlineStr">
+        <is>
+          <t>Rate the executive sponsorship of the assessed detection engineering function.
+  1 = No executive awareness; detection engineering is not recognized as a distinct capability
+  2 = Some leadership awareness but no formal executive sponsor, no dedicated budget allocation
+  3 = Executive sponsor identified; dedicated budget for tooling and headcount; detection engineering formally recognized as a function
+  4 = Strong executive support; detection engineering metrics included in regular executive reporting; function influences security investment decisions
+  5 = Detection engineering is a strategic priority; board-level visibility; leadership actively champions the function across the organization</t>
+        </is>
+      </c>
+      <c r="F50" s="13" t="n"/>
+      <c r="G50" s="19">
+        <f>IF(F50="","",F50)</f>
+        <v/>
+      </c>
+      <c r="H50" s="15" t="n"/>
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="10" t="inlineStr">
         <is>
-          <t>T4-Q1</t>
+          <t>EP-Q4</t>
         </is>
       </c>
       <c r="B51" s="10" t="inlineStr">
         <is>
-          <t>Expert</t>
+          <t>Enrichment: People &amp; Organization</t>
         </is>
       </c>
       <c r="C51" s="11" t="inlineStr">
         <is>
-          <t>Threat Hunting in Telemetry</t>
+          <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
       <c r="D51" s="10" t="inlineStr">
@@ -2546,7 +2583,7 @@
       </c>
       <c r="E51" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team conduct proactive threat hunting?</t>
+          <t>Does the assessed team present metrics to executive leadership at least quarterly?</t>
         </is>
       </c>
       <c r="F51" s="13" t="n"/>
@@ -2556,88 +2593,67 @@
       </c>
       <c r="H51" s="15" t="n"/>
     </row>
-    <row r="52" ht="100" customHeight="1">
+    <row r="52" ht="30" customHeight="1">
       <c r="A52" s="16" t="inlineStr">
         <is>
-          <t>T4-Q2</t>
+          <t>EP-Q5</t>
         </is>
       </c>
       <c r="B52" s="16" t="inlineStr">
         <is>
-          <t>Expert</t>
+          <t>Enrichment: People &amp; Organization</t>
         </is>
       </c>
       <c r="C52" s="17" t="inlineStr">
         <is>
-          <t>Threat Hunting in Telemetry</t>
+          <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
       <c r="D52" s="16" t="inlineStr">
         <is>
-          <t>Scale 1-5</t>
+          <t>Yes/No</t>
         </is>
       </c>
       <c r="E52" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's threat hunting.
-  1 = No proactive hunting; all detection is passive
-  2 = Occasional ad hoc hunting; findings not systematically converted
-  3 = Regular structured hunting driven by intelligence; findings feed detections
-  4 = Comprehensive daily program with advanced analytics and integration
-  5 = Automated real-time hunting augmented by AI/ML</t>
+          <t>Has leadership made investment/staffing decisions based on the assessed team's metrics in the past year?</t>
         </is>
       </c>
       <c r="F52" s="13" t="n"/>
       <c r="G52" s="19">
-        <f>IF(F52="","",F52)</f>
+        <f>IF(F52="Yes",4,IF(F52="No",1,""))</f>
         <v/>
       </c>
       <c r="H52" s="15" t="n"/>
     </row>
-    <row r="53" ht="60" customHeight="1">
-      <c r="A53" s="10" t="inlineStr">
-        <is>
-          <t>T4-Q3</t>
-        </is>
-      </c>
-      <c r="B53" s="10" t="inlineStr">
-        <is>
-          <t>Expert</t>
-        </is>
-      </c>
-      <c r="C53" s="11" t="inlineStr">
-        <is>
-          <t>Threat Hunting in Telemetry</t>
-        </is>
-      </c>
-      <c r="D53" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="E53" s="12" t="inlineStr">
-        <is>
-          <t>Describe the assessed team's hunting program, hypothesis process, and finding integration.</t>
-        </is>
-      </c>
-      <c r="F53" s="15" t="n"/>
-      <c r="G53" s="14" t="inlineStr"/>
-      <c r="H53" s="15" t="n"/>
+    <row r="53" ht="30" customHeight="1">
+      <c r="A53" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Enrichment: Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="B53" s="9" t="n"/>
+      <c r="C53" s="9" t="n"/>
+      <c r="D53" s="9" t="n"/>
+      <c r="E53" s="9" t="n"/>
+      <c r="F53" s="9" t="n"/>
+      <c r="G53" s="9" t="n"/>
+      <c r="H53" s="9" t="n"/>
     </row>
     <row r="54" ht="100" customHeight="1">
       <c r="A54" s="16" t="inlineStr">
         <is>
-          <t>T4-Q4</t>
+          <t>EG-Q1</t>
         </is>
       </c>
       <c r="B54" s="16" t="inlineStr">
         <is>
-          <t>Expert</t>
+          <t>Enrichment: Process &amp; Governance</t>
         </is>
       </c>
       <c r="C54" s="17" t="inlineStr">
         <is>
-          <t>Automation and Continuous Improvement</t>
+          <t>Detection Lifecycle Workflow</t>
         </is>
       </c>
       <c r="D54" s="16" t="inlineStr">
@@ -2647,12 +2663,12 @@
       </c>
       <c r="E54" s="18" t="inlineStr">
         <is>
-          <t>What percentage of the assessed team's DE tasks are automated?
-  1 = None; all processes are manual
-  2 = Less than 30% (basic deployment scripts)
-  3 = 40-60% (lifecycle automation; improvement metrics tracked)
-  4 = 70-80% (advanced automation; AI/LLM tools in use)
-  5 = Over 90% (full AI/LLM lifecycle integration)</t>
+          <t>Rate the maturity of the assessed team's detection lifecycle workflow.
+  1 = No defined lifecycle; detections created and deployed without structured workflow
+  2 = Basic lifecycle covering creation and deployment only; no formal stages for review, testing, or retirement (2-3 stages defined)
+  3 = Full lifecycle defined and followed: request, development, review, testing, deployment, monitoring, and retirement (all 7 stages documented)
+  4 = Lifecycle enforced through tooling and automation; SLAs defined for each stage; cycle time and throughput metrics tracked
+  5 = Optimized lifecycle with automated stage transitions, predictive analytics for rule retirement, and continuous process improvement</t>
         </is>
       </c>
       <c r="F54" s="13" t="n"/>
@@ -2662,600 +2678,137 @@
       </c>
       <c r="H54" s="15" t="n"/>
     </row>
-    <row r="55" ht="30" customHeight="1">
+    <row r="55" ht="100" customHeight="1">
       <c r="A55" s="10" t="inlineStr">
         <is>
-          <t>T4-Q5</t>
+          <t>EG-Q2</t>
         </is>
       </c>
       <c r="B55" s="10" t="inlineStr">
         <is>
-          <t>Expert</t>
+          <t>Enrichment: Process &amp; Governance</t>
         </is>
       </c>
       <c r="C55" s="11" t="inlineStr">
         <is>
-          <t>Automation and Continuous Improvement</t>
+          <t>Metrics and KPI Tracking</t>
         </is>
       </c>
       <c r="D55" s="10" t="inlineStr">
         <is>
-          <t>Yes/No</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E55" s="12" t="inlineStr">
         <is>
-          <t>Does the assessed team use AI/LLM tools for detection work?</t>
+          <t>Rate the maturity of the assessed team's metrics program.
+  1 = No metrics tracked; success is anecdotal or unmeasured
+  2 = 1-2 basic metrics tracked informally (e.g., rule count, alert volume); no formal KPI program or dashboards
+  3 = 3-5 defined KPIs covering key areas with quarterly reporting and dashboards (e.g., coverage %, FP rate, deployment velocity)
+  4 = 5+ KPIs with automated collection, trending, and correlation; metrics actively drive decision-making and resource allocation
+  5 = Advanced analytics with predictive metrics, industry benchmarking, and data-driven continuous optimization</t>
         </is>
       </c>
       <c r="F55" s="13" t="n"/>
       <c r="G55" s="14">
-        <f>IF(F55="Yes",4,IF(F55="No",1,""))</f>
+        <f>IF(F55="","",F55)</f>
         <v/>
       </c>
       <c r="H55" s="15" t="n"/>
     </row>
-    <row r="56" ht="60" customHeight="1">
+    <row r="56" ht="100" customHeight="1">
       <c r="A56" s="16" t="inlineStr">
         <is>
-          <t>T4-Q6</t>
+          <t>EG-Q3</t>
         </is>
       </c>
       <c r="B56" s="16" t="inlineStr">
         <is>
-          <t>Expert</t>
+          <t>Enrichment: Process &amp; Governance</t>
         </is>
       </c>
       <c r="C56" s="17" t="inlineStr">
         <is>
-          <t>Automation and Continuous Improvement</t>
+          <t>Metrics and KPI Tracking</t>
         </is>
       </c>
       <c r="D56" s="16" t="inlineStr">
         <is>
-          <t>Text</t>
+          <t>Scale 1-5</t>
         </is>
       </c>
       <c r="E56" s="18" t="inlineStr">
         <is>
-          <t>Describe the assessed team's automation and AI/LLM integration, tools used, and results.</t>
-        </is>
-      </c>
-      <c r="F56" s="15" t="n"/>
-      <c r="G56" s="19" t="inlineStr"/>
+          <t>How many of these KPI categories does the assessed team track: coverage, quality, velocity, rule health, analyst impact?
+  1 = None of these are tracked
+  2 = 1 category tracked
+  3 = 2-3 categories tracked with regular reporting
+  4 = 4-5 categories tracked with automated collection and dashboards
+  5 = All 5 categories plus additional metrics with trend analysis and benchmarking</t>
+        </is>
+      </c>
+      <c r="F56" s="13" t="n"/>
+      <c r="G56" s="19">
+        <f>IF(F56="","",F56)</f>
+        <v/>
+      </c>
       <c r="H56" s="15" t="n"/>
     </row>
-    <row r="57" ht="30" customHeight="1">
-      <c r="A57" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="B57" s="9" t="n"/>
-      <c r="C57" s="9" t="n"/>
-      <c r="D57" s="9" t="n"/>
-      <c r="E57" s="9" t="n"/>
-      <c r="F57" s="9" t="n"/>
-      <c r="G57" s="9" t="n"/>
-      <c r="H57" s="9" t="n"/>
-    </row>
-    <row r="58" ht="100" customHeight="1">
-      <c r="A58" s="16" t="inlineStr">
-        <is>
-          <t>EP-Q1</t>
-        </is>
-      </c>
-      <c r="B58" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C58" s="17" t="inlineStr">
-        <is>
-          <t>Team Structure and Dedicated Roles</t>
-        </is>
-      </c>
-      <c r="D58" s="16" t="inlineStr">
+    <row r="57" ht="100" customHeight="1">
+      <c r="A57" s="10" t="inlineStr">
+        <is>
+          <t>EG-Q4</t>
+        </is>
+      </c>
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>Enrichment: Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="C57" s="11" t="inlineStr">
+        <is>
+          <t>Cross-Team Collaboration</t>
+        </is>
+      </c>
+      <c r="D57" s="10" t="inlineStr">
         <is>
           <t>Scale 1-5</t>
         </is>
       </c>
-      <c r="E58" s="18" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed detection engineering team structure.
-  1 = No dedicated roles; detection is a side task for other staff
-  2 = Part-time detection responsibilities; no formal team
-  3 = Dedicated role(s) or team with clear responsibilities
-  4 = Established team with domain experts (host, network, cloud, app)
-  5 = Mature team with specialization, mentorship, and strategic influence</t>
-        </is>
-      </c>
-      <c r="F58" s="13" t="n"/>
-      <c r="G58" s="19">
-        <f>IF(F58="","",F58)</f>
-        <v/>
-      </c>
-      <c r="H58" s="15" t="n"/>
-    </row>
-    <row r="59" ht="30" customHeight="1">
-      <c r="A59" s="10" t="inlineStr">
-        <is>
-          <t>EP-Q2</t>
-        </is>
-      </c>
-      <c r="B59" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C59" s="11" t="inlineStr">
-        <is>
-          <t>Team Structure and Dedicated Roles</t>
-        </is>
-      </c>
-      <c r="D59" s="10" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E59" s="12" t="inlineStr">
-        <is>
-          <t>Does the assessed organization have at least one dedicated detection engineer?</t>
-        </is>
-      </c>
-      <c r="F59" s="13" t="n"/>
-      <c r="G59" s="14">
-        <f>IF(F59="Yes",3,IF(F59="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H59" s="15" t="n"/>
-    </row>
-    <row r="60" ht="100" customHeight="1">
-      <c r="A60" s="16" t="inlineStr">
-        <is>
-          <t>EP-Q3</t>
-        </is>
-      </c>
-      <c r="B60" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C60" s="17" t="inlineStr">
-        <is>
-          <t>Skills Development and Training</t>
-        </is>
-      </c>
-      <c r="D60" s="16" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E60" s="18" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's skills development.
-  1 = No formal training; self-directed learning only
-  2 = Ad hoc training; no structured program
-  3 = Defined training program with regular knowledge sharing
-  4 = Comprehensive training with cross-training and certifications
-  5 = Continuous learning culture with community contribution and research</t>
-        </is>
-      </c>
-      <c r="F60" s="13" t="n"/>
-      <c r="G60" s="19">
-        <f>IF(F60="","",F60)</f>
-        <v/>
-      </c>
-      <c r="H60" s="15" t="n"/>
-    </row>
-    <row r="61" ht="30" customHeight="1">
-      <c r="A61" s="10" t="inlineStr">
-        <is>
-          <t>EP-Q4</t>
-        </is>
-      </c>
-      <c r="B61" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C61" s="11" t="inlineStr">
-        <is>
-          <t>Skills Development and Training</t>
-        </is>
-      </c>
-      <c r="D61" s="10" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E61" s="12" t="inlineStr">
-        <is>
-          <t>Does the assessed team have a defined training plan or skills roadmap?</t>
-        </is>
-      </c>
-      <c r="F61" s="13" t="n"/>
-      <c r="G61" s="14">
-        <f>IF(F61="Yes",3,IF(F61="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H61" s="15" t="n"/>
-    </row>
-    <row r="62" ht="100" customHeight="1">
-      <c r="A62" s="16" t="inlineStr">
-        <is>
-          <t>EP-Q5</t>
-        </is>
-      </c>
-      <c r="B62" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C62" s="17" t="inlineStr">
-        <is>
-          <t>Leadership Commitment and Executive Sponsorship</t>
-        </is>
-      </c>
-      <c r="D62" s="16" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E62" s="18" t="inlineStr">
-        <is>
-          <t>Rate the executive sponsorship of the assessed detection engineering function.
-  1 = No executive awareness or sponsorship
-  2 = Some awareness but no formal sponsorship or budget
-  3 = Executive sponsor; dedicated budget; function formally recognized
-  4 = Strong support; metrics reported to leadership; influences investments
-  5 = Strategic priority; board-level visibility; cross-org influence</t>
-        </is>
-      </c>
-      <c r="F62" s="13" t="n"/>
-      <c r="G62" s="19">
-        <f>IF(F62="","",F62)</f>
-        <v/>
-      </c>
-      <c r="H62" s="15" t="n"/>
-    </row>
-    <row r="63" ht="30" customHeight="1">
-      <c r="A63" s="10" t="inlineStr">
-        <is>
-          <t>EP-Q6</t>
-        </is>
-      </c>
-      <c r="B63" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C63" s="11" t="inlineStr">
-        <is>
-          <t>Leadership Commitment and Executive Sponsorship</t>
-        </is>
-      </c>
-      <c r="D63" s="10" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E63" s="12" t="inlineStr">
-        <is>
-          <t>Does the assessed detection engineering function have a dedicated budget?</t>
-        </is>
-      </c>
-      <c r="F63" s="13" t="n"/>
-      <c r="G63" s="14">
-        <f>IF(F63="Yes",3,IF(F63="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H63" s="15" t="n"/>
-    </row>
-    <row r="64" ht="60" customHeight="1">
-      <c r="A64" s="16" t="inlineStr">
-        <is>
-          <t>EP-Q7</t>
-        </is>
-      </c>
-      <c r="B64" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="C64" s="17" t="inlineStr">
-        <is>
-          <t>Leadership Commitment and Executive Sponsorship</t>
-        </is>
-      </c>
-      <c r="D64" s="16" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="E64" s="18" t="inlineStr">
-        <is>
-          <t>Describe executive engagement with the assessed detection engineering function.</t>
-        </is>
-      </c>
-      <c r="F64" s="15" t="n"/>
-      <c r="G64" s="19" t="inlineStr"/>
-      <c r="H64" s="15" t="n"/>
-    </row>
-    <row r="65" ht="30" customHeight="1">
-      <c r="A65" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="B65" s="9" t="n"/>
-      <c r="C65" s="9" t="n"/>
-      <c r="D65" s="9" t="n"/>
-      <c r="E65" s="9" t="n"/>
-      <c r="F65" s="9" t="n"/>
-      <c r="G65" s="9" t="n"/>
-      <c r="H65" s="9" t="n"/>
-    </row>
-    <row r="66" ht="100" customHeight="1">
-      <c r="A66" s="16" t="inlineStr">
-        <is>
-          <t>EG-Q1</t>
-        </is>
-      </c>
-      <c r="B66" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C66" s="17" t="inlineStr">
-        <is>
-          <t>Detection Lifecycle Workflow</t>
-        </is>
-      </c>
-      <c r="D66" s="16" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E66" s="18" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's detection lifecycle workflow.
-  1 = No defined lifecycle; no structured workflow
-  2 = Basic lifecycle covering creation and deployment only
-  3 = Full lifecycle: request, development, review, testing, deploy, monitor, retire
-  4 = Enforced through tooling; SLAs defined; cycle time tracked
-  5 = Optimized with automated transitions and predictive analytics</t>
-        </is>
-      </c>
-      <c r="F66" s="13" t="n"/>
-      <c r="G66" s="19">
-        <f>IF(F66="","",F66)</f>
-        <v/>
-      </c>
-      <c r="H66" s="15" t="n"/>
-    </row>
-    <row r="67" ht="30" customHeight="1">
-      <c r="A67" s="10" t="inlineStr">
-        <is>
-          <t>EG-Q2</t>
-        </is>
-      </c>
-      <c r="B67" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C67" s="11" t="inlineStr">
-        <is>
-          <t>Detection Lifecycle Workflow</t>
-        </is>
-      </c>
-      <c r="D67" s="10" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E67" s="12" t="inlineStr">
-        <is>
-          <t>Does the assessed team have a rule retirement/deprecation process?</t>
-        </is>
-      </c>
-      <c r="F67" s="13" t="n"/>
-      <c r="G67" s="14">
-        <f>IF(F67="Yes",3,IF(F67="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H67" s="15" t="n"/>
-    </row>
-    <row r="68" ht="30" customHeight="1">
-      <c r="A68" s="16" t="inlineStr">
-        <is>
-          <t>EG-Q3</t>
-        </is>
-      </c>
-      <c r="B68" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C68" s="17" t="inlineStr">
-        <is>
-          <t>Metrics and KPI Tracking</t>
-        </is>
-      </c>
-      <c r="D68" s="16" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E68" s="18" t="inlineStr">
-        <is>
-          <t>Does the assessed team track detection engineering KPIs?</t>
-        </is>
-      </c>
-      <c r="F68" s="13" t="n"/>
-      <c r="G68" s="19">
-        <f>IF(F68="Yes",3,IF(F68="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H68" s="15" t="n"/>
-    </row>
-    <row r="69" ht="100" customHeight="1">
-      <c r="A69" s="10" t="inlineStr">
-        <is>
-          <t>EG-Q4</t>
-        </is>
-      </c>
-      <c r="B69" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C69" s="11" t="inlineStr">
-        <is>
-          <t>Metrics and KPI Tracking</t>
-        </is>
-      </c>
-      <c r="D69" s="10" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E69" s="12" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's metrics program.
-  1 = No metrics tracked; success is anecdotal
-  2 = Basic metrics tracked informally (rule count, alert volume)
-  3 = Defined KPIs for coverage, quality, velocity; quarterly reporting
-  4 = Comprehensive program with automated collection; metrics drive decisions
-  5 = Advanced analytics with predictive metrics and benchmarking</t>
-        </is>
-      </c>
-      <c r="F69" s="13" t="n"/>
-      <c r="G69" s="14">
-        <f>IF(F69="","",F69)</f>
-        <v/>
-      </c>
-      <c r="H69" s="15" t="n"/>
-    </row>
-    <row r="70" ht="60" customHeight="1">
-      <c r="A70" s="16" t="inlineStr">
-        <is>
-          <t>EG-Q5</t>
-        </is>
-      </c>
-      <c r="B70" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C70" s="17" t="inlineStr">
-        <is>
-          <t>Metrics and KPI Tracking</t>
-        </is>
-      </c>
-      <c r="D70" s="16" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="E70" s="18" t="inlineStr">
-        <is>
-          <t>List the KPIs tracked by the assessed team and describe collection and reporting.</t>
-        </is>
-      </c>
-      <c r="F70" s="15" t="n"/>
-      <c r="G70" s="19" t="inlineStr"/>
-      <c r="H70" s="15" t="n"/>
-    </row>
-    <row r="71" ht="100" customHeight="1">
-      <c r="A71" s="10" t="inlineStr">
-        <is>
-          <t>EG-Q6</t>
-        </is>
-      </c>
-      <c r="B71" s="10" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C71" s="11" t="inlineStr">
-        <is>
-          <t>Cross-Team Collaboration</t>
-        </is>
-      </c>
-      <c r="D71" s="10" t="inlineStr">
-        <is>
-          <t>Scale 1-5</t>
-        </is>
-      </c>
-      <c r="E71" s="12" t="inlineStr">
+      <c r="E57" s="12" t="inlineStr">
         <is>
           <t>Rate cross-team collaboration involving the assessed detection engineering function.
-  1 = Operates in isolation; no structured collaboration
-  2 = Ad hoc collaboration, reactive to incidents
-  3 = Regular collaboration via defined channels and scheduled touchpoints
-  4 = Deep integration with joint planning and shared objectives
-  5 = Seamless cross-functional collaboration with automated information sharing</t>
-        </is>
-      </c>
-      <c r="F71" s="13" t="n"/>
-      <c r="G71" s="14">
-        <f>IF(F71="","",F71)</f>
-        <v/>
-      </c>
-      <c r="H71" s="15" t="n"/>
-    </row>
-    <row r="72" ht="30" customHeight="1">
-      <c r="A72" s="16" t="inlineStr">
-        <is>
-          <t>EG-Q7</t>
-        </is>
-      </c>
-      <c r="B72" s="16" t="inlineStr">
-        <is>
-          <t>Enrichment: Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="C72" s="17" t="inlineStr">
-        <is>
-          <t>Cross-Team Collaboration</t>
-        </is>
-      </c>
-      <c r="D72" s="16" t="inlineStr">
-        <is>
-          <t>Yes/No</t>
-        </is>
-      </c>
-      <c r="E72" s="18" t="inlineStr">
-        <is>
-          <t>Does the assessed team have regular touchpoints with IR and threat intel?</t>
-        </is>
-      </c>
-      <c r="F72" s="13" t="n"/>
-      <c r="G72" s="19">
-        <f>IF(F72="Yes",3,IF(F72="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="H72" s="15" t="n"/>
+  1 = Operates in isolation; no structured collaboration with other teams
+  2 = Ad hoc collaboration, typically reactive to incidents or specific requests (no scheduled touchpoints)
+  3 = Regular collaboration through defined channels; scheduled touchpoints at least monthly with IR and threat intel teams
+  4 = Deep integration with joint planning sessions at least quarterly, shared OKRs/objectives, and integrated workflows (e.g., threat intel feeds directly inform detection priorities)
+  5 = Seamless cross-functional collaboration with automated information sharing, shared metrics dashboards, and embedded team members</t>
+        </is>
+      </c>
+      <c r="F57" s="13" t="n"/>
+      <c r="G57" s="14">
+        <f>IF(F57="","",F57)</f>
+        <v/>
+      </c>
+      <c r="H57" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A50:H50"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A53:H53"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="A35:H35"/>
     <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A28:H28"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A47:H47"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C6:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G10:G72">
+  <conditionalFormatting sqref="G10:G57">
     <cfRule type="cellIs" priority="1" operator="between" dxfId="0">
       <formula>1</formula>
       <formula>1.49</formula>
@@ -3277,10 +2830,10 @@
     <dataValidation sqref="C7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select Self-Assessment or Audit" type="list">
       <formula1>"Self-Assessment,Audit"</formula1>
     </dataValidation>
-    <dataValidation sqref="F11 F12 F14 F16 F18 F24 F25 F31 F34 F37 F40 F43 F46 F51 F55 F59 F61 F63 F67 F68 F72" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select Yes or No" promptTitle="Answer" prompt="Select Yes or No" type="list">
+    <dataValidation sqref="F12 F16 F17 F23 F24 F32 F33 F43 F44 F51 F52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select Yes or No" promptTitle="Answer" prompt="Select Yes or No" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="F13 F15 F17 F19 F22 F23 F26 F27 F29 F30 F32 F35 F38 F41 F44 F47 F48 F52 F54 F58 F60 F62 F66 F69 F71" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select a value from 1 to 5" promptTitle="Maturity Rating" prompt="Select 1 (Initial) through 5 (Optimized)" type="list">
+    <dataValidation sqref="F11 F13 F14 F15 F19 F20 F21 F22 F25 F26 F27 F29 F30 F31 F34 F36 F37 F38 F39 F40 F42 F45 F46 F48 F49 F50 F54 F55 F56 F57" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select a value from 1 to 5" promptTitle="Maturity Rating" prompt="Select 1 (Initial) through 5 (Optimized)" type="list">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3443,7 +2996,7 @@
         </is>
       </c>
       <c r="C13" s="29">
-        <f>IF(COUNT(Assessment!G11,Assessment!G12,Assessment!G13)=0,"",AVERAGE(Assessment!G11,Assessment!G12,Assessment!G13))</f>
+        <f>IF(COUNT(Assessment!G11,Assessment!G12)=0,"",AVERAGE(Assessment!G11,Assessment!G12))</f>
         <v/>
       </c>
       <c r="D13" s="30">
@@ -3462,7 +3015,7 @@
         </is>
       </c>
       <c r="C14" s="29">
-        <f>IF(COUNT(Assessment!G14,Assessment!G15)=0,"",AVERAGE(Assessment!G14,Assessment!G15))</f>
+        <f>IF(COUNT(Assessment!G13)=0,"",AVERAGE(Assessment!G13))</f>
         <v/>
       </c>
       <c r="D14" s="30">
@@ -3481,7 +3034,7 @@
         </is>
       </c>
       <c r="C15" s="29">
-        <f>IF(COUNT(Assessment!G16,Assessment!G17)=0,"",AVERAGE(Assessment!G16,Assessment!G17))</f>
+        <f>IF(COUNT(Assessment!G14)=0,"",AVERAGE(Assessment!G14))</f>
         <v/>
       </c>
       <c r="D15" s="30">
@@ -3500,7 +3053,7 @@
         </is>
       </c>
       <c r="C16" s="29">
-        <f>IF(COUNT(Assessment!G18,Assessment!G19)=0,"",AVERAGE(Assessment!G18,Assessment!G19))</f>
+        <f>IF(COUNT(Assessment!G15,Assessment!G16,Assessment!G17)=0,"",AVERAGE(Assessment!G15,Assessment!G16,Assessment!G17))</f>
         <v/>
       </c>
       <c r="D16" s="30">
@@ -3535,7 +3088,7 @@
         </is>
       </c>
       <c r="C18" s="29">
-        <f>IF(COUNT(Assessment!G22,Assessment!G23)=0,"",AVERAGE(Assessment!G22,Assessment!G23))</f>
+        <f>IF(COUNT(Assessment!G19,Assessment!G20)=0,"",AVERAGE(Assessment!G19,Assessment!G20))</f>
         <v/>
       </c>
       <c r="D18" s="30">
@@ -3554,7 +3107,7 @@
         </is>
       </c>
       <c r="C19" s="29">
-        <f>IF(COUNT(Assessment!G24,Assessment!G25,Assessment!G26)=0,"",AVERAGE(Assessment!G24,Assessment!G25,Assessment!G26))</f>
+        <f>IF(COUNT(Assessment!G21)=0,"",AVERAGE(Assessment!G21))</f>
         <v/>
       </c>
       <c r="D19" s="30">
@@ -3573,7 +3126,7 @@
         </is>
       </c>
       <c r="C20" s="29">
-        <f>IF(COUNT(Assessment!G27)=0,"",AVERAGE(Assessment!G27))</f>
+        <f>IF(COUNT(Assessment!G22,Assessment!G23,Assessment!G24)=0,"",AVERAGE(Assessment!G22,Assessment!G23,Assessment!G24))</f>
         <v/>
       </c>
       <c r="D20" s="30">
@@ -3592,7 +3145,7 @@
         </is>
       </c>
       <c r="C21" s="29">
-        <f>IF(COUNT(Assessment!G29)=0,"",AVERAGE(Assessment!G29))</f>
+        <f>IF(COUNT(Assessment!G25)=0,"",AVERAGE(Assessment!G25))</f>
         <v/>
       </c>
       <c r="D21" s="30">
@@ -3611,7 +3164,7 @@
         </is>
       </c>
       <c r="C22" s="29">
-        <f>IF(COUNT(Assessment!G30)=0,"",AVERAGE(Assessment!G30))</f>
+        <f>IF(COUNT(Assessment!G26)=0,"",AVERAGE(Assessment!G26))</f>
         <v/>
       </c>
       <c r="D22" s="30">
@@ -3630,7 +3183,7 @@
         </is>
       </c>
       <c r="C23" s="29">
-        <f>IF(COUNT(Assessment!G31,Assessment!G32)=0,"",AVERAGE(Assessment!G31,Assessment!G32))</f>
+        <f>IF(COUNT(Assessment!G27)=0,"",AVERAGE(Assessment!G27))</f>
         <v/>
       </c>
       <c r="D23" s="30">
@@ -3665,7 +3218,7 @@
         </is>
       </c>
       <c r="C25" s="29">
-        <f>IF(COUNT(Assessment!G34,Assessment!G35)=0,"",AVERAGE(Assessment!G34,Assessment!G35))</f>
+        <f>IF(COUNT(Assessment!G29,Assessment!G30)=0,"",AVERAGE(Assessment!G29,Assessment!G30))</f>
         <v/>
       </c>
       <c r="D25" s="30">
@@ -3684,7 +3237,7 @@
         </is>
       </c>
       <c r="C26" s="29">
-        <f>IF(COUNT(Assessment!G37,Assessment!G38)=0,"",AVERAGE(Assessment!G37,Assessment!G38))</f>
+        <f>IF(COUNT(Assessment!G31,Assessment!G32,Assessment!G33)=0,"",AVERAGE(Assessment!G31,Assessment!G32,Assessment!G33))</f>
         <v/>
       </c>
       <c r="D26" s="30">
@@ -3703,7 +3256,7 @@
         </is>
       </c>
       <c r="C27" s="29">
-        <f>IF(COUNT(Assessment!G40,Assessment!G41)=0,"",AVERAGE(Assessment!G40,Assessment!G41))</f>
+        <f>IF(COUNT(Assessment!G34)=0,"",AVERAGE(Assessment!G34))</f>
         <v/>
       </c>
       <c r="D27" s="30">
@@ -3738,7 +3291,7 @@
         </is>
       </c>
       <c r="C29" s="29">
-        <f>IF(COUNT(Assessment!G43,Assessment!G44)=0,"",AVERAGE(Assessment!G43,Assessment!G44))</f>
+        <f>IF(COUNT(Assessment!G36,Assessment!G37)=0,"",AVERAGE(Assessment!G36,Assessment!G37))</f>
         <v/>
       </c>
       <c r="D29" s="30">
@@ -3757,7 +3310,7 @@
         </is>
       </c>
       <c r="C30" s="29">
-        <f>IF(COUNT(Assessment!G46,Assessment!G47)=0,"",AVERAGE(Assessment!G46,Assessment!G47))</f>
+        <f>IF(COUNT(Assessment!G38)=0,"",AVERAGE(Assessment!G38))</f>
         <v/>
       </c>
       <c r="D30" s="30">
@@ -3776,7 +3329,7 @@
         </is>
       </c>
       <c r="C31" s="29">
-        <f>IF(COUNT(Assessment!G48)=0,"",AVERAGE(Assessment!G48))</f>
+        <f>IF(COUNT(Assessment!G39,Assessment!G40)=0,"",AVERAGE(Assessment!G39,Assessment!G40))</f>
         <v/>
       </c>
       <c r="D31" s="30">
@@ -3811,7 +3364,7 @@
         </is>
       </c>
       <c r="C33" s="29">
-        <f>IF(COUNT(Assessment!G51,Assessment!G52)=0,"",AVERAGE(Assessment!G51,Assessment!G52))</f>
+        <f>IF(COUNT(Assessment!G42,Assessment!G43,Assessment!G44)=0,"",AVERAGE(Assessment!G42,Assessment!G43,Assessment!G44))</f>
         <v/>
       </c>
       <c r="D33" s="30">
@@ -3830,7 +3383,7 @@
         </is>
       </c>
       <c r="C34" s="29">
-        <f>IF(COUNT(Assessment!G54,Assessment!G55)=0,"",AVERAGE(Assessment!G54,Assessment!G55))</f>
+        <f>IF(COUNT(Assessment!G45,Assessment!G46)=0,"",AVERAGE(Assessment!G45,Assessment!G46))</f>
         <v/>
       </c>
       <c r="D34" s="30">
@@ -3865,7 +3418,7 @@
         </is>
       </c>
       <c r="C36" s="29">
-        <f>IF(COUNT(Assessment!G58,Assessment!G59)=0,"",AVERAGE(Assessment!G58,Assessment!G59))</f>
+        <f>IF(COUNT(Assessment!G48)=0,"",AVERAGE(Assessment!G48))</f>
         <v/>
       </c>
       <c r="D36" s="30">
@@ -3884,7 +3437,7 @@
         </is>
       </c>
       <c r="C37" s="29">
-        <f>IF(COUNT(Assessment!G60,Assessment!G61)=0,"",AVERAGE(Assessment!G60,Assessment!G61))</f>
+        <f>IF(COUNT(Assessment!G49)=0,"",AVERAGE(Assessment!G49))</f>
         <v/>
       </c>
       <c r="D37" s="30">
@@ -3903,7 +3456,7 @@
         </is>
       </c>
       <c r="C38" s="29">
-        <f>IF(COUNT(Assessment!G62,Assessment!G63)=0,"",AVERAGE(Assessment!G62,Assessment!G63))</f>
+        <f>IF(COUNT(Assessment!G50,Assessment!G51,Assessment!G52)=0,"",AVERAGE(Assessment!G50,Assessment!G51,Assessment!G52))</f>
         <v/>
       </c>
       <c r="D38" s="30">
@@ -3938,7 +3491,7 @@
         </is>
       </c>
       <c r="C40" s="29">
-        <f>IF(COUNT(Assessment!G66,Assessment!G67)=0,"",AVERAGE(Assessment!G66,Assessment!G67))</f>
+        <f>IF(COUNT(Assessment!G54)=0,"",AVERAGE(Assessment!G54))</f>
         <v/>
       </c>
       <c r="D40" s="30">
@@ -3957,7 +3510,7 @@
         </is>
       </c>
       <c r="C41" s="29">
-        <f>IF(COUNT(Assessment!G68,Assessment!G69)=0,"",AVERAGE(Assessment!G68,Assessment!G69))</f>
+        <f>IF(COUNT(Assessment!G55,Assessment!G56)=0,"",AVERAGE(Assessment!G55,Assessment!G56))</f>
         <v/>
       </c>
       <c r="D41" s="30">
@@ -3976,7 +3529,7 @@
         </is>
       </c>
       <c r="C42" s="29">
-        <f>IF(COUNT(Assessment!G71,Assessment!G72)=0,"",AVERAGE(Assessment!G71,Assessment!G72))</f>
+        <f>IF(COUNT(Assessment!G57)=0,"",AVERAGE(Assessment!G57))</f>
         <v/>
       </c>
       <c r="D42" s="30">
@@ -4782,7 +4335,7 @@
       </c>
       <c r="D43" s="12" t="inlineStr">
         <is>
-          <t>30-60 baseline rules; 40-60% ATT&amp;CK technique coverage.</t>
+          <t>30-60 baseline rules; 30-50% ATT&amp;CK technique coverage with documented gaps.</t>
         </is>
       </c>
     </row>
@@ -4800,7 +4353,7 @@
       </c>
       <c r="D44" s="18" t="inlineStr">
         <is>
-          <t>60-100 baseline rules; 60-80% ATT&amp;CK technique coverage.</t>
+          <t>60-100 baseline rules; 50-70% ATT&amp;CK technique coverage including behavioral detections; gaps tracked against threat model.</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4371,7 @@
       </c>
       <c r="D45" s="12" t="inlineStr">
         <is>
-          <t>100+ baseline rules; &gt;80% ATT&amp;CK technique coverage; continuous refinement.</t>
+          <t>100+ baseline rules; &gt;70% ATT&amp;CK technique coverage; continuous gap analysis and automated coverage tracking.</t>
         </is>
       </c>
     </row>
@@ -5802,12 +5355,12 @@
       </c>
       <c r="C109" s="12" t="inlineStr">
         <is>
-          <t>Regular testing program with attack emulation covering major detection categories. Results are documented and tracked.</t>
+          <t>Regular testing program with attack emulation (e.g., Atomic Red Team, Caldera) covering major detection categories. Results documented and tracked.</t>
         </is>
       </c>
       <c r="D109" s="12" t="inlineStr">
         <is>
-          <t>40-60% emulation coverage; quarterly testing cycles.</t>
+          <t>40-70% emulation coverage; at least quarterly testing cycles.</t>
         </is>
       </c>
     </row>
@@ -5825,7 +5378,7 @@
       </c>
       <c r="D110" s="18" t="inlineStr">
         <is>
-          <t>60-80% automated emulation coverage; regular purple team exercises.</t>
+          <t>70-90% automated emulation coverage; regular purple team exercises.</t>
         </is>
       </c>
     </row>
@@ -5838,12 +5391,12 @@
       </c>
       <c r="C111" s="12" t="inlineStr">
         <is>
-          <t>Continuous automated testing with real-time validation. Full emulation coverage with automated regression testing.</t>
+          <t>Continuous automated testing with real-time validation. Full emulation coverage with automated regression testing on every rule change.</t>
         </is>
       </c>
       <c r="D111" s="12" t="inlineStr">
         <is>
-          <t>&gt;80% automated coverage; continuous validation; automated regression.</t>
+          <t>&gt;90% automated coverage; continuous validation; automated regression on every change.</t>
         </is>
       </c>
     </row>
@@ -5945,12 +5498,12 @@
       </c>
       <c r="C119" s="12" t="inlineStr">
         <is>
-          <t>Systematic false negative identification through regular testing and validation exercises. Root causes are analyzed.</t>
+          <t>Systematic false negative identification through regular testing and validation exercises. Root causes are analyzed and documented.</t>
         </is>
       </c>
       <c r="D119" s="12" t="inlineStr">
         <is>
-          <t>70-90% of tested samples trigger alerts; root cause analysis documented.</t>
+          <t>70-90% of tested samples trigger alerts; root cause analysis documented; 30-50% FN reduction from baseline.</t>
         </is>
       </c>
     </row>
@@ -5968,7 +5521,7 @@
       </c>
       <c r="D120" s="18" t="inlineStr">
         <is>
-          <t>90-100% of tested samples trigger alerts; automated validation.</t>
+          <t>90-100% of tested samples trigger alerts; automated validation; &gt;50% FN reduction.</t>
         </is>
       </c>
     </row>
@@ -5986,7 +5539,7 @@
       </c>
       <c r="D121" s="12" t="inlineStr">
         <is>
-          <t>Continuous validation; near-zero FN rate on tested scenarios.</t>
+          <t>Continuous validation; near-zero FN rate on tested scenarios; &gt;75% FN reduction.</t>
         </is>
       </c>
     </row>
@@ -6466,12 +6019,12 @@
       </c>
       <c r="C153" s="12" t="inlineStr">
         <is>
-          <t>Significant automation of rule lifecycle tasks including testing, deployment, and basic tuning. Continuous improvement processes defined.</t>
+          <t>Significant automation of rule lifecycle tasks including testing, deployment, and basic tuning. AI-based quality checks on new rules. Continuous improvement processes defined.</t>
         </is>
       </c>
       <c r="D153" s="12" t="inlineStr">
         <is>
-          <t>40-60% of tasks automated; improvement metrics tracked.</t>
+          <t>40-60% of tasks automated; AI quality checks on new rules; improvement metrics tracked.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Hide chart data columns and add dynamic tier explanation
- Hide columns M-P on dashboard so chart data isn't visible
- Add formula-driven tier explanation below score cards that provides
  a 2-5 sentence description of the achieved tier, including what it
  means and what to focus on to advance to the next level

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -22,7 +22,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,6 +117,12 @@
       <b val="1"/>
       <color rgb="001B2A4A"/>
       <sz val="16"/>
+    </font>
+    <font>
+      <name val="Aptos"/>
+      <i val="1"/>
+      <color rgb="00475569"/>
+      <sz val="10.5"/>
     </font>
     <font>
       <name val="Aptos"/>
@@ -380,8 +386,8 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -413,31 +419,31 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -3140,10 +3146,10 @@
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="3" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="13" max="13"/>
-    <col width="10" customWidth="1" min="14" max="14"/>
-    <col width="18" customWidth="1" min="15" max="15"/>
-    <col width="10" customWidth="1" min="16" max="16"/>
+    <col hidden="1" width="18" customWidth="1" min="13" max="13"/>
+    <col hidden="1" width="10" customWidth="1" min="14" max="14"/>
+    <col hidden="1" width="18" customWidth="1" min="15" max="15"/>
+    <col hidden="1" width="10" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="56" customHeight="1">
@@ -3296,11 +3302,10 @@
         <v/>
       </c>
     </row>
-    <row r="8" ht="22" customHeight="1">
-      <c r="B8" s="46" t="inlineStr">
-        <is>
-          <t>Your achieved tier is the highest tier where all criteria in that tier and all lower tiers score ≥ 3.0 (Defined level).</t>
-        </is>
+    <row r="8" ht="62" customHeight="1">
+      <c r="B8" s="46">
+        <f>IF(D6="","",IF(D6="Tier 4: Expert","Your organization has achieved Tier 4 (Expert)—the highest DEBMM tier. Your detection engineering program is mature across all dimensions: proactive threat hunting, automation of key lifecycle stages, and continuous improvement driven by data. Focus on sustaining this level and contributing to the broader detection engineering community.",IF(D6="Tier 3: Advanced","Your organization has achieved Tier 3 (Advanced). You have a highly capable detection program with systematic FN reduction, external validation, and behavioral detection of advanced TTPs. To reach Tier 4, develop proactive threat hunting capabilities, adopt hypothesis-driven hunting workflows, and integrate automation and AI across the detection lifecycle.",IF(D6="Tier 2: Intermediate","Your organization has achieved Tier 2 (Intermediate). Your detection program has mature processes for rule development, telemetry management, false positive reduction, and gap analysis. To advance to Tier 3, invest in false negative triage, external validation (e.g., purple team exercises), and coverage of advanced TTPs.",IF(D6="Tier 1: Basic","Your organization has achieved Tier 1 (Basic). You have solid foundations and basic detection capabilities in place, including baseline rules, telemetry coverage, and release testing at the Defined level. To advance to Tier 2, focus on systematic false positive reduction, formal gap analysis, and internal testing and validation.",IF(D6="Tier 0: Foundation","Your organization has achieved Tier 0 (Foundation). All foundational criteria meet the Defined level, meaning you have documented processes for rule development, maintenance, roadmaps, and threat modeling. To reach Tier 1, ensure your baseline rules, telemetry quality, threat landscape reviews, and release testing also reach the Defined level.","Your organization has not yet achieved Tier 0 (Foundation). This means one or more foundational criteria—such as structured rule development, rule maintenance, roadmap documentation, or threat modeling—score below the Defined level (3.0). Focus on establishing basic, repeatable processes in these areas before advancing to higher tiers."))))))</f>
+        <v/>
       </c>
       <c r="C8" s="28" t="n"/>
       <c r="D8" s="28" t="n"/>

</xml_diff>

<commit_message>
Add Report Data tab for Power BI consumption
New fifth sheet with three flat tables optimized for Power BI import:
- Summary: org, assessor, date, overall score, achieved tier, completion
- Tier Progression: T0-T4 with score, level, status, and progression
  (Complete/Current/In Progress/Not Started) for tier roadmap visuals
- Criterion Breakdown: section (DEBMM Core vs Enrichment), category,
  criterion name, score, level, pass/fail for every criterion

All values are formula-driven from the Assessment tab and update
automatically as answers change.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Assessment" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Results Dashboard" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Rubric Reference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Report Data" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -269,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -451,6 +452,30 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7012,4 +7037,1074 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="002D3E50"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="34" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="68" t="inlineStr">
+        <is>
+          <t>SUMMARY</t>
+        </is>
+      </c>
+      <c r="B1" s="68" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="69" t="inlineStr">
+        <is>
+          <t>Organization</t>
+        </is>
+      </c>
+      <c r="B2" s="50">
+        <f>Assessment!D4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="69" t="inlineStr">
+        <is>
+          <t>Assessor</t>
+        </is>
+      </c>
+      <c r="B3" s="50">
+        <f>Assessment!D5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="69" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B4" s="50">
+        <f>Assessment!D7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="69" t="inlineStr">
+        <is>
+          <t>Assessment Type</t>
+        </is>
+      </c>
+      <c r="B5" s="50">
+        <f>Assessment!D8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="69" t="inlineStr">
+        <is>
+          <t>Overall Score</t>
+        </is>
+      </c>
+      <c r="B6" s="70">
+        <f>IF(COUNT(D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41)=0,"",ROUND(AVERAGE(D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41),2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="69" t="inlineStr">
+        <is>
+          <t>Achieved Tier</t>
+        </is>
+      </c>
+      <c r="B7" s="50">
+        <f>IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3,C15&gt;=3),"Tier 4: Expert",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Tier 3: Advanced",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Tier 2: Intermediate",IF(AND(C11&gt;=3,C12&gt;=3),"Tier 1: Basic",IF(AND(C11&gt;=3),"Tier 0: Foundation","Below Foundation")))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="69" t="inlineStr">
+        <is>
+          <t>Completion</t>
+        </is>
+      </c>
+      <c r="B8" s="50">
+        <f>COUNTA(Assessment!E15:E71)&amp;" / 41"</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="71" t="inlineStr">
+        <is>
+          <t>Tier</t>
+        </is>
+      </c>
+      <c r="B10" s="71" t="inlineStr">
+        <is>
+          <t>Tier Name</t>
+        </is>
+      </c>
+      <c r="C10" s="71" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="D10" s="71" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="E10" s="71" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="F10" s="71" t="inlineStr">
+        <is>
+          <t>Progression</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="72" t="inlineStr">
+        <is>
+          <t>T0</t>
+        </is>
+      </c>
+      <c r="B11" s="73" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C11" s="74">
+        <f>IF(COUNT(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <v/>
+      </c>
+      <c r="D11" s="75">
+        <f>IF(C11="","",IF(C11&gt;=4.5,"Optimized",IF(C11&gt;=3.5,"Managed",IF(C11&gt;=2.5,"Defined",IF(C11&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="E11" s="75">
+        <f>IF(C11="","",IF(C11&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+      <c r="F11" s="72">
+        <f>IF(C11="","Not Started",IF(AND(C11&gt;=3),"Complete",IF(TRUE,"Current","In Progress")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="72" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B12" s="73" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C12" s="74">
+        <f>IF(COUNT(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32)=0,"",AVERAGE(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32))</f>
+        <v/>
+      </c>
+      <c r="D12" s="75">
+        <f>IF(C12="","",IF(C12&gt;=4.5,"Optimized",IF(C12&gt;=3.5,"Managed",IF(C12&gt;=2.5,"Defined",IF(C12&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="E12" s="75">
+        <f>IF(C12="","",IF(C12&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+      <c r="F12" s="72">
+        <f>IF(C12="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3),"Complete",IF(AND(C11&gt;=3),"Current","In Progress")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="72" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B13" s="73" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C13" s="74">
+        <f>IF(COUNT(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40)=0,"",AVERAGE(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40))</f>
+        <v/>
+      </c>
+      <c r="D13" s="75">
+        <f>IF(C13="","",IF(C13&gt;=4.5,"Optimized",IF(C13&gt;=3.5,"Managed",IF(C13&gt;=2.5,"Defined",IF(C13&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="E13" s="75">
+        <f>IF(C13="","",IF(C13&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+      <c r="F13" s="72">
+        <f>IF(C13="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3),"Current","In Progress")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="72" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="B14" s="73" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C14" s="74">
+        <f>IF(COUNT(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47))</f>
+        <v/>
+      </c>
+      <c r="D14" s="75">
+        <f>IF(C14="","",IF(C14&gt;=4.5,"Optimized",IF(C14&gt;=3.5,"Managed",IF(C14&gt;=2.5,"Defined",IF(C14&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="E14" s="75">
+        <f>IF(C14="","",IF(C14&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+      <c r="F14" s="72">
+        <f>IF(C14="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Current","In Progress")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="72" t="inlineStr">
+        <is>
+          <t>T4</t>
+        </is>
+      </c>
+      <c r="B15" s="73" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="C15" s="74">
+        <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54))</f>
+        <v/>
+      </c>
+      <c r="D15" s="75">
+        <f>IF(C15="","",IF(C15&gt;=4.5,"Optimized",IF(C15&gt;=3.5,"Managed",IF(C15&gt;=2.5,"Defined",IF(C15&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="E15" s="75">
+        <f>IF(C15="","",IF(C15&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+      <c r="F15" s="72">
+        <f>IF(C15="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3,C15&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Current","In Progress")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="14" t="inlineStr">
+        <is>
+          <t>Section</t>
+        </is>
+      </c>
+      <c r="B17" s="14" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C17" s="14" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="D17" s="14" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="E17" s="14" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="F17" s="14" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B18" s="50" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C18" s="69" t="inlineStr">
+        <is>
+          <t>Structured Rule Development Approach</t>
+        </is>
+      </c>
+      <c r="D18" s="51">
+        <f>IF(COUNT(Assessment!F15,Assessment!F16)=0,"",AVERAGE(Assessment!F15,Assessment!F16))</f>
+        <v/>
+      </c>
+      <c r="E18" s="52">
+        <f>IF(D18="","",IF(D18&gt;=4.5,"Optimized",IF(D18&gt;=3.5,"Managed",IF(D18&gt;=2.5,"Defined",IF(D18&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F18" s="52">
+        <f>IF(D18="","",IF(D18&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B19" s="50" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C19" s="69" t="inlineStr">
+        <is>
+          <t>Rule Creation and Maintenance</t>
+        </is>
+      </c>
+      <c r="D19" s="51">
+        <f>IF(COUNT(Assessment!F17)=0,"",AVERAGE(Assessment!F17))</f>
+        <v/>
+      </c>
+      <c r="E19" s="52">
+        <f>IF(D19="","",IF(D19&gt;=4.5,"Optimized",IF(D19&gt;=3.5,"Managed",IF(D19&gt;=2.5,"Defined",IF(D19&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F19" s="52">
+        <f>IF(D19="","",IF(D19&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B20" s="50" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C20" s="69" t="inlineStr">
+        <is>
+          <t>Roadmap Documentation</t>
+        </is>
+      </c>
+      <c r="D20" s="51">
+        <f>IF(COUNT(Assessment!F18)=0,"",AVERAGE(Assessment!F18))</f>
+        <v/>
+      </c>
+      <c r="E20" s="52">
+        <f>IF(D20="","",IF(D20&gt;=4.5,"Optimized",IF(D20&gt;=3.5,"Managed",IF(D20&gt;=2.5,"Defined",IF(D20&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F20" s="52">
+        <f>IF(D20="","",IF(D20&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B21" s="50" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C21" s="69" t="inlineStr">
+        <is>
+          <t>Threat Modeling</t>
+        </is>
+      </c>
+      <c r="D21" s="51">
+        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <v/>
+      </c>
+      <c r="E21" s="52">
+        <f>IF(D21="","",IF(D21&gt;=4.5,"Optimized",IF(D21&gt;=3.5,"Managed",IF(D21&gt;=2.5,"Defined",IF(D21&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F21" s="52">
+        <f>IF(D21="","",IF(D21&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B22" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C22" s="69" t="inlineStr">
+        <is>
+          <t>Baseline Rule Creation</t>
+        </is>
+      </c>
+      <c r="D22" s="51">
+        <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
+        <v/>
+      </c>
+      <c r="E22" s="52">
+        <f>IF(D22="","",IF(D22&gt;=4.5,"Optimized",IF(D22&gt;=3.5,"Managed",IF(D22&gt;=2.5,"Defined",IF(D22&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F22" s="52">
+        <f>IF(D22="","",IF(D22&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B23" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C23" s="69" t="inlineStr">
+        <is>
+          <t>Ruleset Management and Maintenance</t>
+        </is>
+      </c>
+      <c r="D23" s="51">
+        <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
+        <v/>
+      </c>
+      <c r="E23" s="52">
+        <f>IF(D23="","",IF(D23&gt;=4.5,"Optimized",IF(D23&gt;=3.5,"Managed",IF(D23&gt;=2.5,"Defined",IF(D23&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F23" s="52">
+        <f>IF(D23="","",IF(D23&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B24" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C24" s="69" t="inlineStr">
+        <is>
+          <t>Telemetry Quality</t>
+        </is>
+      </c>
+      <c r="D24" s="51">
+        <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
+        <v/>
+      </c>
+      <c r="E24" s="52">
+        <f>IF(D24="","",IF(D24&gt;=4.5,"Optimized",IF(D24&gt;=3.5,"Managed",IF(D24&gt;=2.5,"Defined",IF(D24&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F24" s="52">
+        <f>IF(D24="","",IF(D24&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B25" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C25" s="69" t="inlineStr">
+        <is>
+          <t>Threat Landscape Review</t>
+        </is>
+      </c>
+      <c r="D25" s="51">
+        <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
+        <v/>
+      </c>
+      <c r="E25" s="52">
+        <f>IF(D25="","",IF(D25&gt;=4.5,"Optimized",IF(D25&gt;=3.5,"Managed",IF(D25&gt;=2.5,"Defined",IF(D25&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F25" s="52">
+        <f>IF(D25="","",IF(D25&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B26" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C26" s="69" t="inlineStr">
+        <is>
+          <t>Product Owner Engagement</t>
+        </is>
+      </c>
+      <c r="D26" s="51">
+        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
+        <v/>
+      </c>
+      <c r="E26" s="52">
+        <f>IF(D26="","",IF(D26&gt;=4.5,"Optimized",IF(D26&gt;=3.5,"Managed",IF(D26&gt;=2.5,"Defined",IF(D26&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F26" s="52">
+        <f>IF(D26="","",IF(D26&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B27" s="50" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C27" s="69" t="inlineStr">
+        <is>
+          <t>Release Testing and Validation</t>
+        </is>
+      </c>
+      <c r="D27" s="51">
+        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
+        <v/>
+      </c>
+      <c r="E27" s="52">
+        <f>IF(D27="","",IF(D27&gt;=4.5,"Optimized",IF(D27&gt;=3.5,"Managed",IF(D27&gt;=2.5,"Defined",IF(D27&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F27" s="52">
+        <f>IF(D27="","",IF(D27&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B28" s="50" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C28" s="69" t="inlineStr">
+        <is>
+          <t>False Positive Tuning and Reduction</t>
+        </is>
+      </c>
+      <c r="D28" s="51">
+        <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
+        <v/>
+      </c>
+      <c r="E28" s="52">
+        <f>IF(D28="","",IF(D28&gt;=4.5,"Optimized",IF(D28&gt;=3.5,"Managed",IF(D28&gt;=2.5,"Defined",IF(D28&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F28" s="52">
+        <f>IF(D28="","",IF(D28&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B29" s="50" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C29" s="69" t="inlineStr">
+        <is>
+          <t>Gap Analysis and Documentation</t>
+        </is>
+      </c>
+      <c r="D29" s="51">
+        <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
+        <v/>
+      </c>
+      <c r="E29" s="52">
+        <f>IF(D29="","",IF(D29&gt;=4.5,"Optimized",IF(D29&gt;=3.5,"Managed",IF(D29&gt;=2.5,"Defined",IF(D29&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F29" s="52">
+        <f>IF(D29="","",IF(D29&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B30" s="50" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C30" s="69" t="inlineStr">
+        <is>
+          <t>Internal Testing and Validation</t>
+        </is>
+      </c>
+      <c r="D30" s="51">
+        <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
+        <v/>
+      </c>
+      <c r="E30" s="52">
+        <f>IF(D30="","",IF(D30&gt;=4.5,"Optimized",IF(D30&gt;=3.5,"Managed",IF(D30&gt;=2.5,"Defined",IF(D30&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F30" s="52">
+        <f>IF(D30="","",IF(D30&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B31" s="50" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C31" s="69" t="inlineStr">
+        <is>
+          <t>False Negative Triage</t>
+        </is>
+      </c>
+      <c r="D31" s="51">
+        <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
+        <v/>
+      </c>
+      <c r="E31" s="52">
+        <f>IF(D31="","",IF(D31&gt;=4.5,"Optimized",IF(D31&gt;=3.5,"Managed",IF(D31&gt;=2.5,"Defined",IF(D31&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F31" s="52">
+        <f>IF(D31="","",IF(D31&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B32" s="50" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C32" s="69" t="inlineStr">
+        <is>
+          <t>External Validation</t>
+        </is>
+      </c>
+      <c r="D32" s="51">
+        <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
+        <v/>
+      </c>
+      <c r="E32" s="52">
+        <f>IF(D32="","",IF(D32&gt;=4.5,"Optimized",IF(D32&gt;=3.5,"Managed",IF(D32&gt;=2.5,"Defined",IF(D32&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F32" s="52">
+        <f>IF(D32="","",IF(D32&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B33" s="50" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C33" s="69" t="inlineStr">
+        <is>
+          <t>Advanced TTP Coverage</t>
+        </is>
+      </c>
+      <c r="D33" s="51">
+        <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
+        <v/>
+      </c>
+      <c r="E33" s="52">
+        <f>IF(D33="","",IF(D33&gt;=4.5,"Optimized",IF(D33&gt;=3.5,"Managed",IF(D33&gt;=2.5,"Defined",IF(D33&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F33" s="52">
+        <f>IF(D33="","",IF(D33&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B34" s="50" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="C34" s="69" t="inlineStr">
+        <is>
+          <t>Threat Hunting in Telemetry</t>
+        </is>
+      </c>
+      <c r="D34" s="51">
+        <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52))</f>
+        <v/>
+      </c>
+      <c r="E34" s="52">
+        <f>IF(D34="","",IF(D34&gt;=4.5,"Optimized",IF(D34&gt;=3.5,"Managed",IF(D34&gt;=2.5,"Defined",IF(D34&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F34" s="52">
+        <f>IF(D34="","",IF(D34&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="50" t="inlineStr">
+        <is>
+          <t>DEBMM Core</t>
+        </is>
+      </c>
+      <c r="B35" s="50" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="C35" s="69" t="inlineStr">
+        <is>
+          <t>Automation and Continuous Improvement</t>
+        </is>
+      </c>
+      <c r="D35" s="51">
+        <f>IF(COUNT(Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F53,Assessment!F54))</f>
+        <v/>
+      </c>
+      <c r="E35" s="52">
+        <f>IF(D35="","",IF(D35&gt;=4.5,"Optimized",IF(D35&gt;=3.5,"Managed",IF(D35&gt;=2.5,"Defined",IF(D35&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F35" s="52">
+        <f>IF(D35="","",IF(D35&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B36" s="50" t="inlineStr">
+        <is>
+          <t>People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="C36" s="69" t="inlineStr">
+        <is>
+          <t>Team Structure and Dedicated Roles</t>
+        </is>
+      </c>
+      <c r="D36" s="51">
+        <f>IF(COUNT(Assessment!F61)=0,"",AVERAGE(Assessment!F61))</f>
+        <v/>
+      </c>
+      <c r="E36" s="52">
+        <f>IF(D36="","",IF(D36&gt;=4.5,"Optimized",IF(D36&gt;=3.5,"Managed",IF(D36&gt;=2.5,"Defined",IF(D36&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F36" s="52">
+        <f>IF(D36="","",IF(D36&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B37" s="50" t="inlineStr">
+        <is>
+          <t>People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="C37" s="69" t="inlineStr">
+        <is>
+          <t>Skills Development and Training</t>
+        </is>
+      </c>
+      <c r="D37" s="51">
+        <f>IF(COUNT(Assessment!F62)=0,"",AVERAGE(Assessment!F62))</f>
+        <v/>
+      </c>
+      <c r="E37" s="52">
+        <f>IF(D37="","",IF(D37&gt;=4.5,"Optimized",IF(D37&gt;=3.5,"Managed",IF(D37&gt;=2.5,"Defined",IF(D37&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F37" s="52">
+        <f>IF(D37="","",IF(D37&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B38" s="50" t="inlineStr">
+        <is>
+          <t>People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="C38" s="69" t="inlineStr">
+        <is>
+          <t>Leadership Commitment and Executive Sponsorship</t>
+        </is>
+      </c>
+      <c r="D38" s="51">
+        <f>IF(COUNT(Assessment!F63,Assessment!F64,Assessment!F65)=0,"",AVERAGE(Assessment!F63,Assessment!F64,Assessment!F65))</f>
+        <v/>
+      </c>
+      <c r="E38" s="52">
+        <f>IF(D38="","",IF(D38&gt;=4.5,"Optimized",IF(D38&gt;=3.5,"Managed",IF(D38&gt;=2.5,"Defined",IF(D38&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F38" s="52">
+        <f>IF(D38="","",IF(D38&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B39" s="50" t="inlineStr">
+        <is>
+          <t>Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="C39" s="69" t="inlineStr">
+        <is>
+          <t>Detection Lifecycle Workflow</t>
+        </is>
+      </c>
+      <c r="D39" s="51">
+        <f>IF(COUNT(Assessment!F68)=0,"",AVERAGE(Assessment!F68))</f>
+        <v/>
+      </c>
+      <c r="E39" s="52">
+        <f>IF(D39="","",IF(D39&gt;=4.5,"Optimized",IF(D39&gt;=3.5,"Managed",IF(D39&gt;=2.5,"Defined",IF(D39&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F39" s="52">
+        <f>IF(D39="","",IF(D39&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B40" s="50" t="inlineStr">
+        <is>
+          <t>Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="C40" s="69" t="inlineStr">
+        <is>
+          <t>Metrics and KPI Tracking</t>
+        </is>
+      </c>
+      <c r="D40" s="51">
+        <f>IF(COUNT(Assessment!F69,Assessment!F70)=0,"",AVERAGE(Assessment!F69,Assessment!F70))</f>
+        <v/>
+      </c>
+      <c r="E40" s="52">
+        <f>IF(D40="","",IF(D40&gt;=4.5,"Optimized",IF(D40&gt;=3.5,"Managed",IF(D40&gt;=2.5,"Defined",IF(D40&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F40" s="52">
+        <f>IF(D40="","",IF(D40&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="50" t="inlineStr">
+        <is>
+          <t>Enrichment</t>
+        </is>
+      </c>
+      <c r="B41" s="50" t="inlineStr">
+        <is>
+          <t>Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="C41" s="69" t="inlineStr">
+        <is>
+          <t>Cross-Team Collaboration</t>
+        </is>
+      </c>
+      <c r="D41" s="51">
+        <f>IF(COUNT(Assessment!F71)=0,"",AVERAGE(Assessment!F71))</f>
+        <v/>
+      </c>
+      <c r="E41" s="52">
+        <f>IF(D41="","",IF(D41&gt;=4.5,"Optimized",IF(D41&gt;=3.5,"Managed",IF(D41&gt;=2.5,"Defined",IF(D41&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F41" s="52">
+        <f>IF(D41="","",IF(D41&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F11:F15">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="3">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="2">
+      <formula>"Current"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1">
+      <formula>"In Progress"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C15">
+    <cfRule type="cellIs" priority="4" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D41">
+    <cfRule type="cellIs" priority="8" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F41">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="3">
+      <formula>"✓ Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
+      <formula>"✗ Below Target"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix completion count and tier determination consistency bugs
- Fix 42/41 completion count: COUNTA range included non-question rows
  (enrichment column headers). Now uses explicit cell references targeting
  only actual question rows in both Dashboard and Report Data tabs.
- Fix Report Data tier formula: was checking tier averages instead of
  per-criterion scores, which could show a different tier than Dashboard.
  Now uses identical per-criterion >= 3.0 checks matching Dashboard logic.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -3303,7 +3303,7 @@
       </c>
       <c r="E6" s="44" t="n"/>
       <c r="F6" s="45">
-        <f>COUNTA(Assessment!E15:E71)&amp;" / 41"</f>
+        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
         <v/>
       </c>
       <c r="M6" t="inlineStr">
@@ -7134,7 +7134,7 @@
         </is>
       </c>
       <c r="B7" s="50">
-        <f>IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3,C15&gt;=3),"Tier 4: Expert",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Tier 3: Advanced",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Tier 2: Intermediate",IF(AND(C11&gt;=3,C12&gt;=3),"Tier 1: Basic",IF(AND(C11&gt;=3),"Tier 0: Foundation","Below Foundation")))))</f>
+        <f>IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3),AND(D34&gt;=3,D35&gt;=3)),"Tier 4: Expert",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Tier 3: Advanced",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Tier 1: Basic",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
         <v/>
       </c>
     </row>
@@ -7145,7 +7145,7 @@
         </is>
       </c>
       <c r="B8" s="50">
-        <f>COUNTA(Assessment!E15:E71)&amp;" / 41"</f>
+        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
         <v/>
       </c>
     </row>
@@ -7205,7 +7205,7 @@
         <v/>
       </c>
       <c r="F11" s="72">
-        <f>IF(C11="","Not Started",IF(AND(C11&gt;=3),"Complete",IF(TRUE,"Current","In Progress")))</f>
+        <f>IF(C11="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Complete",IF(TRUE,"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
         <v/>
       </c>
       <c r="F12" s="72">
-        <f>IF(C12="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3),"Complete",IF(AND(C11&gt;=3),"Current","In Progress")))</f>
+        <f>IF(C12="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7261,7 +7261,7 @@
         <v/>
       </c>
       <c r="F13" s="72">
-        <f>IF(C13="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3),"Current","In Progress")))</f>
+        <f>IF(C13="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7289,7 +7289,7 @@
         <v/>
       </c>
       <c r="F14" s="72">
-        <f>IF(C14="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3),"Current","In Progress")))</f>
+        <f>IF(C14="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7317,7 +7317,7 @@
         <v/>
       </c>
       <c r="F15" s="72">
-        <f>IF(C15="","Not Started",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3,C15&gt;=3),"Complete",IF(AND(C11&gt;=3,C12&gt;=3,C13&gt;=3,C14&gt;=3),"Current","In Progress")))</f>
+        <f>IF(C15="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3),AND(D34&gt;=3,D35&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix empty spreadsheet defaulting to Tier 4: Expert
Add ISNUMBER() guard to tier determination formulas on both Dashboard
and Report Data tabs. Excel treats "">=3 as TRUE (text > numbers),
so unfilled criterion cells falsely passed all tier checks.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -3298,7 +3298,7 @@
       </c>
       <c r="C6" s="44" t="n"/>
       <c r="D6" s="45">
-        <f>IF(AND(AND(D13&gt;=3,D14&gt;=3,D15&gt;=3,D16&gt;=3),AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3,D22&gt;=3,D23&gt;=3),AND(D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D29&gt;=3,D30&gt;=3,D31&gt;=3),AND(D33&gt;=3,D34&gt;=3)),"Tier 4: Expert",IF(AND(AND(D13&gt;=3,D14&gt;=3,D15&gt;=3,D16&gt;=3),AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3,D22&gt;=3,D23&gt;=3),AND(D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D29&gt;=3,D30&gt;=3,D31&gt;=3)),"Tier 3: Advanced",IF(AND(AND(D13&gt;=3,D14&gt;=3,D15&gt;=3,D16&gt;=3),AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3,D22&gt;=3,D23&gt;=3),AND(D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(D13&gt;=3,D14&gt;=3,D15&gt;=3,D16&gt;=3),AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3,D22&gt;=3,D23&gt;=3)),"Tier 1: Basic",IF(AND(AND(D13&gt;=3,D14&gt;=3,D15&gt;=3,D16&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
+        <f>IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3,ISNUMBER(D31),D31&gt;=3),AND(ISNUMBER(D33),D33&gt;=3,ISNUMBER(D34),D34&gt;=3)),"Tier 4: Expert",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3,ISNUMBER(D31),D31&gt;=3)),"Tier 3: Advanced",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3)),"Tier 1: Basic",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
         <v/>
       </c>
       <c r="E6" s="44" t="n"/>
@@ -7134,7 +7134,7 @@
         </is>
       </c>
       <c r="B7" s="50">
-        <f>IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3),AND(D34&gt;=3,D35&gt;=3)),"Tier 4: Expert",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Tier 3: Advanced",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Tier 1: Basic",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
+        <f>IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3),AND(ISNUMBER(D34),D34&gt;=3,ISNUMBER(D35),D35&gt;=3)),"Tier 4: Expert",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3)),"Tier 3: Advanced",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Tier 1: Basic",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
         <v/>
       </c>
     </row>
@@ -7205,7 +7205,7 @@
         <v/>
       </c>
       <c r="F11" s="72">
-        <f>IF(C11="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Complete",IF(TRUE,"Current","In Progress")))</f>
+        <f>IF(C11="","Not Started",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3)),"Complete",IF(TRUE,"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
         <v/>
       </c>
       <c r="F12" s="72">
-        <f>IF(C12="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3)),"Current","In Progress")))</f>
+        <f>IF(C12="","Not Started",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Complete",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7261,7 +7261,7 @@
         <v/>
       </c>
       <c r="F13" s="72">
-        <f>IF(C13="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3)),"Current","In Progress")))</f>
+        <f>IF(C13="","Not Started",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3)),"Complete",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7289,7 +7289,7 @@
         <v/>
       </c>
       <c r="F14" s="72">
-        <f>IF(C14="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3)),"Current","In Progress")))</f>
+        <f>IF(C14="","Not Started",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3)),"Complete",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>
@@ -7317,7 +7317,7 @@
         <v/>
       </c>
       <c r="F15" s="72">
-        <f>IF(C15="","Not Started",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3),AND(D34&gt;=3,D35&gt;=3)),"Complete",IF(AND(AND(D18&gt;=3,D19&gt;=3,D20&gt;=3,D21&gt;=3),AND(D22&gt;=3,D23&gt;=3,D24&gt;=3,D25&gt;=3,D26&gt;=3,D27&gt;=3),AND(D28&gt;=3,D29&gt;=3,D30&gt;=3),AND(D31&gt;=3,D32&gt;=3,D33&gt;=3)),"Current","In Progress")))</f>
+        <f>IF(C15="","Not Started",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3),AND(ISNUMBER(D34),D34&gt;=3,ISNUMBER(D35),D35&gt;=3)),"Complete",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3)),"Current","In Progress")))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Add PowerPoint report generator and clean up project structure
- Add scorer/extract_data.py: extracts assessment data from xlsx to JSON
- Add scorer/generate_report.js: generates 4-slide dark-themed PowerPoint
  report from JSON (title, tier overview, core breakdown, enrichment)
- Add package.json for pptxgenjs dependency
- Update README with accurate setup instructions, prerequisites,
  full pipeline documentation, and correct project structure
- Update .gitignore for node_modules, generated outputs, .claude/
- Add python-pptx to requirements.txt
- Remove temp/sample files from repo

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Assessment" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Results Dashboard" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Tier Scores Chart" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Readiness Chart" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Rubric Reference" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Report Data" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assessment" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results Dashboard" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tier Scores Chart" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Readiness Chart" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rubric Reference" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Report Data" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -588,14 +588,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -619,17 +619,17 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <dPt>
             <idx val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="3B82F6"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -637,10 +637,10 @@
           <dPt>
             <idx val="1"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="3B82F6"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -648,10 +648,10 @@
           <dPt>
             <idx val="2"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="3B82F6"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -659,10 +659,10 @@
           <dPt>
             <idx val="3"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="3B82F6"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -670,10 +670,10 @@
           <dPt>
             <idx val="4"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="3B82F6"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -716,8 +716,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -740,14 +740,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -771,17 +771,17 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <dPt>
             <idx val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="0D7377"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -789,10 +789,10 @@
           <dPt>
             <idx val="1"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:srgbClr val="0D7377"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -835,8 +835,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -859,7 +859,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>1</col>
@@ -874,9 +874,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -886,7 +886,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>1</col>
@@ -901,9 +901,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>

<commit_message>
Add 5 questions to close DEBMM example questionnaire gaps
Add checklist questions for: critical asset inventory (T0-Q8),
detection coverage map (T2-Q7), detection failure retrospectives
(T4-Q6), designated activity owners (EP-Q6), and incident lessons
learned process (EG-Q5). Updates questionnaire from 41 to 46
questions. Regenerated both spreadsheet templates.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment-audit.xlsx
+++ b/templates/debmm-assessment-audit.xlsx
@@ -1627,7 +1627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
@@ -1982,41 +1982,64 @@
       </c>
       <c r="G21" s="21" t="n"/>
     </row>
-    <row r="22" ht="34" customHeight="1">
-      <c r="B22" s="15" t="inlineStr">
+    <row r="22" ht="35" customHeight="1">
+      <c r="B22" s="22" t="inlineStr">
+        <is>
+          <t>T0-Q8</t>
+        </is>
+      </c>
+      <c r="C22" s="23" t="inlineStr">
+        <is>
+          <t>Threat Modeling</t>
+        </is>
+      </c>
+      <c r="D22" s="24" t="inlineStr">
+        <is>
+          <t>Does the assessed team maintain a documented inventory of critical assets mapped to detection coverage?</t>
+        </is>
+      </c>
+      <c r="E22" s="19" t="n"/>
+      <c r="F22" s="25">
+        <f>IF(E22="Yes",3,IF(E22="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G22" s="21" t="n"/>
+    </row>
+    <row r="23" ht="34" customHeight="1">
+      <c r="B23" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">  TIER 1: BASIC</t>
         </is>
       </c>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
-    </row>
-    <row r="23" ht="20" customHeight="1">
-      <c r="B23" s="13" t="inlineStr">
+      <c r="C23" s="4" t="n"/>
+      <c r="D23" s="4" t="n"/>
+      <c r="E23" s="4" t="n"/>
+      <c r="F23" s="4" t="n"/>
+      <c r="G23" s="4" t="n"/>
+    </row>
+    <row r="24" ht="20" customHeight="1">
+      <c r="B24" s="13" t="inlineStr">
         <is>
           <t>Establishes baseline detection capabilities with systematic management, version control, and initial alignment with the threat landscape.</t>
         </is>
       </c>
-      <c r="C23" s="6" t="n"/>
-      <c r="D23" s="6" t="n"/>
-      <c r="E23" s="6" t="n"/>
-      <c r="F23" s="6" t="n"/>
-    </row>
-    <row r="24" ht="115" customHeight="1">
-      <c r="B24" s="16" t="inlineStr">
+      <c r="C24" s="6" t="n"/>
+      <c r="D24" s="6" t="n"/>
+      <c r="E24" s="6" t="n"/>
+      <c r="F24" s="6" t="n"/>
+    </row>
+    <row r="25" ht="115" customHeight="1">
+      <c r="B25" s="16" t="inlineStr">
         <is>
           <t>T1-Q1</t>
         </is>
       </c>
-      <c r="C24" s="17" t="inlineStr">
+      <c r="C25" s="17" t="inlineStr">
         <is>
           <t>Baseline Rule Creation</t>
         </is>
       </c>
-      <c r="D24" s="18" t="inlineStr">
+      <c r="D25" s="18" t="inlineStr">
         <is>
           <t>How many custom detection rules does the assessed team maintain?
 1 — Fewer than 10 custom rules; mostly relying on vendor/out-of-the-box rules
@@ -2026,25 +2049,25 @@
 5 — 100+ rules with continuous refinement, environment-specific tuning, and automated coverage analysis</t>
         </is>
       </c>
-      <c r="E24" s="19" t="n"/>
-      <c r="F24" s="20">
-        <f>IF(E24="","",E24)</f>
-        <v/>
-      </c>
-      <c r="G24" s="21" t="n"/>
-    </row>
-    <row r="25" ht="115" customHeight="1">
-      <c r="B25" s="22" t="inlineStr">
+      <c r="E25" s="19" t="n"/>
+      <c r="F25" s="20">
+        <f>IF(E25="","",E25)</f>
+        <v/>
+      </c>
+      <c r="G25" s="21" t="n"/>
+    </row>
+    <row r="26" ht="115" customHeight="1">
+      <c r="B26" s="22" t="inlineStr">
         <is>
           <t>T1-Q2</t>
         </is>
       </c>
-      <c r="C25" s="23" t="inlineStr">
+      <c r="C26" s="23" t="inlineStr">
         <is>
           <t>Baseline Rule Creation</t>
         </is>
       </c>
-      <c r="D25" s="24" t="inlineStr">
+      <c r="D26" s="24" t="inlineStr">
         <is>
           <t>Estimate the assessed team's MITRE ATT&amp;CK technique coverage for priority areas.
 1 — Unknown or not measured; no ATT&amp;CK mapping performed
@@ -2054,25 +2077,25 @@
 5 — Over 70% coverage with continuous gap analysis and automated coverage tracking</t>
         </is>
       </c>
-      <c r="E25" s="19" t="n"/>
-      <c r="F25" s="25">
-        <f>IF(E25="","",E25)</f>
-        <v/>
-      </c>
-      <c r="G25" s="21" t="n"/>
-    </row>
-    <row r="26" ht="115" customHeight="1">
-      <c r="B26" s="16" t="inlineStr">
+      <c r="E26" s="19" t="n"/>
+      <c r="F26" s="25">
+        <f>IF(E26="","",E26)</f>
+        <v/>
+      </c>
+      <c r="G26" s="21" t="n"/>
+    </row>
+    <row r="27" ht="115" customHeight="1">
+      <c r="B27" s="16" t="inlineStr">
         <is>
           <t>T1-Q3</t>
         </is>
       </c>
-      <c r="C26" s="17" t="inlineStr">
+      <c r="C27" s="17" t="inlineStr">
         <is>
           <t>Ruleset Management and Maintenance</t>
         </is>
       </c>
-      <c r="D26" s="18" t="inlineStr">
+      <c r="D27" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's ruleset management.
 1 — No formal management; rules live only in the SIEM console with no version control or documentation (&lt;20% in version control)
@@ -2082,25 +2105,25 @@
 5 — Fully automated rule lifecycle: CI/CD, automated testing, continuous validation, and weekly maintenance cycles (100% DaC)</t>
         </is>
       </c>
-      <c r="E26" s="19" t="n"/>
-      <c r="F26" s="20">
-        <f>IF(E26="","",E26)</f>
-        <v/>
-      </c>
-      <c r="G26" s="21" t="n"/>
-    </row>
-    <row r="27" ht="115" customHeight="1">
-      <c r="B27" s="22" t="inlineStr">
+      <c r="E27" s="19" t="n"/>
+      <c r="F27" s="20">
+        <f>IF(E27="","",E27)</f>
+        <v/>
+      </c>
+      <c r="G27" s="21" t="n"/>
+    </row>
+    <row r="28" ht="115" customHeight="1">
+      <c r="B28" s="22" t="inlineStr">
         <is>
           <t>T1-Q4</t>
         </is>
       </c>
-      <c r="C27" s="26" t="inlineStr">
+      <c r="C28" s="26" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D27" s="24" t="inlineStr">
+      <c r="D28" s="24" t="inlineStr">
         <is>
           <t>Rate the quality and coverage of the assessed team's telemetry.
 1 — No active telemetry management; using whatever data sources happen to be available (&lt;30% of rule types have adequate telemetry)
@@ -2110,71 +2133,71 @@
 5 — Advanced workflows with real-time enrichment, automated remediation of telemetry gaps, full CTI integration (90-100% coverage)</t>
         </is>
       </c>
-      <c r="E27" s="19" t="n"/>
-      <c r="F27" s="25">
-        <f>IF(E27="","",E27)</f>
-        <v/>
-      </c>
-      <c r="G27" s="21" t="n"/>
-    </row>
-    <row r="28" ht="35" customHeight="1">
-      <c r="B28" s="16" t="inlineStr">
+      <c r="E28" s="19" t="n"/>
+      <c r="F28" s="25">
+        <f>IF(E28="","",E28)</f>
+        <v/>
+      </c>
+      <c r="G28" s="21" t="n"/>
+    </row>
+    <row r="29" ht="35" customHeight="1">
+      <c r="B29" s="16" t="inlineStr">
         <is>
           <t>T1-Q5</t>
         </is>
       </c>
-      <c r="C28" s="27" t="inlineStr">
+      <c r="C29" s="27" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D28" s="18" t="inlineStr">
+      <c r="D29" s="18" t="inlineStr">
         <is>
           <t>Does the assessed team maintain a documented data source inventory mapped to use cases?</t>
         </is>
       </c>
-      <c r="E28" s="19" t="n"/>
-      <c r="F28" s="20">
-        <f>IF(E28="Yes",3,IF(E28="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G28" s="21" t="n"/>
-    </row>
-    <row r="29" ht="35" customHeight="1">
-      <c r="B29" s="22" t="inlineStr">
+      <c r="E29" s="19" t="n"/>
+      <c r="F29" s="20">
+        <f>IF(E29="Yes",3,IF(E29="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G29" s="21" t="n"/>
+    </row>
+    <row r="30" ht="35" customHeight="1">
+      <c r="B30" s="22" t="inlineStr">
         <is>
           <t>T1-Q6</t>
         </is>
       </c>
-      <c r="C29" s="23" t="inlineStr">
+      <c r="C30" s="23" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D29" s="24" t="inlineStr">
+      <c r="D30" s="24" t="inlineStr">
         <is>
           <t>Does the assessed team have automated alerting for data source degradation?</t>
         </is>
       </c>
-      <c r="E29" s="19" t="n"/>
-      <c r="F29" s="25">
-        <f>IF(E29="Yes",4,IF(E29="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G29" s="21" t="n"/>
-    </row>
-    <row r="30" ht="115" customHeight="1">
-      <c r="B30" s="16" t="inlineStr">
+      <c r="E30" s="19" t="n"/>
+      <c r="F30" s="25">
+        <f>IF(E30="Yes",4,IF(E30="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G30" s="21" t="n"/>
+    </row>
+    <row r="31" ht="115" customHeight="1">
+      <c r="B31" s="16" t="inlineStr">
         <is>
           <t>T1-Q7</t>
         </is>
       </c>
-      <c r="C30" s="17" t="inlineStr">
+      <c r="C31" s="17" t="inlineStr">
         <is>
           <t>Threat Landscape Review</t>
         </is>
       </c>
-      <c r="D30" s="18" t="inlineStr">
+      <c r="D31" s="18" t="inlineStr">
         <is>
           <t>How frequently does the assessed team review the threat landscape?
 1 — No regular reviews; detection priorities are not informed by current threats
@@ -2184,25 +2207,25 @@
 5 — Real-time threat landscape monitoring with automated intel feeds driving detection priority updates (90-100% aligned)</t>
         </is>
       </c>
-      <c r="E30" s="19" t="n"/>
-      <c r="F30" s="20">
-        <f>IF(E30="","",E30)</f>
-        <v/>
-      </c>
-      <c r="G30" s="21" t="n"/>
-    </row>
-    <row r="31" ht="115" customHeight="1">
-      <c r="B31" s="22" t="inlineStr">
+      <c r="E31" s="19" t="n"/>
+      <c r="F31" s="20">
+        <f>IF(E31="","",E31)</f>
+        <v/>
+      </c>
+      <c r="G31" s="21" t="n"/>
+    </row>
+    <row r="32" ht="115" customHeight="1">
+      <c r="B32" s="22" t="inlineStr">
         <is>
           <t>T1-Q8</t>
         </is>
       </c>
-      <c r="C31" s="26" t="inlineStr">
+      <c r="C32" s="26" t="inlineStr">
         <is>
           <t>Product Owner Engagement</t>
         </is>
       </c>
-      <c r="D31" s="24" t="inlineStr">
+      <c r="D32" s="24" t="inlineStr">
         <is>
           <t>Rate the engagement between the assessed team and product/platform owners.
 1 — No engagement; detection needs are never communicated to product/platform teams
@@ -2212,25 +2235,25 @@
 5 — Continuous engagement with joint planning, shared success metrics, and detection needs directly influencing product development</t>
         </is>
       </c>
-      <c r="E31" s="19" t="n"/>
-      <c r="F31" s="25">
-        <f>IF(E31="","",E31)</f>
-        <v/>
-      </c>
-      <c r="G31" s="21" t="n"/>
-    </row>
-    <row r="32" ht="115" customHeight="1">
-      <c r="B32" s="16" t="inlineStr">
+      <c r="E32" s="19" t="n"/>
+      <c r="F32" s="25">
+        <f>IF(E32="","",E32)</f>
+        <v/>
+      </c>
+      <c r="G32" s="21" t="n"/>
+    </row>
+    <row r="33" ht="115" customHeight="1">
+      <c r="B33" s="16" t="inlineStr">
         <is>
           <t>T1-Q9</t>
         </is>
       </c>
-      <c r="C32" s="17" t="inlineStr">
+      <c r="C33" s="17" t="inlineStr">
         <is>
           <t>Release Testing and Validation</t>
         </is>
       </c>
-      <c r="D32" s="18" t="inlineStr">
+      <c r="D33" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's release testing.
 1 — No testing; rules are deployed to production without validation (&lt;20% tested)
@@ -2240,48 +2263,48 @@
 5 — Continuous automated testing in full CI/CD pipeline; every rule validated before every deployment (90-100% automated)</t>
         </is>
       </c>
-      <c r="E32" s="19" t="n"/>
-      <c r="F32" s="20">
-        <f>IF(E32="","",E32)</f>
-        <v/>
-      </c>
-      <c r="G32" s="21" t="n"/>
-    </row>
-    <row r="33" ht="34" customHeight="1">
-      <c r="B33" s="15" t="inlineStr">
+      <c r="E33" s="19" t="n"/>
+      <c r="F33" s="20">
+        <f>IF(E33="","",E33)</f>
+        <v/>
+      </c>
+      <c r="G33" s="21" t="n"/>
+    </row>
+    <row r="34" ht="34" customHeight="1">
+      <c r="B34" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">  TIER 2: INTERMEDIATE</t>
         </is>
       </c>
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-      <c r="E33" s="4" t="n"/>
-      <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
-    </row>
-    <row r="34" ht="20" customHeight="1">
-      <c r="B34" s="13" t="inlineStr">
+      <c r="C34" s="4" t="n"/>
+      <c r="D34" s="4" t="n"/>
+      <c r="E34" s="4" t="n"/>
+      <c r="F34" s="4" t="n"/>
+      <c r="G34" s="4" t="n"/>
+    </row>
+    <row r="35" ht="20" customHeight="1">
+      <c r="B35" s="13" t="inlineStr">
         <is>
           <t>Focuses on improving detection quality through tuning, gap analysis, and systematic internal validation.</t>
         </is>
       </c>
-      <c r="C34" s="6" t="n"/>
-      <c r="D34" s="6" t="n"/>
-      <c r="E34" s="6" t="n"/>
-      <c r="F34" s="6" t="n"/>
-    </row>
-    <row r="35" ht="115" customHeight="1">
-      <c r="B35" s="16" t="inlineStr">
+      <c r="C35" s="6" t="n"/>
+      <c r="D35" s="6" t="n"/>
+      <c r="E35" s="6" t="n"/>
+      <c r="F35" s="6" t="n"/>
+    </row>
+    <row r="36" ht="115" customHeight="1">
+      <c r="B36" s="16" t="inlineStr">
         <is>
           <t>T2-Q1</t>
         </is>
       </c>
-      <c r="C35" s="17" t="inlineStr">
+      <c r="C36" s="17" t="inlineStr">
         <is>
           <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
-      <c r="D35" s="18" t="inlineStr">
+      <c r="D36" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's FP reduction program.
 1 — Minimal or no tuning; high false positive rates accepted as normal; no FP metrics tracked
@@ -2291,25 +2314,25 @@
 5 — Automated dynamic tuning with ML; near-zero unnecessary alert noise; continuous optimization (&gt;75% FP reduction from baseline)</t>
         </is>
       </c>
-      <c r="E35" s="19" t="n"/>
-      <c r="F35" s="20">
-        <f>IF(E35="","",E35)</f>
-        <v/>
-      </c>
-      <c r="G35" s="21" t="n"/>
-    </row>
-    <row r="36" ht="115" customHeight="1">
-      <c r="B36" s="22" t="inlineStr">
+      <c r="E36" s="19" t="n"/>
+      <c r="F36" s="20">
+        <f>IF(E36="","",E36)</f>
+        <v/>
+      </c>
+      <c r="G36" s="21" t="n"/>
+    </row>
+    <row r="37" ht="115" customHeight="1">
+      <c r="B37" s="22" t="inlineStr">
         <is>
           <t>T2-Q2</t>
         </is>
       </c>
-      <c r="C36" s="23" t="inlineStr">
+      <c r="C37" s="23" t="inlineStr">
         <is>
           <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
-      <c r="D36" s="24" t="inlineStr">
+      <c r="D37" s="24" t="inlineStr">
         <is>
           <t>What is the assessed team's estimated FP reduction from baseline?
 1 — Unknown or not measured
@@ -2319,25 +2342,25 @@
 5 — Over 75% reduction with ML-assisted continuous tuning</t>
         </is>
       </c>
-      <c r="E36" s="19" t="n"/>
-      <c r="F36" s="25">
-        <f>IF(E36="","",E36)</f>
-        <v/>
-      </c>
-      <c r="G36" s="21" t="n"/>
-    </row>
-    <row r="37" ht="115" customHeight="1">
-      <c r="B37" s="16" t="inlineStr">
+      <c r="E37" s="19" t="n"/>
+      <c r="F37" s="25">
+        <f>IF(E37="","",E37)</f>
+        <v/>
+      </c>
+      <c r="G37" s="21" t="n"/>
+    </row>
+    <row r="38" ht="115" customHeight="1">
+      <c r="B38" s="16" t="inlineStr">
         <is>
           <t>T2-Q3</t>
         </is>
       </c>
-      <c r="C37" s="17" t="inlineStr">
+      <c r="C38" s="17" t="inlineStr">
         <is>
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
-      <c r="D37" s="18" t="inlineStr">
+      <c r="D38" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's gap analysis.
 1 — No gap analysis performed; detection coverage gaps are unknown
@@ -2347,71 +2370,94 @@
 5 — Automated gap analysis using coverage mapping tools; real-time dashboards showing detection coverage (automated continuous analysis)</t>
         </is>
       </c>
-      <c r="E37" s="19" t="n"/>
-      <c r="F37" s="20">
-        <f>IF(E37="","",E37)</f>
-        <v/>
-      </c>
-      <c r="G37" s="21" t="n"/>
-    </row>
-    <row r="38" ht="35" customHeight="1">
-      <c r="B38" s="22" t="inlineStr">
+      <c r="E38" s="19" t="n"/>
+      <c r="F38" s="20">
+        <f>IF(E38="","",E38)</f>
+        <v/>
+      </c>
+      <c r="G38" s="21" t="n"/>
+    </row>
+    <row r="39" ht="35" customHeight="1">
+      <c r="B39" s="22" t="inlineStr">
         <is>
           <t>T2-Q4</t>
         </is>
       </c>
-      <c r="C38" s="23" t="inlineStr">
+      <c r="C39" s="23" t="inlineStr">
         <is>
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
-      <c r="D38" s="24" t="inlineStr">
+      <c r="D39" s="24" t="inlineStr">
         <is>
           <t>Does the assessed team maintain a documented, prioritized gap list updated quarterly?</t>
         </is>
       </c>
-      <c r="E38" s="19" t="n"/>
-      <c r="F38" s="25">
-        <f>IF(E38="Yes",3,IF(E38="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G38" s="21" t="n"/>
-    </row>
-    <row r="39" ht="35" customHeight="1">
-      <c r="B39" s="16" t="inlineStr">
+      <c r="E39" s="19" t="n"/>
+      <c r="F39" s="25">
+        <f>IF(E39="Yes",3,IF(E39="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G39" s="21" t="n"/>
+    </row>
+    <row r="40" ht="35" customHeight="1">
+      <c r="B40" s="16" t="inlineStr">
         <is>
           <t>T2-Q5</t>
         </is>
       </c>
-      <c r="C39" s="27" t="inlineStr">
+      <c r="C40" s="27" t="inlineStr">
         <is>
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
-      <c r="D39" s="18" t="inlineStr">
+      <c r="D40" s="18" t="inlineStr">
         <is>
           <t>Are the assessed team's gaps communicated to stakeholders at least quarterly?</t>
         </is>
       </c>
-      <c r="E39" s="19" t="n"/>
-      <c r="F39" s="20">
-        <f>IF(E39="Yes",4,IF(E39="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G39" s="21" t="n"/>
-    </row>
-    <row r="40" ht="115" customHeight="1">
-      <c r="B40" s="22" t="inlineStr">
+      <c r="E40" s="19" t="n"/>
+      <c r="F40" s="20">
+        <f>IF(E40="Yes",4,IF(E40="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G40" s="21" t="n"/>
+    </row>
+    <row r="41" ht="35" customHeight="1">
+      <c r="B41" s="22" t="inlineStr">
+        <is>
+          <t>T2-Q7</t>
+        </is>
+      </c>
+      <c r="C41" s="23" t="inlineStr">
+        <is>
+          <t>Gap Analysis and Documentation</t>
+        </is>
+      </c>
+      <c r="D41" s="24" t="inlineStr">
+        <is>
+          <t>Does the assessed team maintain a formal detection coverage map linking assets and threat actors to detection rules?</t>
+        </is>
+      </c>
+      <c r="E41" s="19" t="n"/>
+      <c r="F41" s="25">
+        <f>IF(E41="Yes",4,IF(E41="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G41" s="21" t="n"/>
+    </row>
+    <row r="42" ht="115" customHeight="1">
+      <c r="B42" s="16" t="inlineStr">
         <is>
           <t>T2-Q6</t>
         </is>
       </c>
-      <c r="C40" s="26" t="inlineStr">
+      <c r="C42" s="17" t="inlineStr">
         <is>
           <t>Internal Testing and Validation</t>
         </is>
       </c>
-      <c r="D40" s="24" t="inlineStr">
+      <c r="D42" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's internal testing program.
 1 — No internal testing; rules are assumed to work once deployed
@@ -2421,48 +2467,48 @@
 5 — Continuous automated testing with full emulation coverage and automated regression testing on every rule change (&gt;90% automated coverage)</t>
         </is>
       </c>
-      <c r="E40" s="19" t="n"/>
-      <c r="F40" s="25">
-        <f>IF(E40="","",E40)</f>
-        <v/>
-      </c>
-      <c r="G40" s="21" t="n"/>
-    </row>
-    <row r="41" ht="34" customHeight="1">
-      <c r="B41" s="15" t="inlineStr">
+      <c r="E42" s="19" t="n"/>
+      <c r="F42" s="20">
+        <f>IF(E42="","",E42)</f>
+        <v/>
+      </c>
+      <c r="G42" s="21" t="n"/>
+    </row>
+    <row r="43" ht="34" customHeight="1">
+      <c r="B43" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">  TIER 3: ADVANCED</t>
         </is>
       </c>
-      <c r="C41" s="4" t="n"/>
-      <c r="D41" s="4" t="n"/>
-      <c r="E41" s="4" t="n"/>
-      <c r="F41" s="4" t="n"/>
-      <c r="G41" s="4" t="n"/>
-    </row>
-    <row r="42" ht="20" customHeight="1">
-      <c r="B42" s="13" t="inlineStr">
+      <c r="C43" s="4" t="n"/>
+      <c r="D43" s="4" t="n"/>
+      <c r="E43" s="4" t="n"/>
+      <c r="F43" s="4" t="n"/>
+      <c r="G43" s="4" t="n"/>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="B44" s="13" t="inlineStr">
         <is>
           <t>Addresses false negatives, external validation, and advanced threat coverage to ensure detections catch real attacks.</t>
         </is>
       </c>
-      <c r="C42" s="6" t="n"/>
-      <c r="D42" s="6" t="n"/>
-      <c r="E42" s="6" t="n"/>
-      <c r="F42" s="6" t="n"/>
-    </row>
-    <row r="43" ht="115" customHeight="1">
-      <c r="B43" s="16" t="inlineStr">
+      <c r="C44" s="6" t="n"/>
+      <c r="D44" s="6" t="n"/>
+      <c r="E44" s="6" t="n"/>
+      <c r="F44" s="6" t="n"/>
+    </row>
+    <row r="45" ht="115" customHeight="1">
+      <c r="B45" s="16" t="inlineStr">
         <is>
           <t>T3-Q1</t>
         </is>
       </c>
-      <c r="C43" s="17" t="inlineStr">
+      <c r="C45" s="17" t="inlineStr">
         <is>
           <t>False Negative Triage</t>
         </is>
       </c>
-      <c r="D43" s="18" t="inlineStr">
+      <c r="D45" s="18" t="inlineStr">
         <is>
           <t>Rate the assessed team's ability to detect and remediate false negatives.
 1 — No FN identification process; missed detections only discovered during incident response
@@ -2472,25 +2518,25 @@
 5 — Continuous automated FN detection using real-time validation against live threat samples (near-zero FN rate; &gt;75% FN reduction)</t>
         </is>
       </c>
-      <c r="E43" s="19" t="n"/>
-      <c r="F43" s="20">
-        <f>IF(E43="","",E43)</f>
-        <v/>
-      </c>
-      <c r="G43" s="21" t="n"/>
-    </row>
-    <row r="44" ht="115" customHeight="1">
-      <c r="B44" s="22" t="inlineStr">
+      <c r="E45" s="19" t="n"/>
+      <c r="F45" s="20">
+        <f>IF(E45="","",E45)</f>
+        <v/>
+      </c>
+      <c r="G45" s="21" t="n"/>
+    </row>
+    <row r="46" ht="115" customHeight="1">
+      <c r="B46" s="22" t="inlineStr">
         <is>
           <t>T3-Q2</t>
         </is>
       </c>
-      <c r="C44" s="23" t="inlineStr">
+      <c r="C46" s="23" t="inlineStr">
         <is>
           <t>False Negative Triage</t>
         </is>
       </c>
-      <c r="D44" s="24" t="inlineStr">
+      <c r="D46" s="24" t="inlineStr">
         <is>
           <t>What is the assessed team's detection trigger rate on tested samples?
 1 — Unknown or not tested
@@ -2500,25 +2546,25 @@
 5 — Over 90% trigger rate with continuous regression testing</t>
         </is>
       </c>
-      <c r="E44" s="19" t="n"/>
-      <c r="F44" s="25">
-        <f>IF(E44="","",E44)</f>
-        <v/>
-      </c>
-      <c r="G44" s="21" t="n"/>
-    </row>
-    <row r="45" ht="115" customHeight="1">
-      <c r="B45" s="16" t="inlineStr">
+      <c r="E46" s="19" t="n"/>
+      <c r="F46" s="25">
+        <f>IF(E46="","",E46)</f>
+        <v/>
+      </c>
+      <c r="G46" s="21" t="n"/>
+    </row>
+    <row r="47" ht="115" customHeight="1">
+      <c r="B47" s="16" t="inlineStr">
         <is>
           <t>T3-Q3</t>
         </is>
       </c>
-      <c r="C45" s="17" t="inlineStr">
+      <c r="C47" s="17" t="inlineStr">
         <is>
           <t>External Validation</t>
         </is>
       </c>
-      <c r="D45" s="18" t="inlineStr">
+      <c r="D47" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's external validation.
 1 — No external validation; no red team, pentest, or third-party assessment of detection effectiveness
@@ -2528,25 +2574,25 @@
 5 — Continuous BAS (breach and attack simulation) tools and regular adversary emulation exercises with real-time feedback loops</t>
         </is>
       </c>
-      <c r="E45" s="19" t="n"/>
-      <c r="F45" s="20">
-        <f>IF(E45="","",E45)</f>
-        <v/>
-      </c>
-      <c r="G45" s="21" t="n"/>
-    </row>
-    <row r="46" ht="115" customHeight="1">
-      <c r="B46" s="22" t="inlineStr">
+      <c r="E47" s="19" t="n"/>
+      <c r="F47" s="20">
+        <f>IF(E47="","",E47)</f>
+        <v/>
+      </c>
+      <c r="G47" s="21" t="n"/>
+    </row>
+    <row r="48" ht="115" customHeight="1">
+      <c r="B48" s="22" t="inlineStr">
         <is>
           <t>T3-Q4</t>
         </is>
       </c>
-      <c r="C46" s="26" t="inlineStr">
+      <c r="C48" s="26" t="inlineStr">
         <is>
           <t>Advanced TTP Coverage</t>
         </is>
       </c>
-      <c r="D46" s="24" t="inlineStr">
+      <c r="D48" s="24" t="inlineStr">
         <is>
           <t>Rate the assessed team's coverage of advanced TTPs.
 1 — No advanced TTP coverage; detections are signature/IOC-based only
@@ -2556,25 +2602,25 @@
 5 — Continuous proactive coverage using AI/ML for anomaly detection and automated response to emerging TTPs; real-time advanced TTP detection</t>
         </is>
       </c>
-      <c r="E46" s="19" t="n"/>
-      <c r="F46" s="25">
-        <f>IF(E46="","",E46)</f>
-        <v/>
-      </c>
-      <c r="G46" s="21" t="n"/>
-    </row>
-    <row r="47" ht="115" customHeight="1">
-      <c r="B47" s="16" t="inlineStr">
+      <c r="E48" s="19" t="n"/>
+      <c r="F48" s="25">
+        <f>IF(E48="","",E48)</f>
+        <v/>
+      </c>
+      <c r="G48" s="21" t="n"/>
+    </row>
+    <row r="49" ht="115" customHeight="1">
+      <c r="B49" s="16" t="inlineStr">
         <is>
           <t>T3-Q5</t>
         </is>
       </c>
-      <c r="C47" s="27" t="inlineStr">
+      <c r="C49" s="27" t="inlineStr">
         <is>
           <t>Advanced TTP Coverage</t>
         </is>
       </c>
-      <c r="D47" s="18" t="inlineStr">
+      <c r="D49" s="18" t="inlineStr">
         <is>
           <t>How many of these categories does the assessed team have behavioral detections for: LOLBins, fileless malware, credential evasion, defense evasion, lateral movement?
 1 — None of these
@@ -2584,48 +2630,48 @@
 5 — All 5 plus additional categories (e.g., supply chain attacks, AI-assisted threats)</t>
         </is>
       </c>
-      <c r="E47" s="19" t="n"/>
-      <c r="F47" s="20">
-        <f>IF(E47="","",E47)</f>
-        <v/>
-      </c>
-      <c r="G47" s="21" t="n"/>
-    </row>
-    <row r="48" ht="34" customHeight="1">
-      <c r="B48" s="15" t="inlineStr">
+      <c r="E49" s="19" t="n"/>
+      <c r="F49" s="20">
+        <f>IF(E49="","",E49)</f>
+        <v/>
+      </c>
+      <c r="G49" s="21" t="n"/>
+    </row>
+    <row r="50" ht="34" customHeight="1">
+      <c r="B50" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">  TIER 4: EXPERT</t>
         </is>
       </c>
-      <c r="C48" s="4" t="n"/>
-      <c r="D48" s="4" t="n"/>
-      <c r="E48" s="4" t="n"/>
-      <c r="F48" s="4" t="n"/>
-      <c r="G48" s="4" t="n"/>
-    </row>
-    <row r="49" ht="20" customHeight="1">
-      <c r="B49" s="13" t="inlineStr">
+      <c r="C50" s="4" t="n"/>
+      <c r="D50" s="4" t="n"/>
+      <c r="E50" s="4" t="n"/>
+      <c r="F50" s="4" t="n"/>
+      <c r="G50" s="4" t="n"/>
+    </row>
+    <row r="51" ht="20" customHeight="1">
+      <c r="B51" s="13" t="inlineStr">
         <is>
           <t>Features proactive threat hunting, advanced automation, AI/LLM integration, and continuous improvement across the detection lifecycle.</t>
         </is>
       </c>
-      <c r="C49" s="6" t="n"/>
-      <c r="D49" s="6" t="n"/>
-      <c r="E49" s="6" t="n"/>
-      <c r="F49" s="6" t="n"/>
-    </row>
-    <row r="50" ht="115" customHeight="1">
-      <c r="B50" s="16" t="inlineStr">
+      <c r="C51" s="6" t="n"/>
+      <c r="D51" s="6" t="n"/>
+      <c r="E51" s="6" t="n"/>
+      <c r="F51" s="6" t="n"/>
+    </row>
+    <row r="52" ht="115" customHeight="1">
+      <c r="B52" s="16" t="inlineStr">
         <is>
           <t>T4-Q1</t>
         </is>
       </c>
-      <c r="C50" s="17" t="inlineStr">
+      <c r="C52" s="17" t="inlineStr">
         <is>
           <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
-      <c r="D50" s="18" t="inlineStr">
+      <c r="D52" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's threat hunting.
 1 — No proactive hunting; all detection is passive through deployed rules
@@ -2635,71 +2681,71 @@
 5 — Automated real-time hunting augmented by AI/ML; hunting outputs automatically generate detection rule candidates</t>
         </is>
       </c>
-      <c r="E50" s="19" t="n"/>
-      <c r="F50" s="20">
-        <f>IF(E50="","",E50)</f>
-        <v/>
-      </c>
-      <c r="G50" s="21" t="n"/>
-    </row>
-    <row r="51" ht="35" customHeight="1">
-      <c r="B51" s="22" t="inlineStr">
-        <is>
-          <t>T4-Q2</t>
-        </is>
-      </c>
-      <c r="C51" s="23" t="inlineStr">
-        <is>
-          <t>Threat Hunting in Telemetry</t>
-        </is>
-      </c>
-      <c r="D51" s="24" t="inlineStr">
-        <is>
-          <t>Are the assessed team's hunts driven by documented hypotheses?</t>
-        </is>
-      </c>
-      <c r="E51" s="19" t="n"/>
-      <c r="F51" s="25">
-        <f>IF(E51="Yes",4,IF(E51="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G51" s="21" t="n"/>
-    </row>
-    <row r="52" ht="35" customHeight="1">
-      <c r="B52" s="16" t="inlineStr">
-        <is>
-          <t>T4-Q3</t>
-        </is>
-      </c>
-      <c r="C52" s="27" t="inlineStr">
-        <is>
-          <t>Threat Hunting in Telemetry</t>
-        </is>
-      </c>
-      <c r="D52" s="18" t="inlineStr">
-        <is>
-          <t>Is there a defined process to convert hunting findings into production rules?</t>
-        </is>
-      </c>
       <c r="E52" s="19" t="n"/>
       <c r="F52" s="20">
-        <f>IF(E52="Yes",4,IF(E52="No",1,""))</f>
+        <f>IF(E52="","",E52)</f>
         <v/>
       </c>
       <c r="G52" s="21" t="n"/>
     </row>
-    <row r="53" ht="115" customHeight="1">
+    <row r="53" ht="35" customHeight="1">
       <c r="B53" s="22" t="inlineStr">
         <is>
+          <t>T4-Q2</t>
+        </is>
+      </c>
+      <c r="C53" s="23" t="inlineStr">
+        <is>
+          <t>Threat Hunting in Telemetry</t>
+        </is>
+      </c>
+      <c r="D53" s="24" t="inlineStr">
+        <is>
+          <t>Are the assessed team's hunts driven by documented hypotheses?</t>
+        </is>
+      </c>
+      <c r="E53" s="19" t="n"/>
+      <c r="F53" s="25">
+        <f>IF(E53="Yes",4,IF(E53="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G53" s="21" t="n"/>
+    </row>
+    <row r="54" ht="35" customHeight="1">
+      <c r="B54" s="16" t="inlineStr">
+        <is>
+          <t>T4-Q3</t>
+        </is>
+      </c>
+      <c r="C54" s="27" t="inlineStr">
+        <is>
+          <t>Threat Hunting in Telemetry</t>
+        </is>
+      </c>
+      <c r="D54" s="18" t="inlineStr">
+        <is>
+          <t>Is there a defined process to convert hunting findings into production rules?</t>
+        </is>
+      </c>
+      <c r="E54" s="19" t="n"/>
+      <c r="F54" s="20">
+        <f>IF(E54="Yes",4,IF(E54="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G54" s="21" t="n"/>
+    </row>
+    <row r="55" ht="115" customHeight="1">
+      <c r="B55" s="22" t="inlineStr">
+        <is>
           <t>T4-Q4</t>
         </is>
       </c>
-      <c r="C53" s="26" t="inlineStr">
+      <c r="C55" s="26" t="inlineStr">
         <is>
           <t>Automation and Continuous Improvement</t>
         </is>
       </c>
-      <c r="D53" s="24" t="inlineStr">
+      <c r="D55" s="24" t="inlineStr">
         <is>
           <t>What percentage of the assessed team's DE tasks are automated?
 1 — None; all processes are manual (0% automated)
@@ -2709,25 +2755,25 @@
 5 — Full AI/LLM integration throughout the detection lifecycle; automated rule generation, tuning, and retirement (&gt;90% automated; 40%+ FP reduction via AI)</t>
         </is>
       </c>
-      <c r="E53" s="19" t="n"/>
-      <c r="F53" s="25">
-        <f>IF(E53="","",E53)</f>
-        <v/>
-      </c>
-      <c r="G53" s="21" t="n"/>
-    </row>
-    <row r="54" ht="115" customHeight="1">
-      <c r="B54" s="16" t="inlineStr">
+      <c r="E55" s="19" t="n"/>
+      <c r="F55" s="25">
+        <f>IF(E55="","",E55)</f>
+        <v/>
+      </c>
+      <c r="G55" s="21" t="n"/>
+    </row>
+    <row r="56" ht="115" customHeight="1">
+      <c r="B56" s="16" t="inlineStr">
         <is>
           <t>T4-Q5</t>
         </is>
       </c>
-      <c r="C54" s="27" t="inlineStr">
+      <c r="C56" s="27" t="inlineStr">
         <is>
           <t>Automation and Continuous Improvement</t>
         </is>
       </c>
-      <c r="D54" s="18" t="inlineStr">
+      <c r="D56" s="18" t="inlineStr">
         <is>
           <t>How many detection lifecycle stages have automation or AI integration?
 1 — None; all stages are manual
@@ -2737,93 +2783,61 @@
 5 — All 6 stages with AI/LLM integration throughout</t>
         </is>
       </c>
-      <c r="E54" s="19" t="n"/>
-      <c r="F54" s="20">
-        <f>IF(E54="","",E54)</f>
-        <v/>
-      </c>
-      <c r="G54" s="21" t="n"/>
-    </row>
-    <row r="55" ht="20" customHeight="1">
-      <c r="A55" s="28" t="n"/>
-      <c r="B55" s="28" t="n"/>
-      <c r="C55" s="28" t="n"/>
-      <c r="D55" s="28" t="n"/>
-      <c r="E55" s="28" t="n"/>
-      <c r="F55" s="28" t="n"/>
-      <c r="G55" s="28" t="n"/>
-      <c r="H55" s="28" t="n"/>
-    </row>
-    <row r="56" ht="32" customHeight="1">
-      <c r="B56" s="29" t="inlineStr">
+      <c r="E56" s="19" t="n"/>
+      <c r="F56" s="20">
+        <f>IF(E56="","",E56)</f>
+        <v/>
+      </c>
+      <c r="G56" s="21" t="n"/>
+    </row>
+    <row r="57" ht="35" customHeight="1">
+      <c r="B57" s="22" t="inlineStr">
+        <is>
+          <t>T4-Q6</t>
+        </is>
+      </c>
+      <c r="C57" s="23" t="inlineStr">
+        <is>
+          <t>Automation and Continuous Improvement</t>
+        </is>
+      </c>
+      <c r="D57" s="24" t="inlineStr">
+        <is>
+          <t>Does the assessed team conduct regular retrospectives on detection failures to improve the process?</t>
+        </is>
+      </c>
+      <c r="E57" s="19" t="n"/>
+      <c r="F57" s="25">
+        <f>IF(E57="Yes",3,IF(E57="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G57" s="21" t="n"/>
+    </row>
+    <row r="58" ht="20" customHeight="1">
+      <c r="A58" s="28" t="n"/>
+      <c r="B58" s="28" t="n"/>
+      <c r="C58" s="28" t="n"/>
+      <c r="D58" s="28" t="n"/>
+      <c r="E58" s="28" t="n"/>
+      <c r="F58" s="28" t="n"/>
+      <c r="G58" s="28" t="n"/>
+      <c r="H58" s="28" t="n"/>
+    </row>
+    <row r="59" ht="32" customHeight="1">
+      <c r="B59" s="29" t="inlineStr">
         <is>
           <t>SUPPLEMENTARY DIMENSIONS — Organizational Readiness</t>
         </is>
       </c>
-      <c r="C56" s="30" t="n"/>
-      <c r="D56" s="30" t="n"/>
-      <c r="E56" s="30" t="n"/>
-      <c r="F56" s="30" t="n"/>
-    </row>
-    <row r="57" ht="22" customHeight="1">
-      <c r="B57" s="31" t="inlineStr">
+      <c r="C59" s="30" t="n"/>
+      <c r="D59" s="30" t="n"/>
+      <c r="E59" s="30" t="n"/>
+      <c r="F59" s="30" t="n"/>
+    </row>
+    <row r="60" ht="22" customHeight="1">
+      <c r="B60" s="31" t="inlineStr">
         <is>
           <t>These dimensions from detectionengineering.io assess people and process factors. They contribute to the overall score but do not affect DEBMM tier determination.</t>
-        </is>
-      </c>
-      <c r="C57" s="30" t="n"/>
-      <c r="D57" s="30" t="n"/>
-      <c r="E57" s="30" t="n"/>
-      <c r="F57" s="30" t="n"/>
-    </row>
-    <row r="58" ht="26" customHeight="1">
-      <c r="B58" s="32" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="C58" s="32" t="inlineStr">
-        <is>
-          <t>Criterion</t>
-        </is>
-      </c>
-      <c r="D58" s="32" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="E58" s="32" t="inlineStr">
-        <is>
-          <t>Answer</t>
-        </is>
-      </c>
-      <c r="F58" s="32" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-      <c r="G58" s="32" t="inlineStr">
-        <is>
-          <t>Evidence / Notes</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="34" customHeight="1">
-      <c r="B59" s="33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  PEOPLE &amp; ORGANIZATION</t>
-        </is>
-      </c>
-      <c r="C59" s="34" t="n"/>
-      <c r="D59" s="34" t="n"/>
-      <c r="E59" s="34" t="n"/>
-      <c r="F59" s="34" t="n"/>
-      <c r="G59" s="34" t="n"/>
-    </row>
-    <row r="60" ht="20" customHeight="1">
-      <c r="B60" s="31" t="inlineStr">
-        <is>
-          <t>Assesses the human and organizational factors that enable effective detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
       <c r="C60" s="30" t="n"/>
@@ -2831,18 +2845,73 @@
       <c r="E60" s="30" t="n"/>
       <c r="F60" s="30" t="n"/>
     </row>
-    <row r="61" ht="115" customHeight="1">
-      <c r="B61" s="16" t="inlineStr">
+    <row r="61" ht="26" customHeight="1">
+      <c r="B61" s="32" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C61" s="32" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="D61" s="32" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="E61" s="32" t="inlineStr">
+        <is>
+          <t>Answer</t>
+        </is>
+      </c>
+      <c r="F61" s="32" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="G61" s="32" t="inlineStr">
+        <is>
+          <t>Evidence / Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="34" customHeight="1">
+      <c r="B62" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  PEOPLE &amp; ORGANIZATION</t>
+        </is>
+      </c>
+      <c r="C62" s="34" t="n"/>
+      <c r="D62" s="34" t="n"/>
+      <c r="E62" s="34" t="n"/>
+      <c r="F62" s="34" t="n"/>
+      <c r="G62" s="34" t="n"/>
+    </row>
+    <row r="63" ht="20" customHeight="1">
+      <c r="B63" s="31" t="inlineStr">
+        <is>
+          <t>Assesses the human and organizational factors that enable effective detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
+        </is>
+      </c>
+      <c r="C63" s="30" t="n"/>
+      <c r="D63" s="30" t="n"/>
+      <c r="E63" s="30" t="n"/>
+      <c r="F63" s="30" t="n"/>
+    </row>
+    <row r="64" ht="115" customHeight="1">
+      <c r="B64" s="16" t="inlineStr">
         <is>
           <t>EP-Q1</t>
         </is>
       </c>
-      <c r="C61" s="17" t="inlineStr">
+      <c r="C64" s="17" t="inlineStr">
         <is>
           <t>Team Structure and Dedicated Roles</t>
         </is>
       </c>
-      <c r="D61" s="18" t="inlineStr">
+      <c r="D64" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed detection engineering team structure.
 1 — No dedicated roles; detection work is a side task for SOC analysts or other staff (0 dedicated FTEs)
@@ -2852,25 +2921,25 @@
 5 — Mature team with deep specialization, mentorship programs, and influence on organizational security strategy</t>
         </is>
       </c>
-      <c r="E61" s="19" t="n"/>
-      <c r="F61" s="20">
-        <f>IF(E61="","",E61)</f>
-        <v/>
-      </c>
-      <c r="G61" s="21" t="n"/>
-    </row>
-    <row r="62" ht="115" customHeight="1">
-      <c r="B62" s="35" t="inlineStr">
+      <c r="E64" s="19" t="n"/>
+      <c r="F64" s="20">
+        <f>IF(E64="","",E64)</f>
+        <v/>
+      </c>
+      <c r="G64" s="21" t="n"/>
+    </row>
+    <row r="65" ht="115" customHeight="1">
+      <c r="B65" s="35" t="inlineStr">
         <is>
           <t>EP-Q2</t>
         </is>
       </c>
-      <c r="C62" s="36" t="inlineStr">
+      <c r="C65" s="36" t="inlineStr">
         <is>
           <t>Skills Development and Training</t>
         </is>
       </c>
-      <c r="D62" s="37" t="inlineStr">
+      <c r="D65" s="37" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's skills development.
 1 — No formal training; learning is entirely self-directed with no organizational support or budget
@@ -2880,25 +2949,25 @@
 5 — Continuous learning culture with community contribution (blog posts, conference talks), internal research programs, and mentorship</t>
         </is>
       </c>
-      <c r="E62" s="19" t="n"/>
-      <c r="F62" s="38">
-        <f>IF(E62="","",E62)</f>
-        <v/>
-      </c>
-      <c r="G62" s="21" t="n"/>
-    </row>
-    <row r="63" ht="115" customHeight="1">
-      <c r="B63" s="16" t="inlineStr">
+      <c r="E65" s="19" t="n"/>
+      <c r="F65" s="38">
+        <f>IF(E65="","",E65)</f>
+        <v/>
+      </c>
+      <c r="G65" s="21" t="n"/>
+    </row>
+    <row r="66" ht="115" customHeight="1">
+      <c r="B66" s="16" t="inlineStr">
         <is>
           <t>EP-Q3</t>
         </is>
       </c>
-      <c r="C63" s="17" t="inlineStr">
+      <c r="C66" s="17" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D63" s="18" t="inlineStr">
+      <c r="D66" s="18" t="inlineStr">
         <is>
           <t>Rate the executive sponsorship of the assessed detection engineering function.
 1 — No executive awareness; detection engineering is not recognized as a distinct capability
@@ -2908,94 +2977,117 @@
 5 — Detection engineering is a strategic priority; board-level visibility; leadership actively champions the function across the organization</t>
         </is>
       </c>
-      <c r="E63" s="19" t="n"/>
-      <c r="F63" s="20">
-        <f>IF(E63="","",E63)</f>
-        <v/>
-      </c>
-      <c r="G63" s="21" t="n"/>
-    </row>
-    <row r="64" ht="35" customHeight="1">
-      <c r="B64" s="35" t="inlineStr">
+      <c r="E66" s="19" t="n"/>
+      <c r="F66" s="20">
+        <f>IF(E66="","",E66)</f>
+        <v/>
+      </c>
+      <c r="G66" s="21" t="n"/>
+    </row>
+    <row r="67" ht="35" customHeight="1">
+      <c r="B67" s="35" t="inlineStr">
         <is>
           <t>EP-Q4</t>
         </is>
       </c>
-      <c r="C64" s="39" t="inlineStr">
+      <c r="C67" s="39" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D64" s="37" t="inlineStr">
+      <c r="D67" s="37" t="inlineStr">
         <is>
           <t>Does the assessed team present metrics to executive leadership at least quarterly?</t>
         </is>
       </c>
-      <c r="E64" s="19" t="n"/>
-      <c r="F64" s="38">
-        <f>IF(E64="Yes",3,IF(E64="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G64" s="21" t="n"/>
-    </row>
-    <row r="65" ht="35" customHeight="1">
-      <c r="B65" s="16" t="inlineStr">
+      <c r="E67" s="19" t="n"/>
+      <c r="F67" s="38">
+        <f>IF(E67="Yes",3,IF(E67="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G67" s="21" t="n"/>
+    </row>
+    <row r="68" ht="35" customHeight="1">
+      <c r="B68" s="16" t="inlineStr">
         <is>
           <t>EP-Q5</t>
         </is>
       </c>
-      <c r="C65" s="27" t="inlineStr">
+      <c r="C68" s="27" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D65" s="18" t="inlineStr">
+      <c r="D68" s="18" t="inlineStr">
         <is>
           <t>Has leadership made investment/staffing decisions based on the assessed team's metrics in the past year?</t>
         </is>
       </c>
-      <c r="E65" s="19" t="n"/>
-      <c r="F65" s="20">
-        <f>IF(E65="Yes",4,IF(E65="No",1,""))</f>
-        <v/>
-      </c>
-      <c r="G65" s="21" t="n"/>
-    </row>
-    <row r="66" ht="34" customHeight="1">
-      <c r="B66" s="33" t="inlineStr">
+      <c r="E68" s="19" t="n"/>
+      <c r="F68" s="20">
+        <f>IF(E68="Yes",4,IF(E68="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G68" s="21" t="n"/>
+    </row>
+    <row r="69" ht="35" customHeight="1">
+      <c r="B69" s="35" t="inlineStr">
+        <is>
+          <t>EP-Q6</t>
+        </is>
+      </c>
+      <c r="C69" s="36" t="inlineStr">
+        <is>
+          <t>Team Structure and Dedicated Roles</t>
+        </is>
+      </c>
+      <c r="D69" s="37" t="inlineStr">
+        <is>
+          <t>Are designated owners assigned for key detection engineering activities in the assessed team?</t>
+        </is>
+      </c>
+      <c r="E69" s="19" t="n"/>
+      <c r="F69" s="38">
+        <f>IF(E69="Yes",3,IF(E69="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G69" s="21" t="n"/>
+    </row>
+    <row r="70" ht="34" customHeight="1">
+      <c r="B70" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">  PROCESS &amp; GOVERNANCE</t>
         </is>
       </c>
-      <c r="C66" s="34" t="n"/>
-      <c r="D66" s="34" t="n"/>
-      <c r="E66" s="34" t="n"/>
-      <c r="F66" s="34" t="n"/>
-      <c r="G66" s="34" t="n"/>
-    </row>
-    <row r="67" ht="20" customHeight="1">
-      <c r="B67" s="31" t="inlineStr">
+      <c r="C70" s="34" t="n"/>
+      <c r="D70" s="34" t="n"/>
+      <c r="E70" s="34" t="n"/>
+      <c r="F70" s="34" t="n"/>
+      <c r="G70" s="34" t="n"/>
+    </row>
+    <row r="71" ht="20" customHeight="1">
+      <c r="B71" s="31" t="inlineStr">
         <is>
           <t>Assesses the process maturity and governance structures supporting detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
-      <c r="C67" s="30" t="n"/>
-      <c r="D67" s="30" t="n"/>
-      <c r="E67" s="30" t="n"/>
-      <c r="F67" s="30" t="n"/>
-    </row>
-    <row r="68" ht="115" customHeight="1">
-      <c r="B68" s="16" t="inlineStr">
+      <c r="C71" s="30" t="n"/>
+      <c r="D71" s="30" t="n"/>
+      <c r="E71" s="30" t="n"/>
+      <c r="F71" s="30" t="n"/>
+    </row>
+    <row r="72" ht="115" customHeight="1">
+      <c r="B72" s="16" t="inlineStr">
         <is>
           <t>EG-Q1</t>
         </is>
       </c>
-      <c r="C68" s="17" t="inlineStr">
+      <c r="C72" s="17" t="inlineStr">
         <is>
           <t>Detection Lifecycle Workflow</t>
         </is>
       </c>
-      <c r="D68" s="18" t="inlineStr">
+      <c r="D72" s="18" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's detection lifecycle workflow.
 1 — No defined lifecycle; detections created and deployed without structured workflow
@@ -3005,25 +3097,25 @@
 5 — Optimized lifecycle with automated stage transitions, predictive analytics for rule retirement, and continuous process improvement</t>
         </is>
       </c>
-      <c r="E68" s="19" t="n"/>
-      <c r="F68" s="20">
-        <f>IF(E68="","",E68)</f>
-        <v/>
-      </c>
-      <c r="G68" s="21" t="n"/>
-    </row>
-    <row r="69" ht="115" customHeight="1">
-      <c r="B69" s="35" t="inlineStr">
+      <c r="E72" s="19" t="n"/>
+      <c r="F72" s="20">
+        <f>IF(E72="","",E72)</f>
+        <v/>
+      </c>
+      <c r="G72" s="21" t="n"/>
+    </row>
+    <row r="73" ht="115" customHeight="1">
+      <c r="B73" s="35" t="inlineStr">
         <is>
           <t>EG-Q2</t>
         </is>
       </c>
-      <c r="C69" s="36" t="inlineStr">
+      <c r="C73" s="36" t="inlineStr">
         <is>
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="D69" s="37" t="inlineStr">
+      <c r="D73" s="37" t="inlineStr">
         <is>
           <t>Rate the maturity of the assessed team's metrics program.
 1 — No metrics tracked; success is anecdotal or unmeasured
@@ -3033,25 +3125,25 @@
 5 — Advanced analytics with predictive metrics, industry benchmarking, and data-driven continuous optimization</t>
         </is>
       </c>
-      <c r="E69" s="19" t="n"/>
-      <c r="F69" s="38">
-        <f>IF(E69="","",E69)</f>
-        <v/>
-      </c>
-      <c r="G69" s="21" t="n"/>
-    </row>
-    <row r="70" ht="115" customHeight="1">
-      <c r="B70" s="16" t="inlineStr">
+      <c r="E73" s="19" t="n"/>
+      <c r="F73" s="38">
+        <f>IF(E73="","",E73)</f>
+        <v/>
+      </c>
+      <c r="G73" s="21" t="n"/>
+    </row>
+    <row r="74" ht="115" customHeight="1">
+      <c r="B74" s="16" t="inlineStr">
         <is>
           <t>EG-Q3</t>
         </is>
       </c>
-      <c r="C70" s="27" t="inlineStr">
+      <c r="C74" s="27" t="inlineStr">
         <is>
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="D70" s="18" t="inlineStr">
+      <c r="D74" s="18" t="inlineStr">
         <is>
           <t>How many of these KPI categories does the assessed team track: coverage, quality, velocity, rule health, analyst impact?
 1 — None of these are tracked
@@ -3061,25 +3153,25 @@
 5 — All 5 categories plus additional metrics with trend analysis and benchmarking</t>
         </is>
       </c>
-      <c r="E70" s="19" t="n"/>
-      <c r="F70" s="20">
-        <f>IF(E70="","",E70)</f>
-        <v/>
-      </c>
-      <c r="G70" s="21" t="n"/>
-    </row>
-    <row r="71" ht="115" customHeight="1">
-      <c r="B71" s="35" t="inlineStr">
+      <c r="E74" s="19" t="n"/>
+      <c r="F74" s="20">
+        <f>IF(E74="","",E74)</f>
+        <v/>
+      </c>
+      <c r="G74" s="21" t="n"/>
+    </row>
+    <row r="75" ht="115" customHeight="1">
+      <c r="B75" s="35" t="inlineStr">
         <is>
           <t>EG-Q4</t>
         </is>
       </c>
-      <c r="C71" s="36" t="inlineStr">
+      <c r="C75" s="36" t="inlineStr">
         <is>
           <t>Cross-Team Collaboration</t>
         </is>
       </c>
-      <c r="D71" s="37" t="inlineStr">
+      <c r="D75" s="37" t="inlineStr">
         <is>
           <t>Rate cross-team collaboration involving the assessed detection engineering function.
 1 — Operates in isolation; no structured collaboration with other teams
@@ -3089,42 +3181,65 @@
 5 — Seamless cross-functional collaboration with automated information sharing, shared metrics dashboards, and embedded team members</t>
         </is>
       </c>
-      <c r="E71" s="19" t="n"/>
-      <c r="F71" s="38">
-        <f>IF(E71="","",E71)</f>
-        <v/>
-      </c>
-      <c r="G71" s="21" t="n"/>
+      <c r="E75" s="19" t="n"/>
+      <c r="F75" s="38">
+        <f>IF(E75="","",E75)</f>
+        <v/>
+      </c>
+      <c r="G75" s="21" t="n"/>
+    </row>
+    <row r="76" ht="35" customHeight="1">
+      <c r="B76" s="16" t="inlineStr">
+        <is>
+          <t>EG-Q5</t>
+        </is>
+      </c>
+      <c r="C76" s="17" t="inlineStr">
+        <is>
+          <t>Detection Lifecycle Workflow</t>
+        </is>
+      </c>
+      <c r="D76" s="18" t="inlineStr">
+        <is>
+          <t>Is there a defined process to incorporate incident lessons learned into the assessed team's detection rule updates?</t>
+        </is>
+      </c>
+      <c r="E76" s="19" t="n"/>
+      <c r="F76" s="20">
+        <f>IF(E76="Yes",4,IF(E76="No",1,""))</f>
+        <v/>
+      </c>
+      <c r="G76" s="21" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B62:F62"/>
     <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B71:F71"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B70:F70"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B43:F43"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B42:F42"/>
     <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B67:F67"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B44:F44"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B49:F49"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B24:F24"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B35:F35"/>
   </mergeCells>
-  <conditionalFormatting sqref="F13:F71">
+  <conditionalFormatting sqref="F13:F76">
     <cfRule type="cellIs" priority="1" operator="between" dxfId="0">
       <formula>1</formula>
       <formula>1.49</formula>
@@ -3146,10 +3261,10 @@
     <dataValidation sqref="D8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Entry" error="Please select Self-Assessment or Audit" type="list">
       <formula1>"Self-Assessment,Audit"</formula1>
     </dataValidation>
-    <dataValidation sqref="E16 E20 E21 E28 E29 E38 E39 E51 E52 E64 E65" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select Yes or No" promptTitle="Answer" prompt="Select Yes or No" type="list">
+    <dataValidation sqref="E16 E20 E21 E22 E29 E30 E39 E40 E41 E53 E54 E57 E67 E68 E69 E76" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select Yes or No" promptTitle="Answer" prompt="Select Yes or No" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="E15 E17 E18 E19 E24 E25 E26 E27 E30 E31 E32 E35 E36 E37 E40 E43 E44 E45 E46 E47 E50 E53 E54 E61 E62 E63 E68 E69 E70 E71" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select a value from 1 to 5" promptTitle="Maturity Rating" prompt="Select 1 (Initial) through 5 (Optimized)" type="list">
+    <dataValidation sqref="E15 E17 E18 E19 E25 E26 E27 E28 E31 E32 E33 E36 E37 E38 E42 E45 E46 E47 E48 E49 E52 E55 E56 E64 E65 E66 E72 E73 E74 E75" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Please select a value from 1 to 5" promptTitle="Maturity Rating" prompt="Select 1 (Initial) through 5 (Optimized)" type="list">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3238,7 +3353,7 @@
       </c>
       <c r="E6" s="43" t="n"/>
       <c r="F6" s="44">
-        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
+        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E22,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E33,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E41,Assessment!E42,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E48,Assessment!E49,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E55,Assessment!E56,Assessment!E57,Assessment!E64,Assessment!E65,Assessment!E66,Assessment!E67,Assessment!E68,Assessment!E69,Assessment!E72,Assessment!E73,Assessment!E74,Assessment!E75,Assessment!E76)&amp;" / 46"</f>
         <v/>
       </c>
     </row>
@@ -3369,7 +3484,7 @@
         </is>
       </c>
       <c r="D16" s="50">
-        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22))</f>
         <v/>
       </c>
       <c r="E16" s="51">
@@ -3407,7 +3522,7 @@
         </is>
       </c>
       <c r="D18" s="50">
-        <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
+        <f>IF(COUNT(Assessment!F25,Assessment!F26)=0,"",AVERAGE(Assessment!F25,Assessment!F26))</f>
         <v/>
       </c>
       <c r="E18" s="51">
@@ -3426,7 +3541,7 @@
         </is>
       </c>
       <c r="D19" s="50">
-        <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
+        <f>IF(COUNT(Assessment!F27)=0,"",AVERAGE(Assessment!F27))</f>
         <v/>
       </c>
       <c r="E19" s="51">
@@ -3445,7 +3560,7 @@
         </is>
       </c>
       <c r="D20" s="50">
-        <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
+        <f>IF(COUNT(Assessment!F28,Assessment!F29,Assessment!F30)=0,"",AVERAGE(Assessment!F28,Assessment!F29,Assessment!F30))</f>
         <v/>
       </c>
       <c r="E20" s="51">
@@ -3464,7 +3579,7 @@
         </is>
       </c>
       <c r="D21" s="50">
-        <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
+        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
         <v/>
       </c>
       <c r="E21" s="51">
@@ -3483,7 +3598,7 @@
         </is>
       </c>
       <c r="D22" s="50">
-        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
+        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
         <v/>
       </c>
       <c r="E22" s="51">
@@ -3502,7 +3617,7 @@
         </is>
       </c>
       <c r="D23" s="50">
-        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
+        <f>IF(COUNT(Assessment!F33)=0,"",AVERAGE(Assessment!F33))</f>
         <v/>
       </c>
       <c r="E23" s="51">
@@ -3540,7 +3655,7 @@
         </is>
       </c>
       <c r="D25" s="50">
-        <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
+        <f>IF(COUNT(Assessment!F36,Assessment!F37)=0,"",AVERAGE(Assessment!F36,Assessment!F37))</f>
         <v/>
       </c>
       <c r="E25" s="51">
@@ -3559,7 +3674,7 @@
         </is>
       </c>
       <c r="D26" s="50">
-        <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
+        <f>IF(COUNT(Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41)=0,"",AVERAGE(Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41))</f>
         <v/>
       </c>
       <c r="E26" s="51">
@@ -3578,7 +3693,7 @@
         </is>
       </c>
       <c r="D27" s="50">
-        <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
+        <f>IF(COUNT(Assessment!F42)=0,"",AVERAGE(Assessment!F42))</f>
         <v/>
       </c>
       <c r="E27" s="51">
@@ -3616,7 +3731,7 @@
         </is>
       </c>
       <c r="D29" s="50">
-        <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
+        <f>IF(COUNT(Assessment!F45,Assessment!F46)=0,"",AVERAGE(Assessment!F45,Assessment!F46))</f>
         <v/>
       </c>
       <c r="E29" s="51">
@@ -3635,7 +3750,7 @@
         </is>
       </c>
       <c r="D30" s="50">
-        <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
+        <f>IF(COUNT(Assessment!F47)=0,"",AVERAGE(Assessment!F47))</f>
         <v/>
       </c>
       <c r="E30" s="51">
@@ -3654,7 +3769,7 @@
         </is>
       </c>
       <c r="D31" s="50">
-        <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
+        <f>IF(COUNT(Assessment!F48,Assessment!F49)=0,"",AVERAGE(Assessment!F48,Assessment!F49))</f>
         <v/>
       </c>
       <c r="E31" s="51">
@@ -3692,7 +3807,7 @@
         </is>
       </c>
       <c r="D33" s="50">
-        <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52))</f>
+        <f>IF(COUNT(Assessment!F52,Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F52,Assessment!F53,Assessment!F54))</f>
         <v/>
       </c>
       <c r="E33" s="51">
@@ -3711,7 +3826,7 @@
         </is>
       </c>
       <c r="D34" s="50">
-        <f>IF(COUNT(Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F53,Assessment!F54))</f>
+        <f>IF(COUNT(Assessment!F55,Assessment!F56,Assessment!F57)=0,"",AVERAGE(Assessment!F55,Assessment!F56,Assessment!F57))</f>
         <v/>
       </c>
       <c r="E34" s="51">
@@ -3802,7 +3917,7 @@
         </is>
       </c>
       <c r="D40" s="50">
-        <f>IF(COUNT(Assessment!F61)=0,"",AVERAGE(Assessment!F61))</f>
+        <f>IF(COUNT(Assessment!F64,Assessment!F69)=0,"",AVERAGE(Assessment!F64,Assessment!F69))</f>
         <v/>
       </c>
       <c r="E40" s="51">
@@ -3821,7 +3936,7 @@
         </is>
       </c>
       <c r="D41" s="50">
-        <f>IF(COUNT(Assessment!F62)=0,"",AVERAGE(Assessment!F62))</f>
+        <f>IF(COUNT(Assessment!F65)=0,"",AVERAGE(Assessment!F65))</f>
         <v/>
       </c>
       <c r="E41" s="51">
@@ -3840,7 +3955,7 @@
         </is>
       </c>
       <c r="D42" s="50">
-        <f>IF(COUNT(Assessment!F63,Assessment!F64,Assessment!F65)=0,"",AVERAGE(Assessment!F63,Assessment!F64,Assessment!F65))</f>
+        <f>IF(COUNT(Assessment!F66,Assessment!F67,Assessment!F68)=0,"",AVERAGE(Assessment!F66,Assessment!F67,Assessment!F68))</f>
         <v/>
       </c>
       <c r="E42" s="51">
@@ -3878,7 +3993,7 @@
         </is>
       </c>
       <c r="D44" s="50">
-        <f>IF(COUNT(Assessment!F68)=0,"",AVERAGE(Assessment!F68))</f>
+        <f>IF(COUNT(Assessment!F72,Assessment!F76)=0,"",AVERAGE(Assessment!F72,Assessment!F76))</f>
         <v/>
       </c>
       <c r="E44" s="51">
@@ -3897,7 +4012,7 @@
         </is>
       </c>
       <c r="D45" s="50">
-        <f>IF(COUNT(Assessment!F69,Assessment!F70)=0,"",AVERAGE(Assessment!F69,Assessment!F70))</f>
+        <f>IF(COUNT(Assessment!F73,Assessment!F74)=0,"",AVERAGE(Assessment!F73,Assessment!F74))</f>
         <v/>
       </c>
       <c r="E45" s="51">
@@ -3916,7 +4031,7 @@
         </is>
       </c>
       <c r="D46" s="50">
-        <f>IF(COUNT(Assessment!F71)=0,"",AVERAGE(Assessment!F71))</f>
+        <f>IF(COUNT(Assessment!F75)=0,"",AVERAGE(Assessment!F75))</f>
         <v/>
       </c>
       <c r="E46" s="51">
@@ -7339,7 +7454,7 @@
         </is>
       </c>
       <c r="B8" s="49">
-        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
+        <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E22,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E33,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E41,Assessment!E42,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E48,Assessment!E49,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E55,Assessment!E56,Assessment!E57,Assessment!E64,Assessment!E65,Assessment!E66,Assessment!E67,Assessment!E68,Assessment!E69,Assessment!E72,Assessment!E73,Assessment!E74,Assessment!E75,Assessment!E76)&amp;" / 46"</f>
         <v/>
       </c>
     </row>
@@ -7387,7 +7502,7 @@
         </is>
       </c>
       <c r="C11" s="55">
-        <f>IF(COUNT(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <f>IF(COUNT(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22)=0,"",AVERAGE(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22))</f>
         <v/>
       </c>
       <c r="D11" s="75">
@@ -7415,7 +7530,7 @@
         </is>
       </c>
       <c r="C12" s="55">
-        <f>IF(COUNT(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32)=0,"",AVERAGE(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32))</f>
+        <f>IF(COUNT(Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32,Assessment!F33)=0,"",AVERAGE(Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32,Assessment!F33))</f>
         <v/>
       </c>
       <c r="D12" s="75">
@@ -7443,7 +7558,7 @@
         </is>
       </c>
       <c r="C13" s="55">
-        <f>IF(COUNT(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40)=0,"",AVERAGE(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40))</f>
+        <f>IF(COUNT(Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41,Assessment!F42)=0,"",AVERAGE(Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41,Assessment!F42))</f>
         <v/>
       </c>
       <c r="D13" s="75">
@@ -7471,7 +7586,7 @@
         </is>
       </c>
       <c r="C14" s="55">
-        <f>IF(COUNT(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47))</f>
+        <f>IF(COUNT(Assessment!F45,Assessment!F46,Assessment!F47,Assessment!F48,Assessment!F49)=0,"",AVERAGE(Assessment!F45,Assessment!F46,Assessment!F47,Assessment!F48,Assessment!F49))</f>
         <v/>
       </c>
       <c r="D14" s="75">
@@ -7499,7 +7614,7 @@
         </is>
       </c>
       <c r="C15" s="55">
-        <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54))</f>
+        <f>IF(COUNT(Assessment!F52,Assessment!F53,Assessment!F54,Assessment!F55,Assessment!F56,Assessment!F57)=0,"",AVERAGE(Assessment!F52,Assessment!F53,Assessment!F54,Assessment!F55,Assessment!F56,Assessment!F57))</f>
         <v/>
       </c>
       <c r="D15" s="75">
@@ -7651,7 +7766,7 @@
         </is>
       </c>
       <c r="D21" s="50">
-        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21,Assessment!F22))</f>
         <v/>
       </c>
       <c r="E21" s="51">
@@ -7680,7 +7795,7 @@
         </is>
       </c>
       <c r="D22" s="50">
-        <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
+        <f>IF(COUNT(Assessment!F25,Assessment!F26)=0,"",AVERAGE(Assessment!F25,Assessment!F26))</f>
         <v/>
       </c>
       <c r="E22" s="51">
@@ -7709,7 +7824,7 @@
         </is>
       </c>
       <c r="D23" s="50">
-        <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
+        <f>IF(COUNT(Assessment!F27)=0,"",AVERAGE(Assessment!F27))</f>
         <v/>
       </c>
       <c r="E23" s="51">
@@ -7738,7 +7853,7 @@
         </is>
       </c>
       <c r="D24" s="50">
-        <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
+        <f>IF(COUNT(Assessment!F28,Assessment!F29,Assessment!F30)=0,"",AVERAGE(Assessment!F28,Assessment!F29,Assessment!F30))</f>
         <v/>
       </c>
       <c r="E24" s="51">
@@ -7767,7 +7882,7 @@
         </is>
       </c>
       <c r="D25" s="50">
-        <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
+        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
         <v/>
       </c>
       <c r="E25" s="51">
@@ -7796,7 +7911,7 @@
         </is>
       </c>
       <c r="D26" s="50">
-        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
+        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
         <v/>
       </c>
       <c r="E26" s="51">
@@ -7825,7 +7940,7 @@
         </is>
       </c>
       <c r="D27" s="50">
-        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
+        <f>IF(COUNT(Assessment!F33)=0,"",AVERAGE(Assessment!F33))</f>
         <v/>
       </c>
       <c r="E27" s="51">
@@ -7854,7 +7969,7 @@
         </is>
       </c>
       <c r="D28" s="50">
-        <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
+        <f>IF(COUNT(Assessment!F36,Assessment!F37)=0,"",AVERAGE(Assessment!F36,Assessment!F37))</f>
         <v/>
       </c>
       <c r="E28" s="51">
@@ -7883,7 +7998,7 @@
         </is>
       </c>
       <c r="D29" s="50">
-        <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
+        <f>IF(COUNT(Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41)=0,"",AVERAGE(Assessment!F38,Assessment!F39,Assessment!F40,Assessment!F41))</f>
         <v/>
       </c>
       <c r="E29" s="51">
@@ -7912,7 +8027,7 @@
         </is>
       </c>
       <c r="D30" s="50">
-        <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
+        <f>IF(COUNT(Assessment!F42)=0,"",AVERAGE(Assessment!F42))</f>
         <v/>
       </c>
       <c r="E30" s="51">
@@ -7941,7 +8056,7 @@
         </is>
       </c>
       <c r="D31" s="50">
-        <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
+        <f>IF(COUNT(Assessment!F45,Assessment!F46)=0,"",AVERAGE(Assessment!F45,Assessment!F46))</f>
         <v/>
       </c>
       <c r="E31" s="51">
@@ -7970,7 +8085,7 @@
         </is>
       </c>
       <c r="D32" s="50">
-        <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
+        <f>IF(COUNT(Assessment!F47)=0,"",AVERAGE(Assessment!F47))</f>
         <v/>
       </c>
       <c r="E32" s="51">
@@ -7999,7 +8114,7 @@
         </is>
       </c>
       <c r="D33" s="50">
-        <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
+        <f>IF(COUNT(Assessment!F48,Assessment!F49)=0,"",AVERAGE(Assessment!F48,Assessment!F49))</f>
         <v/>
       </c>
       <c r="E33" s="51">
@@ -8028,7 +8143,7 @@
         </is>
       </c>
       <c r="D34" s="50">
-        <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52))</f>
+        <f>IF(COUNT(Assessment!F52,Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F52,Assessment!F53,Assessment!F54))</f>
         <v/>
       </c>
       <c r="E34" s="51">
@@ -8057,7 +8172,7 @@
         </is>
       </c>
       <c r="D35" s="50">
-        <f>IF(COUNT(Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F53,Assessment!F54))</f>
+        <f>IF(COUNT(Assessment!F55,Assessment!F56,Assessment!F57)=0,"",AVERAGE(Assessment!F55,Assessment!F56,Assessment!F57))</f>
         <v/>
       </c>
       <c r="E35" s="51">
@@ -8086,7 +8201,7 @@
         </is>
       </c>
       <c r="D36" s="50">
-        <f>IF(COUNT(Assessment!F61)=0,"",AVERAGE(Assessment!F61))</f>
+        <f>IF(COUNT(Assessment!F64,Assessment!F69)=0,"",AVERAGE(Assessment!F64,Assessment!F69))</f>
         <v/>
       </c>
       <c r="E36" s="51">
@@ -8115,7 +8230,7 @@
         </is>
       </c>
       <c r="D37" s="50">
-        <f>IF(COUNT(Assessment!F62)=0,"",AVERAGE(Assessment!F62))</f>
+        <f>IF(COUNT(Assessment!F65)=0,"",AVERAGE(Assessment!F65))</f>
         <v/>
       </c>
       <c r="E37" s="51">
@@ -8144,7 +8259,7 @@
         </is>
       </c>
       <c r="D38" s="50">
-        <f>IF(COUNT(Assessment!F63,Assessment!F64,Assessment!F65)=0,"",AVERAGE(Assessment!F63,Assessment!F64,Assessment!F65))</f>
+        <f>IF(COUNT(Assessment!F66,Assessment!F67,Assessment!F68)=0,"",AVERAGE(Assessment!F66,Assessment!F67,Assessment!F68))</f>
         <v/>
       </c>
       <c r="E38" s="51">
@@ -8173,7 +8288,7 @@
         </is>
       </c>
       <c r="D39" s="50">
-        <f>IF(COUNT(Assessment!F68)=0,"",AVERAGE(Assessment!F68))</f>
+        <f>IF(COUNT(Assessment!F72,Assessment!F76)=0,"",AVERAGE(Assessment!F72,Assessment!F76))</f>
         <v/>
       </c>
       <c r="E39" s="51">
@@ -8202,7 +8317,7 @@
         </is>
       </c>
       <c r="D40" s="50">
-        <f>IF(COUNT(Assessment!F69,Assessment!F70)=0,"",AVERAGE(Assessment!F69,Assessment!F70))</f>
+        <f>IF(COUNT(Assessment!F73,Assessment!F74)=0,"",AVERAGE(Assessment!F73,Assessment!F74))</f>
         <v/>
       </c>
       <c r="E40" s="51">
@@ -8231,7 +8346,7 @@
         </is>
       </c>
       <c r="D41" s="50">
-        <f>IF(COUNT(Assessment!F71)=0,"",AVERAGE(Assessment!F71))</f>
+        <f>IF(COUNT(Assessment!F75)=0,"",AVERAGE(Assessment!F75))</f>
         <v/>
       </c>
       <c r="E41" s="51">

</xml_diff>